<commit_message>
FIFA Futsal 2016 Date 2 Group A.B.C.D
FIFA Futsal 2016 Date 2 Group A.B.C.D
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -46743,18 +46743,18 @@
       <c r="C90" s="3">
         <v>507</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>18</v>
+      <c r="D90" s="3">
+        <v>0</v>
+      </c>
+      <c r="E90" s="3">
+        <v>0</v>
       </c>
       <c r="F90" s="3">
         <v>2</v>
       </c>
       <c r="G90" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1279, 311, 507, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1279, 311, 507, 0, 0, 2);</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -46769,18 +46769,18 @@
       <c r="C91" s="3">
         <v>507</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>18</v>
+      <c r="D91" s="3">
+        <v>0</v>
+      </c>
+      <c r="E91" s="3">
+        <v>0</v>
       </c>
       <c r="F91" s="3">
         <v>1</v>
       </c>
       <c r="G91" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1280, 311, 507, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1280, 311, 507, 0, 0, 1);</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -46795,18 +46795,18 @@
       <c r="C92" s="3">
         <v>351</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>18</v>
+      <c r="D92" s="3">
+        <v>9</v>
+      </c>
+      <c r="E92" s="3">
+        <v>3</v>
       </c>
       <c r="F92" s="3">
         <v>2</v>
       </c>
       <c r="G92" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1281, 311, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1281, 311, 351, 9, 3, 2);</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -46821,18 +46821,18 @@
       <c r="C93" s="3">
         <v>351</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>18</v>
+      <c r="D93" s="3">
+        <v>8</v>
+      </c>
+      <c r="E93" s="3">
+        <v>0</v>
       </c>
       <c r="F93" s="3">
         <v>1</v>
       </c>
       <c r="G93" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1282, 311, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1282, 311, 351, 8, 0, 1);</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -46847,18 +46847,18 @@
       <c r="C94" s="4">
         <v>57</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>18</v>
+      <c r="D94" s="4">
+        <v>3</v>
+      </c>
+      <c r="E94" s="4">
+        <v>1</v>
       </c>
       <c r="F94" s="4">
         <v>2</v>
       </c>
       <c r="G94" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1283, 312, 57, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1283, 312, 57, 3, 1, 2);</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -46873,18 +46873,18 @@
       <c r="C95" s="4">
         <v>57</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>18</v>
+      <c r="D95" s="4">
+        <v>1</v>
+      </c>
+      <c r="E95" s="4">
+        <v>0</v>
       </c>
       <c r="F95" s="4">
         <v>1</v>
       </c>
       <c r="G95" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1284, 312, 57, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1284, 312, 57, 1, 0, 1);</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -46899,18 +46899,18 @@
       <c r="C96" s="4">
         <v>998</v>
       </c>
-      <c r="D96" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E96" s="4" t="s">
-        <v>18</v>
+      <c r="D96" s="4">
+        <v>3</v>
+      </c>
+      <c r="E96" s="4">
+        <v>1</v>
       </c>
       <c r="F96" s="4">
         <v>2</v>
       </c>
       <c r="G96" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1285, 312, 998, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1285, 312, 998, 3, 1, 2);</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -46925,18 +46925,18 @@
       <c r="C97" s="4">
         <v>998</v>
       </c>
-      <c r="D97" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E97" s="4" t="s">
-        <v>18</v>
+      <c r="D97" s="4">
+        <v>2</v>
+      </c>
+      <c r="E97" s="4">
+        <v>0</v>
       </c>
       <c r="F97" s="4">
         <v>1</v>
       </c>
       <c r="G97" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1286, 312, 998, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1286, 312, 998, 2, 0, 1);</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -47367,18 +47367,18 @@
       <c r="C114" s="3">
         <v>20</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>18</v>
+      <c r="D114" s="3">
+        <v>1</v>
+      </c>
+      <c r="E114" s="3">
+        <v>0</v>
       </c>
       <c r="F114" s="3">
         <v>2</v>
       </c>
       <c r="G114" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1303, 317, 20, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1303, 317, 20, 1, 0, 2);</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -47393,18 +47393,18 @@
       <c r="C115" s="3">
         <v>20</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>18</v>
+      <c r="D115" s="3">
+        <v>0</v>
+      </c>
+      <c r="E115" s="3">
+        <v>0</v>
       </c>
       <c r="F115" s="3">
         <v>1</v>
       </c>
       <c r="G115" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1304, 317, 20, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1304, 317, 20, 0, 0, 1);</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -47419,18 +47419,18 @@
       <c r="C116" s="3">
         <v>7</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>18</v>
+      <c r="D116" s="3">
+        <v>6</v>
+      </c>
+      <c r="E116" s="3">
+        <v>3</v>
       </c>
       <c r="F116" s="3">
         <v>2</v>
       </c>
       <c r="G116" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1305, 317, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1305, 317, 7, 6, 3, 2);</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -47445,18 +47445,18 @@
       <c r="C117" s="3">
         <v>7</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>18</v>
+      <c r="D117" s="3">
+        <v>4</v>
+      </c>
+      <c r="E117" s="3">
+        <v>0</v>
       </c>
       <c r="F117" s="3">
         <v>1</v>
       </c>
       <c r="G117" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1306, 317, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1306, 317, 7, 4, 0, 1);</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -47471,18 +47471,18 @@
       <c r="C118" s="4">
         <v>66</v>
       </c>
-      <c r="D118" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>18</v>
+      <c r="D118" s="4">
+        <v>8</v>
+      </c>
+      <c r="E118" s="4">
+        <v>3</v>
       </c>
       <c r="F118" s="4">
         <v>2</v>
       </c>
       <c r="G118" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1307, 318, 66, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1307, 318, 66, 8, 3, 2);</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -47497,18 +47497,18 @@
       <c r="C119" s="4">
         <v>66</v>
       </c>
-      <c r="D119" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>18</v>
+      <c r="D119" s="4">
+        <v>3</v>
+      </c>
+      <c r="E119" s="4">
+        <v>0</v>
       </c>
       <c r="F119" s="4">
         <v>1</v>
       </c>
       <c r="G119" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1308, 318, 66, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1308, 318, 66, 3, 0, 1);</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -47523,18 +47523,18 @@
       <c r="C120" s="4">
         <v>53</v>
       </c>
-      <c r="D120" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>18</v>
+      <c r="D120" s="4">
+        <v>5</v>
+      </c>
+      <c r="E120" s="4">
+        <v>0</v>
       </c>
       <c r="F120" s="4">
         <v>2</v>
       </c>
       <c r="G120" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1309, 318, 53, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1309, 318, 53, 5, 0, 2);</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -47549,18 +47549,18 @@
       <c r="C121" s="4">
         <v>53</v>
       </c>
-      <c r="D121" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E121" s="4" t="s">
-        <v>18</v>
+      <c r="D121" s="4">
+        <v>4</v>
+      </c>
+      <c r="E121" s="4">
+        <v>0</v>
       </c>
       <c r="F121" s="4">
         <v>1</v>
       </c>
       <c r="G121" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1310, 318, 53, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1310, 318, 53, 4, 0, 1);</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -49031,18 +49031,18 @@
       <c r="C178" s="3">
         <v>677</v>
       </c>
-      <c r="D178" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E178" s="3" t="s">
-        <v>18</v>
+      <c r="D178" s="3">
+        <v>2</v>
+      </c>
+      <c r="E178" s="3">
+        <v>0</v>
       </c>
       <c r="F178" s="3">
         <v>2</v>
       </c>
       <c r="G178" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1367, 333, 677, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1367, 333, 677, 2, 0, 2);</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -49057,18 +49057,18 @@
       <c r="C179" s="3">
         <v>677</v>
       </c>
-      <c r="D179" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E179" s="3" t="s">
-        <v>18</v>
+      <c r="D179" s="3">
+        <v>0</v>
+      </c>
+      <c r="E179" s="3">
+        <v>0</v>
       </c>
       <c r="F179" s="3">
         <v>1</v>
       </c>
       <c r="G179" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1368, 333, 677, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1368, 333, 677, 0, 0, 1);</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -49083,18 +49083,18 @@
       <c r="C180" s="3">
         <v>506</v>
       </c>
-      <c r="D180" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E180" s="3" t="s">
-        <v>18</v>
+      <c r="D180" s="3">
+        <v>4</v>
+      </c>
+      <c r="E180" s="3">
+        <v>3</v>
       </c>
       <c r="F180" s="3">
         <v>2</v>
       </c>
       <c r="G180" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1369, 333, 506, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1369, 333, 506, 4, 3, 2);</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -49109,18 +49109,18 @@
       <c r="C181" s="3">
         <v>506</v>
       </c>
-      <c r="D181" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E181" s="3" t="s">
-        <v>18</v>
+      <c r="D181" s="3">
+        <v>1</v>
+      </c>
+      <c r="E181" s="3">
+        <v>0</v>
       </c>
       <c r="F181" s="3">
         <v>1</v>
       </c>
       <c r="G181" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1370, 333, 506, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1370, 333, 506, 1, 0, 1);</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -49135,18 +49135,18 @@
       <c r="C182" s="4">
         <v>54</v>
       </c>
-      <c r="D182" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E182" s="4" t="s">
-        <v>18</v>
+      <c r="D182" s="4">
+        <v>1</v>
+      </c>
+      <c r="E182" s="4">
+        <v>3</v>
       </c>
       <c r="F182" s="4">
         <v>2</v>
       </c>
       <c r="G182" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1371, 334, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1371, 334, 54, 1, 3, 2);</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -49161,18 +49161,18 @@
       <c r="C183" s="4">
         <v>54</v>
       </c>
-      <c r="D183" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E183" s="4" t="s">
-        <v>18</v>
+      <c r="D183" s="4">
+        <v>1</v>
+      </c>
+      <c r="E183" s="4">
+        <v>0</v>
       </c>
       <c r="F183" s="4">
         <v>1</v>
       </c>
       <c r="G183" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1372, 334, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1372, 334, 54, 1, 0, 1);</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -49187,18 +49187,18 @@
       <c r="C184" s="4">
         <v>76</v>
       </c>
-      <c r="D184" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E184" s="4" t="s">
-        <v>18</v>
+      <c r="D184" s="4">
+        <v>0</v>
+      </c>
+      <c r="E184" s="4">
+        <v>0</v>
       </c>
       <c r="F184" s="4">
         <v>2</v>
       </c>
       <c r="G184" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1373, 334, 76, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1373, 334, 76, 0, 0, 2);</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -49213,18 +49213,18 @@
       <c r="C185" s="4">
         <v>76</v>
       </c>
-      <c r="D185" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E185" s="4" t="s">
-        <v>18</v>
+      <c r="D185" s="4">
+        <v>0</v>
+      </c>
+      <c r="E185" s="4">
+        <v>0</v>
       </c>
       <c r="F185" s="4">
         <v>1</v>
       </c>
       <c r="G185" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1374, 334, 76, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1374, 334, 76, 0, 0, 1);</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -49655,18 +49655,18 @@
       <c r="C202" s="3">
         <v>212</v>
       </c>
-      <c r="D202" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E202" s="3" t="s">
-        <v>18</v>
+      <c r="D202" s="3">
+        <v>0</v>
+      </c>
+      <c r="E202" s="3">
+        <v>0</v>
       </c>
       <c r="F202" s="3">
         <v>2</v>
       </c>
       <c r="G202" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1391, 339, 212, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1391, 339, 212, 0, 0, 2);</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -49681,18 +49681,18 @@
       <c r="C203" s="3">
         <v>212</v>
       </c>
-      <c r="D203" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E203" s="3" t="s">
-        <v>18</v>
+      <c r="D203" s="3">
+        <v>0</v>
+      </c>
+      <c r="E203" s="3">
+        <v>0</v>
       </c>
       <c r="F203" s="3">
         <v>1</v>
       </c>
       <c r="G203" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1392, 339, 212, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1392, 339, 212, 0, 0, 1);</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -49707,18 +49707,18 @@
       <c r="C204" s="3">
         <v>994</v>
       </c>
-      <c r="D204" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E204" s="3" t="s">
-        <v>18</v>
+      <c r="D204" s="3">
+        <v>5</v>
+      </c>
+      <c r="E204" s="3">
+        <v>3</v>
       </c>
       <c r="F204" s="3">
         <v>2</v>
       </c>
       <c r="G204" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1393, 339, 994, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1393, 339, 994, 5, 3, 2);</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -49733,18 +49733,18 @@
       <c r="C205" s="3">
         <v>994</v>
       </c>
-      <c r="D205" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E205" s="3" t="s">
-        <v>18</v>
+      <c r="D205" s="3">
+        <v>2</v>
+      </c>
+      <c r="E205" s="3">
+        <v>0</v>
       </c>
       <c r="F205" s="3">
         <v>1</v>
       </c>
       <c r="G205" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1394, 339, 994, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1394, 339, 994, 2, 0, 1);</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -49759,18 +49759,18 @@
       <c r="C206" s="4">
         <v>98</v>
       </c>
-      <c r="D206" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E206" s="4" t="s">
-        <v>18</v>
+      <c r="D206" s="4">
+        <v>1</v>
+      </c>
+      <c r="E206" s="4">
+        <v>0</v>
       </c>
       <c r="F206" s="4">
         <v>2</v>
       </c>
       <c r="G206" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1395, 340, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1395, 340, 98, 1, 0, 2);</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -49785,18 +49785,18 @@
       <c r="C207" s="4">
         <v>98</v>
       </c>
-      <c r="D207" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E207" s="4" t="s">
-        <v>18</v>
+      <c r="D207" s="4">
+        <v>0</v>
+      </c>
+      <c r="E207" s="4">
+        <v>0</v>
       </c>
       <c r="F207" s="4">
         <v>1</v>
       </c>
       <c r="G207" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1396, 340, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1396, 340, 98, 0, 0, 1);</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -49811,18 +49811,18 @@
       <c r="C208" s="4">
         <v>34</v>
       </c>
-      <c r="D208" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E208" s="4" t="s">
-        <v>18</v>
+      <c r="D208" s="4">
+        <v>5</v>
+      </c>
+      <c r="E208" s="4">
+        <v>3</v>
       </c>
       <c r="F208" s="4">
         <v>2</v>
       </c>
       <c r="G208" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1397, 340, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1397, 340, 34, 5, 3, 2);</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -49837,18 +49837,18 @@
       <c r="C209" s="4">
         <v>34</v>
       </c>
-      <c r="D209" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E209" s="4" t="s">
-        <v>18</v>
+      <c r="D209" s="4">
+        <v>3</v>
+      </c>
+      <c r="E209" s="4">
+        <v>0</v>
       </c>
       <c r="F209" s="4">
         <v>1</v>
       </c>
       <c r="G209" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1398, 340, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1398, 340, 34, 3, 0, 1);</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Futsal WorldCup 2016 2nd date Africa Cup of Nations
Futsal WorldCup 2016 2nd date groups F and G Africa Cup of Nations 1984,
1986, 1988, 1990
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -119,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -127,6 +127,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -46636,7 +46637,7 @@
         <f>B82+1</f>
         <v>310</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="5">
         <v>57</v>
       </c>
       <c r="D86" s="4">
@@ -46662,7 +46663,7 @@
         <f>B86</f>
         <v>310</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="5">
         <v>57</v>
       </c>
       <c r="D87" s="4">
@@ -46688,7 +46689,7 @@
         <f>B86</f>
         <v>310</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="5">
         <v>351</v>
       </c>
       <c r="D88" s="4">
@@ -46714,7 +46715,7 @@
         <f>B86</f>
         <v>310</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="5">
         <v>351</v>
       </c>
       <c r="D89" s="4">
@@ -47991,18 +47992,18 @@
       <c r="C138" s="3">
         <v>502</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>18</v>
+      <c r="D138" s="3">
+        <v>1</v>
+      </c>
+      <c r="E138" s="3">
+        <v>3</v>
       </c>
       <c r="F138" s="3">
         <v>2</v>
       </c>
       <c r="G138" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1327, 323, 502, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1327, 323, 502, 1, 3, 2);</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -48017,18 +48018,18 @@
       <c r="C139" s="3">
         <v>502</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>18</v>
+      <c r="D139" s="3">
+        <v>1</v>
+      </c>
+      <c r="E139" s="3">
+        <v>0</v>
       </c>
       <c r="F139" s="3">
         <v>1</v>
       </c>
       <c r="G139" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1328, 323, 502, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1328, 323, 502, 1, 0, 1);</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -48043,18 +48044,18 @@
       <c r="C140" s="3">
         <v>39</v>
       </c>
-      <c r="D140" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>18</v>
+      <c r="D140" s="3">
+        <v>5</v>
+      </c>
+      <c r="E140" s="3">
+        <v>0</v>
       </c>
       <c r="F140" s="3">
         <v>2</v>
       </c>
       <c r="G140" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1329, 323, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1329, 323, 39, 5, 0, 2);</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -48069,18 +48070,18 @@
       <c r="C141" s="3">
         <v>39</v>
       </c>
-      <c r="D141" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>18</v>
+      <c r="D141" s="3">
+        <v>3</v>
+      </c>
+      <c r="E141" s="3">
+        <v>0</v>
       </c>
       <c r="F141" s="3">
         <v>1</v>
       </c>
       <c r="G141" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1330, 323, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1330, 323, 39, 3, 0, 1);</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -48095,18 +48096,18 @@
       <c r="C142" s="4">
         <v>595</v>
       </c>
-      <c r="D142" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>18</v>
+      <c r="D142" s="4">
+        <v>7</v>
+      </c>
+      <c r="E142" s="4">
+        <v>3</v>
       </c>
       <c r="F142" s="4">
         <v>2</v>
       </c>
       <c r="G142" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1331, 324, 595, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1331, 324, 595, 7, 3, 2);</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -48121,18 +48122,18 @@
       <c r="C143" s="4">
         <v>595</v>
       </c>
-      <c r="D143" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E143" s="4" t="s">
-        <v>18</v>
+      <c r="D143" s="4">
+        <v>5</v>
+      </c>
+      <c r="E143" s="4">
+        <v>0</v>
       </c>
       <c r="F143" s="4">
         <v>1</v>
       </c>
       <c r="G143" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1332, 324, 595, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1332, 324, 595, 5, 0, 1);</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -48147,18 +48148,18 @@
       <c r="C144" s="4">
         <v>84</v>
       </c>
-      <c r="D144" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E144" s="4" t="s">
-        <v>18</v>
+      <c r="D144" s="4">
+        <v>1</v>
+      </c>
+      <c r="E144" s="4">
+        <v>0</v>
       </c>
       <c r="F144" s="4">
         <v>2</v>
       </c>
       <c r="G144" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1333, 324, 84, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1333, 324, 84, 1, 0, 2);</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -48173,18 +48174,18 @@
       <c r="C145" s="4">
         <v>84</v>
       </c>
-      <c r="D145" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E145" s="4" t="s">
-        <v>18</v>
+      <c r="D145" s="4">
+        <v>0</v>
+      </c>
+      <c r="E145" s="4">
+        <v>0</v>
       </c>
       <c r="F145" s="4">
         <v>1</v>
       </c>
       <c r="G145" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1334, 324, 84, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1334, 324, 84, 0, 0, 1);</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -48615,18 +48616,18 @@
       <c r="C162" s="3">
         <v>61</v>
       </c>
-      <c r="D162" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>18</v>
+      <c r="D162" s="3">
+        <v>1</v>
+      </c>
+      <c r="E162" s="3">
+        <v>0</v>
       </c>
       <c r="F162" s="3">
         <v>2</v>
       </c>
       <c r="G162" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1351, 329, 61, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1351, 329, 61, 1, 0, 2);</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -48641,18 +48642,18 @@
       <c r="C163" s="3">
         <v>61</v>
       </c>
-      <c r="D163" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>18</v>
+      <c r="D163" s="3">
+        <v>1</v>
+      </c>
+      <c r="E163" s="3">
+        <v>0</v>
       </c>
       <c r="F163" s="3">
         <v>1</v>
       </c>
       <c r="G163" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1352, 329, 61, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1352, 329, 61, 1, 0, 1);</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -48667,18 +48668,18 @@
       <c r="C164" s="3">
         <v>55</v>
       </c>
-      <c r="D164" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>18</v>
+      <c r="D164" s="3">
+        <v>11</v>
+      </c>
+      <c r="E164" s="3">
+        <v>3</v>
       </c>
       <c r="F164" s="3">
         <v>2</v>
       </c>
       <c r="G164" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1353, 329, 55, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1353, 329, 55, 11, 3, 2);</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -48693,18 +48694,18 @@
       <c r="C165" s="3">
         <v>55</v>
       </c>
-      <c r="D165" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>18</v>
+      <c r="D165" s="3">
+        <v>4</v>
+      </c>
+      <c r="E165" s="3">
+        <v>0</v>
       </c>
       <c r="F165" s="3">
         <v>1</v>
       </c>
       <c r="G165" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1354, 329, 55, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1354, 329, 55, 4, 0, 1);</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -48719,18 +48720,18 @@
       <c r="C166" s="4">
         <v>380</v>
       </c>
-      <c r="D166" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E166" s="4" t="s">
-        <v>18</v>
+      <c r="D166" s="4">
+        <v>4</v>
+      </c>
+      <c r="E166" s="4">
+        <v>3</v>
       </c>
       <c r="F166" s="4">
         <v>2</v>
       </c>
       <c r="G166" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1355, 330, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1355, 330, 380, 4, 3, 2);</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -48745,18 +48746,18 @@
       <c r="C167" s="4">
         <v>380</v>
       </c>
-      <c r="D167" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E167" s="4" t="s">
-        <v>18</v>
+      <c r="D167" s="4">
+        <v>2</v>
+      </c>
+      <c r="E167" s="4">
+        <v>0</v>
       </c>
       <c r="F167" s="4">
         <v>1</v>
       </c>
       <c r="G167" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1356, 330, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1356, 330, 380, 2, 0, 1);</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -48771,18 +48772,18 @@
       <c r="C168" s="4">
         <v>258</v>
       </c>
-      <c r="D168" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E168" s="4" t="s">
-        <v>18</v>
+      <c r="D168" s="4">
+        <v>2</v>
+      </c>
+      <c r="E168" s="4">
+        <v>0</v>
       </c>
       <c r="F168" s="4">
         <v>2</v>
       </c>
       <c r="G168" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1357, 330, 258, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1357, 330, 258, 2, 0, 2);</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -48797,18 +48798,18 @@
       <c r="C169" s="4">
         <v>258</v>
       </c>
-      <c r="D169" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E169" s="4" t="s">
-        <v>18</v>
+      <c r="D169" s="4">
+        <v>2</v>
+      </c>
+      <c r="E169" s="4">
+        <v>0</v>
       </c>
       <c r="F169" s="4">
         <v>1</v>
       </c>
       <c r="G169" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1358, 330, 258, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1358, 330, 258, 2, 0, 1);</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -49239,18 +49240,18 @@
       <c r="C186" s="3">
         <v>506</v>
       </c>
-      <c r="D186" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>18</v>
+      <c r="D186" s="3">
+        <v>1</v>
+      </c>
+      <c r="E186" s="3">
+        <v>0</v>
       </c>
       <c r="F186" s="3">
         <v>2</v>
       </c>
       <c r="G186" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1375, 335, 506, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1375, 335, 506, 1, 0, 2);</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -49265,18 +49266,18 @@
       <c r="C187" s="3">
         <v>506</v>
       </c>
-      <c r="D187" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E187" s="3" t="s">
-        <v>18</v>
+      <c r="D187" s="3">
+        <v>1</v>
+      </c>
+      <c r="E187" s="3">
+        <v>0</v>
       </c>
       <c r="F187" s="3">
         <v>1</v>
       </c>
       <c r="G187" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1376, 335, 506, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1376, 335, 506, 1, 0, 1);</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -49291,18 +49292,18 @@
       <c r="C188" s="3">
         <v>76</v>
       </c>
-      <c r="D188" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>18</v>
+      <c r="D188" s="3">
+        <v>3</v>
+      </c>
+      <c r="E188" s="3">
+        <v>3</v>
       </c>
       <c r="F188" s="3">
         <v>2</v>
       </c>
       <c r="G188" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1377, 335, 76, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1377, 335, 76, 3, 3, 2);</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -49317,18 +49318,18 @@
       <c r="C189" s="3">
         <v>76</v>
       </c>
-      <c r="D189" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E189" s="3" t="s">
-        <v>18</v>
+      <c r="D189" s="3">
+        <v>2</v>
+      </c>
+      <c r="E189" s="3">
+        <v>0</v>
       </c>
       <c r="F189" s="3">
         <v>1</v>
       </c>
       <c r="G189" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1378, 335, 76, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1378, 335, 76, 2, 0, 1);</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -49343,18 +49344,18 @@
       <c r="C190" s="4">
         <v>54</v>
       </c>
-      <c r="D190" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E190" s="4" t="s">
-        <v>18</v>
+      <c r="D190" s="4">
+        <v>7</v>
+      </c>
+      <c r="E190" s="4">
+        <v>3</v>
       </c>
       <c r="F190" s="4">
         <v>2</v>
       </c>
       <c r="G190" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1379, 336, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1379, 336, 54, 7, 3, 2);</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -49369,18 +49370,18 @@
       <c r="C191" s="4">
         <v>54</v>
       </c>
-      <c r="D191" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E191" s="4" t="s">
-        <v>18</v>
+      <c r="D191" s="4">
+        <v>5</v>
+      </c>
+      <c r="E191" s="4">
+        <v>0</v>
       </c>
       <c r="F191" s="4">
         <v>1</v>
       </c>
       <c r="G191" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1380, 336, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1380, 336, 54, 5, 0, 1);</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -49395,18 +49396,18 @@
       <c r="C192" s="4">
         <v>677</v>
       </c>
-      <c r="D192" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E192" s="4" t="s">
-        <v>18</v>
+      <c r="D192" s="4">
+        <v>3</v>
+      </c>
+      <c r="E192" s="4">
+        <v>0</v>
       </c>
       <c r="F192" s="4">
         <v>2</v>
       </c>
       <c r="G192" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1381, 336, 677, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1381, 336, 677, 3, 0, 2);</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -49421,18 +49422,18 @@
       <c r="C193" s="4">
         <v>677</v>
       </c>
-      <c r="D193" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E193" s="4" t="s">
-        <v>18</v>
+      <c r="D193" s="4">
+        <v>2</v>
+      </c>
+      <c r="E193" s="4">
+        <v>0</v>
       </c>
       <c r="F193" s="4">
         <v>1</v>
       </c>
       <c r="G193" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1382, 336, 677, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1382, 336, 677, 2, 0, 1);</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -49863,18 +49864,18 @@
       <c r="C210" s="3">
         <v>994</v>
       </c>
-      <c r="D210" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E210" s="3" t="s">
-        <v>18</v>
+      <c r="D210" s="3">
+        <v>2</v>
+      </c>
+      <c r="E210" s="3">
+        <v>0</v>
       </c>
       <c r="F210" s="3">
         <v>2</v>
       </c>
       <c r="G210" s="3" t="str">
         <f t="shared" ref="G210:G273" si="34">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A210 &amp; ", " &amp; B210 &amp; ", " &amp; C210 &amp; ", " &amp; D210 &amp; ", " &amp; E210 &amp; ", " &amp; F210 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1399, 341, 994, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1399, 341, 994, 2, 0, 2);</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -49889,18 +49890,18 @@
       <c r="C211" s="3">
         <v>994</v>
       </c>
-      <c r="D211" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E211" s="3" t="s">
-        <v>18</v>
+      <c r="D211" s="3">
+        <v>1</v>
+      </c>
+      <c r="E211" s="3">
+        <v>0</v>
       </c>
       <c r="F211" s="3">
         <v>1</v>
       </c>
       <c r="G211" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1400, 341, 994, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1400, 341, 994, 1, 0, 1);</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -49915,18 +49916,18 @@
       <c r="C212" s="3">
         <v>34</v>
       </c>
-      <c r="D212" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E212" s="3" t="s">
-        <v>18</v>
+      <c r="D212" s="3">
+        <v>4</v>
+      </c>
+      <c r="E212" s="3">
+        <v>3</v>
       </c>
       <c r="F212" s="3">
         <v>2</v>
       </c>
       <c r="G212" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1401, 341, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1401, 341, 34, 4, 3, 2);</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -49941,18 +49942,18 @@
       <c r="C213" s="3">
         <v>34</v>
       </c>
-      <c r="D213" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E213" s="3" t="s">
-        <v>18</v>
+      <c r="D213" s="3">
+        <v>2</v>
+      </c>
+      <c r="E213" s="3">
+        <v>0</v>
       </c>
       <c r="F213" s="3">
         <v>1</v>
       </c>
       <c r="G213" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1402, 341, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1402, 341, 34, 2, 0, 1);</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -49967,18 +49968,18 @@
       <c r="C214" s="4">
         <v>98</v>
       </c>
-      <c r="D214" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E214" s="4" t="s">
-        <v>18</v>
+      <c r="D214" s="4">
+        <v>5</v>
+      </c>
+      <c r="E214" s="4">
+        <v>3</v>
       </c>
       <c r="F214" s="4">
         <v>2</v>
       </c>
       <c r="G214" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1403, 342, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1403, 342, 98, 5, 3, 2);</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -49993,18 +49994,18 @@
       <c r="C215" s="4">
         <v>98</v>
       </c>
-      <c r="D215" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E215" s="4" t="s">
-        <v>18</v>
+      <c r="D215" s="4">
+        <v>4</v>
+      </c>
+      <c r="E215" s="4">
+        <v>0</v>
       </c>
       <c r="F215" s="4">
         <v>1</v>
       </c>
       <c r="G215" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1404, 342, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1404, 342, 98, 4, 0, 1);</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -50019,18 +50020,18 @@
       <c r="C216" s="4">
         <v>212</v>
       </c>
-      <c r="D216" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E216" s="4" t="s">
-        <v>18</v>
+      <c r="D216" s="4">
+        <v>3</v>
+      </c>
+      <c r="E216" s="4">
+        <v>0</v>
       </c>
       <c r="F216" s="4">
         <v>2</v>
       </c>
       <c r="G216" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1405, 342, 212, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1405, 342, 212, 3, 0, 2);</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
@@ -50045,18 +50046,18 @@
       <c r="C217" s="4">
         <v>212</v>
       </c>
-      <c r="D217" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E217" s="4" t="s">
-        <v>18</v>
+      <c r="D217" s="4">
+        <v>2</v>
+      </c>
+      <c r="E217" s="4">
+        <v>0</v>
       </c>
       <c r="F217" s="4">
         <v>1</v>
       </c>
       <c r="G217" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1406, 342, 212, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1406, 342, 212, 2, 0, 1);</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Futsal World Cup 3rd Date and Africa Cup of Nations
Futsal World Cup 3rd Date and Round of 16. Africa Cup of Nations 1992,
1994, 1996, 1998, 2000, 2002
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -84,8 +84,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,6 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -44736,7 +44745,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -46952,18 +46961,18 @@
       <c r="C98" s="3">
         <v>507</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>18</v>
+      <c r="D98" s="3">
+        <v>3</v>
+      </c>
+      <c r="E98" s="3">
+        <v>0</v>
       </c>
       <c r="F98" s="3">
         <v>2</v>
       </c>
       <c r="G98" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1287, 313, 507, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1287, 313, 507, 3, 0, 2);</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -46978,18 +46987,18 @@
       <c r="C99" s="3">
         <v>507</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>18</v>
+      <c r="D99" s="3">
+        <v>1</v>
+      </c>
+      <c r="E99" s="3">
+        <v>0</v>
       </c>
       <c r="F99" s="3">
         <v>1</v>
       </c>
       <c r="G99" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1288, 313, 507, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1288, 313, 507, 1, 0, 1);</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -47004,18 +47013,18 @@
       <c r="C100" s="3">
         <v>57</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>18</v>
+      <c r="D100" s="3">
+        <v>4</v>
+      </c>
+      <c r="E100" s="3">
+        <v>3</v>
       </c>
       <c r="F100" s="3">
         <v>2</v>
       </c>
       <c r="G100" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1289, 313, 57, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1289, 313, 57, 4, 3, 2);</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -47030,18 +47039,18 @@
       <c r="C101" s="3">
         <v>57</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>18</v>
+      <c r="D101" s="3">
+        <v>2</v>
+      </c>
+      <c r="E101" s="3">
+        <v>0</v>
       </c>
       <c r="F101" s="3">
         <v>1</v>
       </c>
       <c r="G101" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1290, 313, 57, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1290, 313, 57, 2, 0, 1);</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -47056,18 +47065,18 @@
       <c r="C102" s="4">
         <v>351</v>
       </c>
-      <c r="D102" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>18</v>
+      <c r="D102" s="4">
+        <v>5</v>
+      </c>
+      <c r="E102" s="4">
+        <v>3</v>
       </c>
       <c r="F102" s="4">
         <v>2</v>
       </c>
       <c r="G102" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1291, 314, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1291, 314, 351, 5, 3, 2);</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -47082,18 +47091,18 @@
       <c r="C103" s="4">
         <v>351</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>18</v>
+      <c r="D103" s="4">
+        <v>2</v>
+      </c>
+      <c r="E103" s="4">
+        <v>0</v>
       </c>
       <c r="F103" s="4">
         <v>1</v>
       </c>
       <c r="G103" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1292, 314, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1292, 314, 351, 2, 0, 1);</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -47108,18 +47117,18 @@
       <c r="C104" s="4">
         <v>998</v>
       </c>
-      <c r="D104" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>18</v>
+      <c r="D104" s="4">
+        <v>1</v>
+      </c>
+      <c r="E104" s="4">
+        <v>0</v>
       </c>
       <c r="F104" s="4">
         <v>2</v>
       </c>
       <c r="G104" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1293, 314, 998, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1293, 314, 998, 1, 0, 2);</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -47134,18 +47143,18 @@
       <c r="C105" s="4">
         <v>998</v>
       </c>
-      <c r="D105" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E105" s="4" t="s">
-        <v>18</v>
+      <c r="D105" s="4">
+        <v>1</v>
+      </c>
+      <c r="E105" s="4">
+        <v>0</v>
       </c>
       <c r="F105" s="4">
         <v>1</v>
       </c>
       <c r="G105" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1294, 314, 998, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1294, 314, 998, 1, 0, 1);</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -47576,18 +47585,18 @@
       <c r="C122" s="3">
         <v>20</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>18</v>
+      <c r="D122" s="3">
+        <v>1</v>
+      </c>
+      <c r="E122" s="3">
+        <v>0</v>
       </c>
       <c r="F122" s="3">
         <v>2</v>
       </c>
       <c r="G122" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1311, 319, 20, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1311, 319, 20, 1, 0, 2);</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -47602,18 +47611,18 @@
       <c r="C123" s="3">
         <v>20</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>18</v>
+      <c r="D123" s="3">
+        <v>1</v>
+      </c>
+      <c r="E123" s="3">
+        <v>0</v>
       </c>
       <c r="F123" s="3">
         <v>1</v>
       </c>
       <c r="G123" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1312, 319, 20, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1312, 319, 20, 1, 0, 1);</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -47628,18 +47637,18 @@
       <c r="C124" s="3">
         <v>66</v>
       </c>
-      <c r="D124" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>18</v>
+      <c r="D124" s="3">
+        <v>2</v>
+      </c>
+      <c r="E124" s="3">
+        <v>3</v>
       </c>
       <c r="F124" s="3">
         <v>2</v>
       </c>
       <c r="G124" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1313, 319, 66, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1313, 319, 66, 2, 3, 2);</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -47654,18 +47663,18 @@
       <c r="C125" s="3">
         <v>66</v>
       </c>
-      <c r="D125" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>18</v>
+      <c r="D125" s="3">
+        <v>1</v>
+      </c>
+      <c r="E125" s="3">
+        <v>0</v>
       </c>
       <c r="F125" s="3">
         <v>1</v>
       </c>
       <c r="G125" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1314, 319, 66, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1314, 319, 66, 1, 0, 1);</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -47680,18 +47689,18 @@
       <c r="C126" s="4">
         <v>7</v>
       </c>
-      <c r="D126" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E126" s="4" t="s">
-        <v>18</v>
+      <c r="D126" s="4">
+        <v>7</v>
+      </c>
+      <c r="E126" s="4">
+        <v>3</v>
       </c>
       <c r="F126" s="4">
         <v>2</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1315, 320, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1315, 320, 7, 7, 3, 2);</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -47706,18 +47715,18 @@
       <c r="C127" s="4">
         <v>7</v>
       </c>
-      <c r="D127" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E127" s="4" t="s">
-        <v>18</v>
+      <c r="D127" s="4">
+        <v>4</v>
+      </c>
+      <c r="E127" s="4">
+        <v>0</v>
       </c>
       <c r="F127" s="4">
         <v>1</v>
       </c>
       <c r="G127" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1316, 320, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1316, 320, 7, 4, 0, 1);</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -47732,18 +47741,18 @@
       <c r="C128" s="4">
         <v>53</v>
       </c>
-      <c r="D128" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E128" s="4" t="s">
-        <v>18</v>
+      <c r="D128" s="4">
+        <v>1</v>
+      </c>
+      <c r="E128" s="4">
+        <v>0</v>
       </c>
       <c r="F128" s="4">
         <v>2</v>
       </c>
       <c r="G128" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1317, 320, 53, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1317, 320, 53, 1, 0, 2);</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -47758,18 +47767,18 @@
       <c r="C129" s="4">
         <v>53</v>
       </c>
-      <c r="D129" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E129" s="4" t="s">
-        <v>18</v>
+      <c r="D129" s="4">
+        <v>0</v>
+      </c>
+      <c r="E129" s="4">
+        <v>0</v>
       </c>
       <c r="F129" s="4">
         <v>1</v>
       </c>
       <c r="G129" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1318, 320, 53, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1318, 320, 53, 0, 0, 1);</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -47996,14 +48005,14 @@
         <v>1</v>
       </c>
       <c r="E138" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F138" s="3">
         <v>2</v>
       </c>
       <c r="G138" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1327, 323, 502, 1, 3, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1327, 323, 502, 1, 0, 2);</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -48048,14 +48057,14 @@
         <v>5</v>
       </c>
       <c r="E140" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F140" s="3">
         <v>2</v>
       </c>
       <c r="G140" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1329, 323, 39, 5, 0, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1329, 323, 39, 5, 3, 2);</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -48200,18 +48209,18 @@
       <c r="C146" s="3">
         <v>502</v>
       </c>
-      <c r="D146" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E146" s="3" t="s">
-        <v>18</v>
+      <c r="D146" s="3">
+        <v>4</v>
+      </c>
+      <c r="E146" s="3">
+        <v>0</v>
       </c>
       <c r="F146" s="3">
         <v>2</v>
       </c>
       <c r="G146" s="3" t="str">
         <f t="shared" ref="G146:G209" si="20">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A146 &amp; ", " &amp; B146 &amp; ", " &amp; C146 &amp; ", " &amp; D146 &amp; ", " &amp; E146 &amp; ", " &amp; F146 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1335, 325, 502, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1335, 325, 502, 4, 0, 2);</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -48226,18 +48235,18 @@
       <c r="C147" s="3">
         <v>502</v>
       </c>
-      <c r="D147" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>18</v>
+      <c r="D147" s="3">
+        <v>2</v>
+      </c>
+      <c r="E147" s="3">
+        <v>0</v>
       </c>
       <c r="F147" s="3">
         <v>1</v>
       </c>
       <c r="G147" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1336, 325, 502, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1336, 325, 502, 2, 0, 1);</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -48252,18 +48261,18 @@
       <c r="C148" s="3">
         <v>595</v>
       </c>
-      <c r="D148" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>18</v>
+      <c r="D148" s="3">
+        <v>8</v>
+      </c>
+      <c r="E148" s="3">
+        <v>3</v>
       </c>
       <c r="F148" s="3">
         <v>2</v>
       </c>
       <c r="G148" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1337, 325, 595, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1337, 325, 595, 8, 3, 2);</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -48278,18 +48287,18 @@
       <c r="C149" s="3">
         <v>595</v>
       </c>
-      <c r="D149" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>18</v>
+      <c r="D149" s="3">
+        <v>3</v>
+      </c>
+      <c r="E149" s="3">
+        <v>0</v>
       </c>
       <c r="F149" s="3">
         <v>1</v>
       </c>
       <c r="G149" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1338, 325, 595, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1338, 325, 595, 3, 0, 1);</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -48304,18 +48313,18 @@
       <c r="C150" s="4">
         <v>39</v>
       </c>
-      <c r="D150" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E150" s="4" t="s">
-        <v>18</v>
+      <c r="D150" s="4">
+        <v>2</v>
+      </c>
+      <c r="E150" s="4">
+        <v>3</v>
       </c>
       <c r="F150" s="4">
         <v>2</v>
       </c>
       <c r="G150" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1339, 326, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1339, 326, 39, 2, 3, 2);</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -48330,18 +48339,18 @@
       <c r="C151" s="4">
         <v>39</v>
       </c>
-      <c r="D151" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E151" s="4" t="s">
-        <v>18</v>
+      <c r="D151" s="4">
+        <v>1</v>
+      </c>
+      <c r="E151" s="4">
+        <v>0</v>
       </c>
       <c r="F151" s="4">
         <v>1</v>
       </c>
       <c r="G151" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1340, 326, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1340, 326, 39, 1, 0, 1);</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -48356,18 +48365,18 @@
       <c r="C152" s="4">
         <v>84</v>
       </c>
-      <c r="D152" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E152" s="4" t="s">
-        <v>18</v>
+      <c r="D152" s="4">
+        <v>0</v>
+      </c>
+      <c r="E152" s="4">
+        <v>0</v>
       </c>
       <c r="F152" s="4">
         <v>2</v>
       </c>
       <c r="G152" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1341, 326, 84, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1341, 326, 84, 0, 0, 2);</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -48382,18 +48391,18 @@
       <c r="C153" s="4">
         <v>84</v>
       </c>
-      <c r="D153" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E153" s="4" t="s">
-        <v>18</v>
+      <c r="D153" s="4">
+        <v>0</v>
+      </c>
+      <c r="E153" s="4">
+        <v>0</v>
       </c>
       <c r="F153" s="4">
         <v>1</v>
       </c>
       <c r="G153" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1342, 326, 84, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1342, 326, 84, 0, 0, 1);</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -48824,18 +48833,18 @@
       <c r="C170" s="3">
         <v>61</v>
       </c>
-      <c r="D170" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>18</v>
+      <c r="D170" s="3">
+        <v>1</v>
+      </c>
+      <c r="E170" s="3">
+        <v>0</v>
       </c>
       <c r="F170" s="3">
         <v>2</v>
       </c>
       <c r="G170" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1359, 331, 61, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1359, 331, 61, 1, 0, 2);</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -48850,18 +48859,18 @@
       <c r="C171" s="3">
         <v>61</v>
       </c>
-      <c r="D171" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>18</v>
+      <c r="D171" s="3">
+        <v>0</v>
+      </c>
+      <c r="E171" s="3">
+        <v>0</v>
       </c>
       <c r="F171" s="3">
         <v>1</v>
       </c>
       <c r="G171" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1360, 331, 61, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1360, 331, 61, 0, 0, 1);</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -48876,18 +48885,18 @@
       <c r="C172" s="3">
         <v>380</v>
       </c>
-      <c r="D172" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>18</v>
+      <c r="D172" s="3">
+        <v>3</v>
+      </c>
+      <c r="E172" s="3">
+        <v>3</v>
       </c>
       <c r="F172" s="3">
         <v>2</v>
       </c>
       <c r="G172" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1361, 331, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1361, 331, 380, 3, 3, 2);</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -48902,18 +48911,18 @@
       <c r="C173" s="3">
         <v>380</v>
       </c>
-      <c r="D173" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>18</v>
+      <c r="D173" s="3">
+        <v>1</v>
+      </c>
+      <c r="E173" s="3">
+        <v>0</v>
       </c>
       <c r="F173" s="3">
         <v>1</v>
       </c>
       <c r="G173" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1362, 331, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1362, 331, 380, 1, 0, 1);</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -48928,18 +48937,18 @@
       <c r="C174" s="4">
         <v>55</v>
       </c>
-      <c r="D174" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E174" s="4" t="s">
-        <v>18</v>
+      <c r="D174" s="4">
+        <v>15</v>
+      </c>
+      <c r="E174" s="4">
+        <v>3</v>
       </c>
       <c r="F174" s="4">
         <v>2</v>
       </c>
       <c r="G174" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1363, 332, 55, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1363, 332, 55, 15, 3, 2);</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -48954,18 +48963,18 @@
       <c r="C175" s="4">
         <v>55</v>
       </c>
-      <c r="D175" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E175" s="4" t="s">
-        <v>18</v>
+      <c r="D175" s="4">
+        <v>8</v>
+      </c>
+      <c r="E175" s="4">
+        <v>0</v>
       </c>
       <c r="F175" s="4">
         <v>1</v>
       </c>
       <c r="G175" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1364, 332, 55, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1364, 332, 55, 8, 0, 1);</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -48980,18 +48989,18 @@
       <c r="C176" s="4">
         <v>258</v>
       </c>
-      <c r="D176" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E176" s="4" t="s">
-        <v>18</v>
+      <c r="D176" s="4">
+        <v>3</v>
+      </c>
+      <c r="E176" s="4">
+        <v>0</v>
       </c>
       <c r="F176" s="4">
         <v>2</v>
       </c>
       <c r="G176" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1365, 332, 258, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1365, 332, 258, 3, 0, 2);</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -49006,18 +49015,18 @@
       <c r="C177" s="4">
         <v>258</v>
       </c>
-      <c r="D177" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E177" s="4" t="s">
-        <v>18</v>
+      <c r="D177" s="4">
+        <v>1</v>
+      </c>
+      <c r="E177" s="4">
+        <v>0</v>
       </c>
       <c r="F177" s="4">
         <v>1</v>
       </c>
       <c r="G177" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1366, 332, 258, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1366, 332, 258, 1, 0, 1);</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -49448,18 +49457,18 @@
       <c r="C194" s="3">
         <v>506</v>
       </c>
-      <c r="D194" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E194" s="3" t="s">
-        <v>18</v>
+      <c r="D194" s="3">
+        <v>2</v>
+      </c>
+      <c r="E194" s="3">
+        <v>1</v>
       </c>
       <c r="F194" s="3">
         <v>2</v>
       </c>
       <c r="G194" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1383, 337, 506, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1383, 337, 506, 2, 1, 2);</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -49474,18 +49483,18 @@
       <c r="C195" s="3">
         <v>506</v>
       </c>
-      <c r="D195" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>18</v>
+      <c r="D195" s="3">
+        <v>1</v>
+      </c>
+      <c r="E195" s="3">
+        <v>0</v>
       </c>
       <c r="F195" s="3">
         <v>1</v>
       </c>
       <c r="G195" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1384, 337, 506, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1384, 337, 506, 1, 0, 1);</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -49500,18 +49509,18 @@
       <c r="C196" s="3">
         <v>54</v>
       </c>
-      <c r="D196" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>18</v>
+      <c r="D196" s="3">
+        <v>2</v>
+      </c>
+      <c r="E196" s="3">
+        <v>1</v>
       </c>
       <c r="F196" s="3">
         <v>2</v>
       </c>
       <c r="G196" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1385, 337, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1385, 337, 54, 2, 1, 2);</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -49526,18 +49535,18 @@
       <c r="C197" s="3">
         <v>54</v>
       </c>
-      <c r="D197" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E197" s="3" t="s">
-        <v>18</v>
+      <c r="D197" s="3">
+        <v>0</v>
+      </c>
+      <c r="E197" s="3">
+        <v>0</v>
       </c>
       <c r="F197" s="3">
         <v>1</v>
       </c>
       <c r="G197" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1386, 337, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1386, 337, 54, 0, 0, 1);</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -49552,18 +49561,18 @@
       <c r="C198" s="4">
         <v>76</v>
       </c>
-      <c r="D198" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>18</v>
+      <c r="D198" s="4">
+        <v>10</v>
+      </c>
+      <c r="E198" s="4">
+        <v>3</v>
       </c>
       <c r="F198" s="4">
         <v>2</v>
       </c>
       <c r="G198" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1387, 338, 76, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1387, 338, 76, 10, 3, 2);</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -49578,18 +49587,18 @@
       <c r="C199" s="4">
         <v>76</v>
       </c>
-      <c r="D199" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E199" s="4" t="s">
-        <v>18</v>
+      <c r="D199" s="4">
+        <v>4</v>
+      </c>
+      <c r="E199" s="4">
+        <v>0</v>
       </c>
       <c r="F199" s="4">
         <v>1</v>
       </c>
       <c r="G199" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1388, 338, 76, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1388, 338, 76, 4, 0, 1);</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -49604,18 +49613,18 @@
       <c r="C200" s="4">
         <v>677</v>
       </c>
-      <c r="D200" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E200" s="4" t="s">
-        <v>18</v>
+      <c r="D200" s="4">
+        <v>0</v>
+      </c>
+      <c r="E200" s="4">
+        <v>0</v>
       </c>
       <c r="F200" s="4">
         <v>2</v>
       </c>
       <c r="G200" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1389, 338, 677, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1389, 338, 677, 0, 0, 2);</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -49630,18 +49639,18 @@
       <c r="C201" s="4">
         <v>677</v>
       </c>
-      <c r="D201" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E201" s="4" t="s">
-        <v>18</v>
+      <c r="D201" s="4">
+        <v>0</v>
+      </c>
+      <c r="E201" s="4">
+        <v>0</v>
       </c>
       <c r="F201" s="4">
         <v>1</v>
       </c>
       <c r="G201" s="4" t="str">
         <f t="shared" si="20"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1390, 338, 677, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1390, 338, 677, 0, 0, 1);</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -50072,18 +50081,18 @@
       <c r="C218" s="3">
         <v>994</v>
       </c>
-      <c r="D218" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E218" s="3" t="s">
-        <v>18</v>
+      <c r="D218" s="3">
+        <v>3</v>
+      </c>
+      <c r="E218" s="3">
+        <v>1</v>
       </c>
       <c r="F218" s="3">
         <v>2</v>
       </c>
       <c r="G218" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1407, 343, 994, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1407, 343, 994, 3, 1, 2);</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -50098,18 +50107,18 @@
       <c r="C219" s="3">
         <v>994</v>
       </c>
-      <c r="D219" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E219" s="3" t="s">
-        <v>18</v>
+      <c r="D219" s="3">
+        <v>1</v>
+      </c>
+      <c r="E219" s="3">
+        <v>0</v>
       </c>
       <c r="F219" s="3">
         <v>1</v>
       </c>
       <c r="G219" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1408, 343, 994, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1408, 343, 994, 1, 0, 1);</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -50124,18 +50133,18 @@
       <c r="C220" s="3">
         <v>98</v>
       </c>
-      <c r="D220" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E220" s="3" t="s">
-        <v>18</v>
+      <c r="D220" s="3">
+        <v>3</v>
+      </c>
+      <c r="E220" s="3">
+        <v>1</v>
       </c>
       <c r="F220" s="3">
         <v>2</v>
       </c>
       <c r="G220" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1409, 343, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1409, 343, 98, 3, 1, 2);</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -50150,18 +50159,18 @@
       <c r="C221" s="3">
         <v>98</v>
       </c>
-      <c r="D221" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E221" s="3" t="s">
-        <v>18</v>
+      <c r="D221" s="3">
+        <v>1</v>
+      </c>
+      <c r="E221" s="3">
+        <v>0</v>
       </c>
       <c r="F221" s="3">
         <v>1</v>
       </c>
       <c r="G221" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1410, 343, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1410, 343, 98, 1, 0, 1);</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -50176,18 +50185,18 @@
       <c r="C222" s="4">
         <v>34</v>
       </c>
-      <c r="D222" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E222" s="4" t="s">
-        <v>18</v>
+      <c r="D222" s="4">
+        <v>4</v>
+      </c>
+      <c r="E222" s="4">
+        <v>3</v>
       </c>
       <c r="F222" s="4">
         <v>2</v>
       </c>
       <c r="G222" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1411, 344, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1411, 344, 34, 4, 3, 2);</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -50202,18 +50211,18 @@
       <c r="C223" s="4">
         <v>34</v>
       </c>
-      <c r="D223" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E223" s="4" t="s">
-        <v>18</v>
+      <c r="D223" s="4">
+        <v>3</v>
+      </c>
+      <c r="E223" s="4">
+        <v>0</v>
       </c>
       <c r="F223" s="4">
         <v>1</v>
       </c>
       <c r="G223" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1412, 344, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1412, 344, 34, 3, 0, 1);</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -50228,18 +50237,18 @@
       <c r="C224" s="4">
         <v>212</v>
       </c>
-      <c r="D224" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E224" s="4" t="s">
-        <v>18</v>
+      <c r="D224" s="4">
+        <v>3</v>
+      </c>
+      <c r="E224" s="4">
+        <v>0</v>
       </c>
       <c r="F224" s="4">
         <v>2</v>
       </c>
       <c r="G224" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1413, 344, 212, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1413, 344, 212, 3, 0, 2);</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -50254,18 +50263,18 @@
       <c r="C225" s="4">
         <v>212</v>
       </c>
-      <c r="D225" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E225" s="4" t="s">
-        <v>18</v>
+      <c r="D225" s="4">
+        <v>1</v>
+      </c>
+      <c r="E225" s="4">
+        <v>0</v>
       </c>
       <c r="F225" s="4">
         <v>1</v>
       </c>
       <c r="G225" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1414, 344, 212, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1414, 344, 212, 1, 0, 1);</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -50277,8 +50286,8 @@
         <f>B222+1</f>
         <v>345</v>
       </c>
-      <c r="C226" s="3" t="s">
-        <v>18</v>
+      <c r="C226" s="3">
+        <v>57</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>18</v>
@@ -50291,7 +50300,7 @@
       </c>
       <c r="G226" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1415, 345, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1415, 345, 57, null, null, 2);</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -50303,8 +50312,8 @@
         <f>B226</f>
         <v>345</v>
       </c>
-      <c r="C227" s="3" t="s">
-        <v>18</v>
+      <c r="C227" s="3">
+        <v>57</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>18</v>
@@ -50317,7 +50326,7 @@
       </c>
       <c r="G227" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1416, 345, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1416, 345, 57, null, null, 1);</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -50329,8 +50338,8 @@
         <f>B226</f>
         <v>345</v>
       </c>
-      <c r="C228" s="3" t="s">
-        <v>18</v>
+      <c r="C228" s="3">
+        <v>595</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>18</v>
@@ -50343,7 +50352,7 @@
       </c>
       <c r="G228" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1417, 345, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1417, 345, 595, null, null, 2);</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -50355,8 +50364,8 @@
         <f t="shared" ref="B229" si="40">B226</f>
         <v>345</v>
       </c>
-      <c r="C229" s="3" t="s">
-        <v>18</v>
+      <c r="C229" s="3">
+        <v>595</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>18</v>
@@ -50369,7 +50378,7 @@
       </c>
       <c r="G229" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1418, 345, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1418, 345, 595, null, null, 1);</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -50381,8 +50390,8 @@
         <f>B226+1</f>
         <v>346</v>
       </c>
-      <c r="C230" s="4" t="s">
-        <v>18</v>
+      <c r="C230" s="4">
+        <v>55</v>
       </c>
       <c r="D230" s="4" t="s">
         <v>18</v>
@@ -50395,7 +50404,7 @@
       </c>
       <c r="G230" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1419, 346, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1419, 346, 55, null, null, 2);</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -50407,8 +50416,8 @@
         <f>B230</f>
         <v>346</v>
       </c>
-      <c r="C231" s="4" t="s">
-        <v>18</v>
+      <c r="C231" s="4">
+        <v>55</v>
       </c>
       <c r="D231" s="4" t="s">
         <v>18</v>
@@ -50421,7 +50430,7 @@
       </c>
       <c r="G231" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1420, 346, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1420, 346, 55, null, null, 1);</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -50433,8 +50442,8 @@
         <f>B230</f>
         <v>346</v>
       </c>
-      <c r="C232" s="4" t="s">
-        <v>18</v>
+      <c r="C232" s="4">
+        <v>98</v>
       </c>
       <c r="D232" s="4" t="s">
         <v>18</v>
@@ -50447,7 +50456,7 @@
       </c>
       <c r="G232" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1421, 346, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1421, 346, 98, null, null, 2);</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -50459,8 +50468,8 @@
         <f t="shared" ref="B233" si="41">B230</f>
         <v>346</v>
       </c>
-      <c r="C233" s="4" t="s">
-        <v>18</v>
+      <c r="C233" s="4">
+        <v>98</v>
       </c>
       <c r="D233" s="4" t="s">
         <v>18</v>
@@ -50473,7 +50482,7 @@
       </c>
       <c r="G233" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1422, 346, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1422, 346, 98, null, null, 1);</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -50485,8 +50494,8 @@
         <f>B230+1</f>
         <v>347</v>
       </c>
-      <c r="C234" s="3" t="s">
-        <v>18</v>
+      <c r="C234" s="3">
+        <v>7</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>18</v>
@@ -50499,7 +50508,7 @@
       </c>
       <c r="G234" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1423, 347, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1423, 347, 7, null, null, 2);</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -50511,8 +50520,8 @@
         <f>B234</f>
         <v>347</v>
       </c>
-      <c r="C235" s="3" t="s">
-        <v>18</v>
+      <c r="C235" s="3">
+        <v>7</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>18</v>
@@ -50525,7 +50534,7 @@
       </c>
       <c r="G235" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1424, 347, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1424, 347, 7, null, null, 1);</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -50537,8 +50546,8 @@
         <f>B234</f>
         <v>347</v>
       </c>
-      <c r="C236" s="3" t="s">
-        <v>18</v>
+      <c r="C236" s="3">
+        <v>84</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>18</v>
@@ -50551,7 +50560,7 @@
       </c>
       <c r="G236" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1425, 347, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1425, 347, 84, null, null, 2);</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -50563,8 +50572,8 @@
         <f t="shared" ref="B237" si="42">B234</f>
         <v>347</v>
       </c>
-      <c r="C237" s="3" t="s">
-        <v>18</v>
+      <c r="C237" s="3">
+        <v>84</v>
       </c>
       <c r="D237" s="3" t="s">
         <v>18</v>
@@ -50577,7 +50586,7 @@
       </c>
       <c r="G237" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1426, 347, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1426, 347, 84, null, null, 1);</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -50589,8 +50598,8 @@
         <f>B234+1</f>
         <v>348</v>
       </c>
-      <c r="C238" s="4" t="s">
-        <v>18</v>
+      <c r="C238" s="4">
+        <v>34</v>
       </c>
       <c r="D238" s="4" t="s">
         <v>18</v>
@@ -50603,7 +50612,7 @@
       </c>
       <c r="G238" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1427, 348, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1427, 348, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -50615,8 +50624,8 @@
         <f>B238</f>
         <v>348</v>
       </c>
-      <c r="C239" s="4" t="s">
-        <v>18</v>
+      <c r="C239" s="4">
+        <v>34</v>
       </c>
       <c r="D239" s="4" t="s">
         <v>18</v>
@@ -50629,7 +50638,7 @@
       </c>
       <c r="G239" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1428, 348, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1428, 348, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
@@ -50641,8 +50650,8 @@
         <f>B238</f>
         <v>348</v>
       </c>
-      <c r="C240" s="4" t="s">
-        <v>18</v>
+      <c r="C240" s="4">
+        <v>76</v>
       </c>
       <c r="D240" s="4" t="s">
         <v>18</v>
@@ -50655,7 +50664,7 @@
       </c>
       <c r="G240" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1429, 348, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1429, 348, 76, null, null, 2);</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -50667,8 +50676,8 @@
         <f t="shared" ref="B241" si="43">B238</f>
         <v>348</v>
       </c>
-      <c r="C241" s="4" t="s">
-        <v>18</v>
+      <c r="C241" s="4">
+        <v>76</v>
       </c>
       <c r="D241" s="4" t="s">
         <v>18</v>
@@ -50681,7 +50690,7 @@
       </c>
       <c r="G241" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1430, 348, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1430, 348, 76, null, null, 1);</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -50693,8 +50702,8 @@
         <f>B238+1</f>
         <v>349</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>18</v>
+      <c r="C242" s="3">
+        <v>54</v>
       </c>
       <c r="D242" s="3" t="s">
         <v>18</v>
@@ -50707,7 +50716,7 @@
       </c>
       <c r="G242" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1431, 349, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1431, 349, 54, null, null, 2);</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -50719,8 +50728,8 @@
         <f>B242</f>
         <v>349</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>18</v>
+      <c r="C243" s="3">
+        <v>54</v>
       </c>
       <c r="D243" s="3" t="s">
         <v>18</v>
@@ -50733,7 +50742,7 @@
       </c>
       <c r="G243" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1432, 349, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1432, 349, 54, null, null, 1);</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -50745,8 +50754,8 @@
         <f>B242</f>
         <v>349</v>
       </c>
-      <c r="C244" s="3" t="s">
-        <v>18</v>
+      <c r="C244" s="3">
+        <v>380</v>
       </c>
       <c r="D244" s="3" t="s">
         <v>18</v>
@@ -50759,7 +50768,7 @@
       </c>
       <c r="G244" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1433, 349, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1433, 349, 380, null, null, 2);</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -50771,8 +50780,8 @@
         <f t="shared" ref="B245" si="44">B242</f>
         <v>349</v>
       </c>
-      <c r="C245" s="3" t="s">
-        <v>18</v>
+      <c r="C245" s="3">
+        <v>380</v>
       </c>
       <c r="D245" s="3" t="s">
         <v>18</v>
@@ -50785,7 +50794,7 @@
       </c>
       <c r="G245" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1434, 349, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1434, 349, 380, null, null, 1);</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -50797,8 +50806,8 @@
         <f>B242+1</f>
         <v>350</v>
       </c>
-      <c r="C246" s="4" t="s">
-        <v>18</v>
+      <c r="C246" s="4">
+        <v>39</v>
       </c>
       <c r="D246" s="4" t="s">
         <v>18</v>
@@ -50811,7 +50820,7 @@
       </c>
       <c r="G246" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1435, 350, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1435, 350, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -50823,8 +50832,8 @@
         <f>B246</f>
         <v>350</v>
       </c>
-      <c r="C247" s="4" t="s">
-        <v>18</v>
+      <c r="C247" s="4">
+        <v>39</v>
       </c>
       <c r="D247" s="4" t="s">
         <v>18</v>
@@ -50837,7 +50846,7 @@
       </c>
       <c r="G247" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1436, 350, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1436, 350, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -50849,8 +50858,8 @@
         <f>B246</f>
         <v>350</v>
       </c>
-      <c r="C248" s="4" t="s">
-        <v>18</v>
+      <c r="C248" s="4">
+        <v>20</v>
       </c>
       <c r="D248" s="4" t="s">
         <v>18</v>
@@ -50863,7 +50872,7 @@
       </c>
       <c r="G248" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1437, 350, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1437, 350, 20, null, null, 2);</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -50875,8 +50884,8 @@
         <f t="shared" ref="B249" si="45">B246</f>
         <v>350</v>
       </c>
-      <c r="C249" s="4" t="s">
-        <v>18</v>
+      <c r="C249" s="4">
+        <v>20</v>
       </c>
       <c r="D249" s="4" t="s">
         <v>18</v>
@@ -50889,7 +50898,7 @@
       </c>
       <c r="G249" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1438, 350, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1438, 350, 20, null, null, 1);</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -50901,8 +50910,8 @@
         <f>B246+1</f>
         <v>351</v>
       </c>
-      <c r="C250" s="3" t="s">
-        <v>18</v>
+      <c r="C250" s="3">
+        <v>66</v>
       </c>
       <c r="D250" s="3" t="s">
         <v>18</v>
@@ -50915,7 +50924,7 @@
       </c>
       <c r="G250" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1439, 351, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1439, 351, 66, null, null, 2);</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -50927,8 +50936,8 @@
         <f>B250</f>
         <v>351</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>18</v>
+      <c r="C251" s="3">
+        <v>66</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>18</v>
@@ -50941,7 +50950,7 @@
       </c>
       <c r="G251" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1440, 351, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1440, 351, 66, null, null, 1);</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -50953,8 +50962,8 @@
         <f>B250</f>
         <v>351</v>
       </c>
-      <c r="C252" s="3" t="s">
-        <v>18</v>
+      <c r="C252" s="3">
+        <v>994</v>
       </c>
       <c r="D252" s="3" t="s">
         <v>18</v>
@@ -50967,7 +50976,7 @@
       </c>
       <c r="G252" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1441, 351, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1441, 351, 994, null, null, 2);</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -50979,8 +50988,8 @@
         <f t="shared" ref="B253" si="46">B250</f>
         <v>351</v>
       </c>
-      <c r="C253" s="3" t="s">
-        <v>18</v>
+      <c r="C253" s="3">
+        <v>994</v>
       </c>
       <c r="D253" s="3" t="s">
         <v>18</v>
@@ -50993,7 +51002,7 @@
       </c>
       <c r="G253" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1442, 351, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1442, 351, 994, null, null, 1);</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -51005,8 +51014,8 @@
         <f>B250+1</f>
         <v>352</v>
       </c>
-      <c r="C254" s="4" t="s">
-        <v>18</v>
+      <c r="C254" s="4">
+        <v>351</v>
       </c>
       <c r="D254" s="4" t="s">
         <v>18</v>
@@ -51019,7 +51028,7 @@
       </c>
       <c r="G254" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1443, 352, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1443, 352, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -51031,8 +51040,8 @@
         <f>B254</f>
         <v>352</v>
       </c>
-      <c r="C255" s="4" t="s">
-        <v>18</v>
+      <c r="C255" s="4">
+        <v>351</v>
       </c>
       <c r="D255" s="4" t="s">
         <v>18</v>
@@ -51045,7 +51054,7 @@
       </c>
       <c r="G255" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1444, 352, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1444, 352, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -51057,8 +51066,8 @@
         <f>B254</f>
         <v>352</v>
       </c>
-      <c r="C256" s="4" t="s">
-        <v>18</v>
+      <c r="C256" s="4">
+        <v>506</v>
       </c>
       <c r="D256" s="4" t="s">
         <v>18</v>
@@ -51071,7 +51080,7 @@
       </c>
       <c r="G256" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1445, 352, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1445, 352, 506, null, null, 2);</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -51083,8 +51092,8 @@
         <f t="shared" ref="B257" si="47">B254</f>
         <v>352</v>
       </c>
-      <c r="C257" s="4" t="s">
-        <v>18</v>
+      <c r="C257" s="4">
+        <v>506</v>
       </c>
       <c r="D257" s="4" t="s">
         <v>18</v>
@@ -51097,7 +51106,7 @@
       </c>
       <c r="G257" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1446, 352, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1446, 352, 506, null, null, 1);</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -51934,5 +51943,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FutsalWorldCup Round of 16 Date 1
FutsalWorldCup Round of 16 Date 1
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -44729,7 +44729,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G289"/>
+  <dimension ref="A1:G295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -47612,7 +47612,7 @@
         <v>20</v>
       </c>
       <c r="D123" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123" s="3">
         <v>0</v>
@@ -47622,7 +47622,7 @@
       </c>
       <c r="G123" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1312, 319, 20, 1, 0, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1312, 319, 20, 0, 0, 1);</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -49883,7 +49883,7 @@
         <v>2</v>
       </c>
       <c r="G210" s="3" t="str">
-        <f t="shared" ref="G210:G273" si="34">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A210 &amp; ", " &amp; B210 &amp; ", " &amp; C210 &amp; ", " &amp; D210 &amp; ", " &amp; E210 &amp; ", " &amp; F210 &amp; ");"</f>
+        <f t="shared" ref="G210:G279" si="34">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A210 &amp; ", " &amp; B210 &amp; ", " &amp; C210 &amp; ", " &amp; D210 &amp; ", " &amp; E210 &amp; ", " &amp; F210 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1399, 341, 994, 2, 0, 2);</v>
       </c>
     </row>
@@ -49967,7 +49967,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
-        <f t="shared" ref="A214:A277" si="36">A213+1</f>
+        <f t="shared" ref="A214:A283" si="36">A213+1</f>
         <v>1403</v>
       </c>
       <c r="B214" s="4">
@@ -50287,20 +50287,20 @@
         <v>345</v>
       </c>
       <c r="C226" s="3">
-        <v>57</v>
-      </c>
-      <c r="D226" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E226" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D226" s="3">
+        <v>7</v>
+      </c>
+      <c r="E226" s="3">
+        <v>3</v>
       </c>
       <c r="F226" s="3">
         <v>2</v>
       </c>
       <c r="G226" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1415, 345, 57, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1415, 345, 7, 7, 3, 2);</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -50313,20 +50313,20 @@
         <v>345</v>
       </c>
       <c r="C227" s="3">
-        <v>57</v>
-      </c>
-      <c r="D227" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E227" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D227" s="3">
+        <v>4</v>
+      </c>
+      <c r="E227" s="3">
+        <v>0</v>
       </c>
       <c r="F227" s="3">
         <v>1</v>
       </c>
       <c r="G227" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1416, 345, 57, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1416, 345, 7, 4, 0, 1);</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -50339,20 +50339,20 @@
         <v>345</v>
       </c>
       <c r="C228" s="3">
-        <v>595</v>
-      </c>
-      <c r="D228" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E228" s="3" t="s">
-        <v>18</v>
+        <v>84</v>
+      </c>
+      <c r="D228" s="3">
+        <v>0</v>
+      </c>
+      <c r="E228" s="3">
+        <v>0</v>
       </c>
       <c r="F228" s="3">
         <v>2</v>
       </c>
       <c r="G228" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1417, 345, 595, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1417, 345, 84, 0, 0, 2);</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -50365,20 +50365,20 @@
         <v>345</v>
       </c>
       <c r="C229" s="3">
-        <v>595</v>
-      </c>
-      <c r="D229" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E229" s="3" t="s">
-        <v>18</v>
+        <v>84</v>
+      </c>
+      <c r="D229" s="3">
+        <v>0</v>
+      </c>
+      <c r="E229" s="3">
+        <v>0</v>
       </c>
       <c r="F229" s="3">
         <v>1</v>
       </c>
       <c r="G229" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1418, 345, 595, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1418, 345, 84, 0, 0, 1);</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -50391,20 +50391,20 @@
         <v>346</v>
       </c>
       <c r="C230" s="4">
-        <v>55</v>
-      </c>
-      <c r="D230" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E230" s="4" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="D230" s="4">
+        <v>0</v>
+      </c>
+      <c r="E230" s="4">
+        <v>0</v>
       </c>
       <c r="F230" s="4">
         <v>2</v>
       </c>
       <c r="G230" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1419, 346, 55, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1419, 346, 57, 0, 0, 2);</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -50417,20 +50417,20 @@
         <v>346</v>
       </c>
       <c r="C231" s="4">
-        <v>55</v>
-      </c>
-      <c r="D231" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E231" s="4" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="D231" s="4">
+        <v>0</v>
+      </c>
+      <c r="E231" s="4">
+        <v>0</v>
       </c>
       <c r="F231" s="4">
         <v>1</v>
       </c>
       <c r="G231" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1420, 346, 55, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1420, 346, 57, 0, 0, 1);</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -50443,20 +50443,20 @@
         <v>346</v>
       </c>
       <c r="C232" s="4">
-        <v>98</v>
-      </c>
-      <c r="D232" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E232" s="4" t="s">
-        <v>18</v>
+        <v>595</v>
+      </c>
+      <c r="D232" s="4">
+        <v>0</v>
+      </c>
+      <c r="E232" s="4">
+        <v>0</v>
       </c>
       <c r="F232" s="4">
         <v>2</v>
       </c>
       <c r="G232" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1421, 346, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1421, 346, 595, 0, 0, 2);</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -50465,128 +50465,128 @@
         <v>1422</v>
       </c>
       <c r="B233" s="4">
-        <f t="shared" ref="B233" si="41">B230</f>
+        <f t="shared" ref="B233:B239" si="41">B230</f>
         <v>346</v>
       </c>
       <c r="C233" s="4">
-        <v>98</v>
-      </c>
-      <c r="D233" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E233" s="4" t="s">
-        <v>18</v>
+        <v>595</v>
+      </c>
+      <c r="D233" s="4">
+        <v>0</v>
+      </c>
+      <c r="E233" s="4">
+        <v>0</v>
       </c>
       <c r="F233" s="4">
         <v>1</v>
       </c>
       <c r="G233" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1422, 346, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1422, 346, 595, 0, 0, 1);</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A234" s="3">
+      <c r="A234" s="4">
         <f t="shared" si="36"/>
         <v>1423</v>
       </c>
-      <c r="B234" s="3">
-        <f>B230+1</f>
-        <v>347</v>
-      </c>
-      <c r="C234" s="3">
-        <v>7</v>
-      </c>
-      <c r="D234" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E234" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F234" s="3">
-        <v>2</v>
-      </c>
-      <c r="G234" s="3" t="str">
+      <c r="B234" s="4">
+        <f t="shared" si="41"/>
+        <v>346</v>
+      </c>
+      <c r="C234" s="4">
+        <v>57</v>
+      </c>
+      <c r="D234" s="4">
+        <v>0</v>
+      </c>
+      <c r="E234" s="4">
+        <v>1</v>
+      </c>
+      <c r="F234" s="4">
+        <v>4</v>
+      </c>
+      <c r="G234" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1423, 347, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1423, 346, 57, 0, 1, 4);</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A235" s="3">
+      <c r="A235" s="4">
         <f t="shared" si="36"/>
         <v>1424</v>
       </c>
-      <c r="B235" s="3">
-        <f>B234</f>
-        <v>347</v>
-      </c>
-      <c r="C235" s="3">
-        <v>7</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E235" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F235" s="3">
-        <v>1</v>
-      </c>
-      <c r="G235" s="3" t="str">
+      <c r="B235" s="4">
+        <f t="shared" si="41"/>
+        <v>346</v>
+      </c>
+      <c r="C235" s="4">
+        <v>57</v>
+      </c>
+      <c r="D235" s="4">
+        <v>0</v>
+      </c>
+      <c r="E235" s="4">
+        <v>0</v>
+      </c>
+      <c r="F235" s="4">
+        <v>3</v>
+      </c>
+      <c r="G235" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1424, 347, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1424, 346, 57, 0, 0, 3);</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A236" s="3">
+      <c r="A236" s="4">
         <f t="shared" si="36"/>
         <v>1425</v>
       </c>
-      <c r="B236" s="3">
-        <f>B234</f>
-        <v>347</v>
-      </c>
-      <c r="C236" s="3">
-        <v>84</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E236" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F236" s="3">
-        <v>2</v>
-      </c>
-      <c r="G236" s="3" t="str">
+      <c r="B236" s="4">
+        <f t="shared" si="41"/>
+        <v>346</v>
+      </c>
+      <c r="C236" s="4">
+        <v>595</v>
+      </c>
+      <c r="D236" s="4">
+        <v>0</v>
+      </c>
+      <c r="E236" s="4">
+        <v>1</v>
+      </c>
+      <c r="F236" s="4">
+        <v>4</v>
+      </c>
+      <c r="G236" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1425, 347, 84, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1425, 346, 595, 0, 1, 4);</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A237" s="3">
+      <c r="A237" s="4">
         <f t="shared" si="36"/>
         <v>1426</v>
       </c>
-      <c r="B237" s="3">
-        <f t="shared" ref="B237" si="42">B234</f>
-        <v>347</v>
-      </c>
-      <c r="C237" s="3">
-        <v>84</v>
-      </c>
-      <c r="D237" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E237" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F237" s="3">
-        <v>1</v>
-      </c>
-      <c r="G237" s="3" t="str">
+      <c r="B237" s="4">
+        <f t="shared" si="41"/>
+        <v>346</v>
+      </c>
+      <c r="C237" s="4">
+        <v>595</v>
+      </c>
+      <c r="D237" s="4">
+        <v>0</v>
+      </c>
+      <c r="E237" s="4">
+        <v>0</v>
+      </c>
+      <c r="F237" s="4">
+        <v>3</v>
+      </c>
+      <c r="G237" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1426, 347, 84, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1426, 346, 595, 0, 0, 3);</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -50595,24 +50595,24 @@
         <v>1427</v>
       </c>
       <c r="B238" s="4">
-        <f>B234+1</f>
-        <v>348</v>
+        <f t="shared" si="41"/>
+        <v>346</v>
       </c>
       <c r="C238" s="4">
-        <v>34</v>
-      </c>
-      <c r="D238" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E238" s="4" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="D238" s="4">
+        <v>2</v>
+      </c>
+      <c r="E238" s="4">
+        <v>0</v>
       </c>
       <c r="F238" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G238" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1427, 348, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1427, 346, 57, 2, 0, 7);</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -50621,76 +50621,76 @@
         <v>1428</v>
       </c>
       <c r="B239" s="4">
-        <f>B238</f>
-        <v>348</v>
+        <f t="shared" si="41"/>
+        <v>346</v>
       </c>
       <c r="C239" s="4">
-        <v>34</v>
-      </c>
-      <c r="D239" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E239" s="4" t="s">
-        <v>18</v>
+        <v>595</v>
+      </c>
+      <c r="D239" s="4">
+        <v>3</v>
+      </c>
+      <c r="E239" s="4">
+        <v>0</v>
       </c>
       <c r="F239" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G239" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1428, 348, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1428, 346, 595, 3, 0, 7);</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A240" s="4">
+      <c r="A240" s="3">
         <f t="shared" si="36"/>
         <v>1429</v>
       </c>
-      <c r="B240" s="4">
-        <f>B238</f>
-        <v>348</v>
-      </c>
-      <c r="C240" s="4">
-        <v>76</v>
-      </c>
-      <c r="D240" s="4" t="s">
+      <c r="B240" s="3">
+        <f>B230+1</f>
+        <v>347</v>
+      </c>
+      <c r="C240" s="3">
+        <v>55</v>
+      </c>
+      <c r="D240" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E240" s="4" t="s">
+      <c r="E240" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F240" s="4">
-        <v>2</v>
-      </c>
-      <c r="G240" s="4" t="str">
+      <c r="F240" s="3">
+        <v>2</v>
+      </c>
+      <c r="G240" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1429, 348, 76, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1429, 347, 55, null, null, 2);</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A241" s="4">
+      <c r="A241" s="3">
         <f t="shared" si="36"/>
         <v>1430</v>
       </c>
-      <c r="B241" s="4">
-        <f t="shared" ref="B241" si="43">B238</f>
-        <v>348</v>
-      </c>
-      <c r="C241" s="4">
-        <v>76</v>
-      </c>
-      <c r="D241" s="4" t="s">
+      <c r="B241" s="3">
+        <f>B240</f>
+        <v>347</v>
+      </c>
+      <c r="C241" s="3">
+        <v>55</v>
+      </c>
+      <c r="D241" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E241" s="4" t="s">
+      <c r="E241" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F241" s="4">
-        <v>1</v>
-      </c>
-      <c r="G241" s="4" t="str">
+      <c r="F241" s="3">
+        <v>1</v>
+      </c>
+      <c r="G241" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1430, 348, 76, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1430, 347, 55, null, null, 1);</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -50699,11 +50699,11 @@
         <v>1431</v>
       </c>
       <c r="B242" s="3">
-        <f>B238+1</f>
-        <v>349</v>
+        <f>B240</f>
+        <v>347</v>
       </c>
       <c r="C242" s="3">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="D242" s="3" t="s">
         <v>18</v>
@@ -50716,7 +50716,7 @@
       </c>
       <c r="G242" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1431, 349, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1431, 347, 98, null, null, 2);</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -50725,11 +50725,11 @@
         <v>1432</v>
       </c>
       <c r="B243" s="3">
-        <f>B242</f>
-        <v>349</v>
+        <f t="shared" ref="B243" si="42">B240</f>
+        <v>347</v>
       </c>
       <c r="C243" s="3">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="D243" s="3" t="s">
         <v>18</v>
@@ -50742,59 +50742,59 @@
       </c>
       <c r="G243" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1432, 349, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1432, 347, 98, null, null, 1);</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="3">
+      <c r="A244" s="4">
         <f t="shared" si="36"/>
         <v>1433</v>
       </c>
-      <c r="B244" s="3">
-        <f>B242</f>
-        <v>349</v>
-      </c>
-      <c r="C244" s="3">
-        <v>380</v>
-      </c>
-      <c r="D244" s="3" t="s">
+      <c r="B244" s="4">
+        <f>B240+1</f>
+        <v>348</v>
+      </c>
+      <c r="C244" s="4">
+        <v>34</v>
+      </c>
+      <c r="D244" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E244" s="3" t="s">
+      <c r="E244" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F244" s="3">
-        <v>2</v>
-      </c>
-      <c r="G244" s="3" t="str">
+      <c r="F244" s="4">
+        <v>2</v>
+      </c>
+      <c r="G244" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1433, 349, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1433, 348, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A245" s="3">
+      <c r="A245" s="4">
         <f t="shared" si="36"/>
         <v>1434</v>
       </c>
-      <c r="B245" s="3">
-        <f t="shared" ref="B245" si="44">B242</f>
-        <v>349</v>
-      </c>
-      <c r="C245" s="3">
-        <v>380</v>
-      </c>
-      <c r="D245" s="3" t="s">
+      <c r="B245" s="4">
+        <f>B244</f>
+        <v>348</v>
+      </c>
+      <c r="C245" s="4">
+        <v>34</v>
+      </c>
+      <c r="D245" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E245" s="3" t="s">
+      <c r="E245" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F245" s="3">
-        <v>1</v>
-      </c>
-      <c r="G245" s="3" t="str">
+      <c r="F245" s="4">
+        <v>1</v>
+      </c>
+      <c r="G245" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1434, 349, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1434, 348, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -50803,11 +50803,11 @@
         <v>1435</v>
       </c>
       <c r="B246" s="4">
-        <f>B242+1</f>
-        <v>350</v>
+        <f>B244</f>
+        <v>348</v>
       </c>
       <c r="C246" s="4">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D246" s="4" t="s">
         <v>18</v>
@@ -50820,7 +50820,7 @@
       </c>
       <c r="G246" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1435, 350, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1435, 348, 76, null, null, 2);</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -50829,11 +50829,11 @@
         <v>1436</v>
       </c>
       <c r="B247" s="4">
-        <f>B246</f>
-        <v>350</v>
+        <f t="shared" ref="B247" si="43">B244</f>
+        <v>348</v>
       </c>
       <c r="C247" s="4">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D247" s="4" t="s">
         <v>18</v>
@@ -50846,59 +50846,59 @@
       </c>
       <c r="G247" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1436, 350, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1436, 348, 76, null, null, 1);</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A248" s="4">
+      <c r="A248" s="3">
         <f t="shared" si="36"/>
         <v>1437</v>
       </c>
-      <c r="B248" s="4">
-        <f>B246</f>
-        <v>350</v>
-      </c>
-      <c r="C248" s="4">
-        <v>20</v>
-      </c>
-      <c r="D248" s="4" t="s">
+      <c r="B248" s="3">
+        <f>B244+1</f>
+        <v>349</v>
+      </c>
+      <c r="C248" s="3">
+        <v>351</v>
+      </c>
+      <c r="D248" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E248" s="4" t="s">
+      <c r="E248" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F248" s="4">
-        <v>2</v>
-      </c>
-      <c r="G248" s="4" t="str">
+      <c r="F248" s="3">
+        <v>2</v>
+      </c>
+      <c r="G248" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1437, 350, 20, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1437, 349, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249" s="4">
+      <c r="A249" s="3">
         <f t="shared" si="36"/>
         <v>1438</v>
       </c>
-      <c r="B249" s="4">
-        <f t="shared" ref="B249" si="45">B246</f>
-        <v>350</v>
-      </c>
-      <c r="C249" s="4">
-        <v>20</v>
-      </c>
-      <c r="D249" s="4" t="s">
+      <c r="B249" s="3">
+        <f>B248</f>
+        <v>349</v>
+      </c>
+      <c r="C249" s="3">
+        <v>351</v>
+      </c>
+      <c r="D249" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E249" s="4" t="s">
+      <c r="E249" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F249" s="4">
-        <v>1</v>
-      </c>
-      <c r="G249" s="4" t="str">
+      <c r="F249" s="3">
+        <v>1</v>
+      </c>
+      <c r="G249" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1438, 350, 20, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1438, 349, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -50907,11 +50907,11 @@
         <v>1439</v>
       </c>
       <c r="B250" s="3">
-        <f>B246+1</f>
-        <v>351</v>
+        <f>B248</f>
+        <v>349</v>
       </c>
       <c r="C250" s="3">
-        <v>66</v>
+        <v>506</v>
       </c>
       <c r="D250" s="3" t="s">
         <v>18</v>
@@ -50924,7 +50924,7 @@
       </c>
       <c r="G250" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1439, 351, 66, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1439, 349, 506, null, null, 2);</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -50933,11 +50933,11 @@
         <v>1440</v>
       </c>
       <c r="B251" s="3">
-        <f>B250</f>
-        <v>351</v>
+        <f t="shared" ref="B251" si="44">B248</f>
+        <v>349</v>
       </c>
       <c r="C251" s="3">
-        <v>66</v>
+        <v>506</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>18</v>
@@ -50950,59 +50950,59 @@
       </c>
       <c r="G251" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1440, 351, 66, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1440, 349, 506, null, null, 1);</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A252" s="3">
+      <c r="A252" s="4">
         <f t="shared" si="36"/>
         <v>1441</v>
       </c>
-      <c r="B252" s="3">
-        <f>B250</f>
-        <v>351</v>
-      </c>
-      <c r="C252" s="3">
-        <v>994</v>
-      </c>
-      <c r="D252" s="3" t="s">
+      <c r="B252" s="4">
+        <f>B248+1</f>
+        <v>350</v>
+      </c>
+      <c r="C252" s="4">
+        <v>54</v>
+      </c>
+      <c r="D252" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E252" s="3" t="s">
+      <c r="E252" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F252" s="3">
-        <v>2</v>
-      </c>
-      <c r="G252" s="3" t="str">
+      <c r="F252" s="4">
+        <v>2</v>
+      </c>
+      <c r="G252" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1441, 351, 994, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1441, 350, 54, null, null, 2);</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="3">
+      <c r="A253" s="4">
         <f t="shared" si="36"/>
         <v>1442</v>
       </c>
-      <c r="B253" s="3">
-        <f t="shared" ref="B253" si="46">B250</f>
-        <v>351</v>
-      </c>
-      <c r="C253" s="3">
-        <v>994</v>
-      </c>
-      <c r="D253" s="3" t="s">
+      <c r="B253" s="4">
+        <f>B252</f>
+        <v>350</v>
+      </c>
+      <c r="C253" s="4">
+        <v>54</v>
+      </c>
+      <c r="D253" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E253" s="3" t="s">
+      <c r="E253" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F253" s="3">
-        <v>1</v>
-      </c>
-      <c r="G253" s="3" t="str">
+      <c r="F253" s="4">
+        <v>1</v>
+      </c>
+      <c r="G253" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1442, 351, 994, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1442, 350, 54, null, null, 1);</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -51011,11 +51011,11 @@
         <v>1443</v>
       </c>
       <c r="B254" s="4">
-        <f>B250+1</f>
-        <v>352</v>
+        <f>B252</f>
+        <v>350</v>
       </c>
       <c r="C254" s="4">
-        <v>351</v>
+        <v>380</v>
       </c>
       <c r="D254" s="4" t="s">
         <v>18</v>
@@ -51028,7 +51028,7 @@
       </c>
       <c r="G254" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1443, 352, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1443, 350, 380, null, null, 2);</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -51037,11 +51037,11 @@
         <v>1444</v>
       </c>
       <c r="B255" s="4">
-        <f>B254</f>
-        <v>352</v>
+        <f t="shared" ref="B255" si="45">B252</f>
+        <v>350</v>
       </c>
       <c r="C255" s="4">
-        <v>351</v>
+        <v>380</v>
       </c>
       <c r="D255" s="4" t="s">
         <v>18</v>
@@ -51054,59 +51054,59 @@
       </c>
       <c r="G255" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1444, 352, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1444, 350, 380, null, null, 1);</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A256" s="4">
+      <c r="A256" s="3">
         <f t="shared" si="36"/>
         <v>1445</v>
       </c>
-      <c r="B256" s="4">
-        <f>B254</f>
-        <v>352</v>
-      </c>
-      <c r="C256" s="4">
-        <v>506</v>
-      </c>
-      <c r="D256" s="4" t="s">
+      <c r="B256" s="3">
+        <f>B252+1</f>
+        <v>351</v>
+      </c>
+      <c r="C256" s="3">
+        <v>66</v>
+      </c>
+      <c r="D256" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E256" s="4" t="s">
+      <c r="E256" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F256" s="4">
-        <v>2</v>
-      </c>
-      <c r="G256" s="4" t="str">
+      <c r="F256" s="3">
+        <v>2</v>
+      </c>
+      <c r="G256" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1445, 352, 506, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1445, 351, 66, null, null, 2);</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A257" s="4">
+      <c r="A257" s="3">
         <f t="shared" si="36"/>
         <v>1446</v>
       </c>
-      <c r="B257" s="4">
-        <f t="shared" ref="B257" si="47">B254</f>
-        <v>352</v>
-      </c>
-      <c r="C257" s="4">
-        <v>506</v>
-      </c>
-      <c r="D257" s="4" t="s">
+      <c r="B257" s="3">
+        <f>B256</f>
+        <v>351</v>
+      </c>
+      <c r="C257" s="3">
+        <v>66</v>
+      </c>
+      <c r="D257" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E257" s="4" t="s">
+      <c r="E257" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F257" s="4">
-        <v>1</v>
-      </c>
-      <c r="G257" s="4" t="str">
+      <c r="F257" s="3">
+        <v>1</v>
+      </c>
+      <c r="G257" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1446, 352, 506, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1446, 351, 66, null, null, 1);</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -51115,11 +51115,11 @@
         <v>1447</v>
       </c>
       <c r="B258" s="3">
-        <f>B254+1</f>
-        <v>353</v>
-      </c>
-      <c r="C258" s="3" t="s">
-        <v>18</v>
+        <f>B256</f>
+        <v>351</v>
+      </c>
+      <c r="C258" s="3">
+        <v>994</v>
       </c>
       <c r="D258" s="3" t="s">
         <v>18</v>
@@ -51132,7 +51132,7 @@
       </c>
       <c r="G258" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1447, 353, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1447, 351, 994, null, null, 2);</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
@@ -51141,11 +51141,11 @@
         <v>1448</v>
       </c>
       <c r="B259" s="3">
-        <f>B258</f>
-        <v>353</v>
-      </c>
-      <c r="C259" s="3" t="s">
-        <v>18</v>
+        <f t="shared" ref="B259" si="46">B256</f>
+        <v>351</v>
+      </c>
+      <c r="C259" s="3">
+        <v>994</v>
       </c>
       <c r="D259" s="3" t="s">
         <v>18</v>
@@ -51158,59 +51158,59 @@
       </c>
       <c r="G259" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1448, 353, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1448, 351, 994, null, null, 1);</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A260" s="3">
+      <c r="A260" s="4">
         <f t="shared" si="36"/>
         <v>1449</v>
       </c>
-      <c r="B260" s="3">
-        <f>B258</f>
-        <v>353</v>
-      </c>
-      <c r="C260" s="3" t="s">
+      <c r="B260" s="4">
+        <f>B256+1</f>
+        <v>352</v>
+      </c>
+      <c r="C260" s="4">
+        <v>39</v>
+      </c>
+      <c r="D260" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D260" s="3" t="s">
+      <c r="E260" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E260" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F260" s="3">
-        <v>2</v>
-      </c>
-      <c r="G260" s="3" t="str">
+      <c r="F260" s="4">
+        <v>2</v>
+      </c>
+      <c r="G260" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1449, 353, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1449, 352, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A261" s="3">
+      <c r="A261" s="4">
         <f t="shared" si="36"/>
         <v>1450</v>
       </c>
-      <c r="B261" s="3">
-        <f t="shared" ref="B261" si="48">B258</f>
-        <v>353</v>
-      </c>
-      <c r="C261" s="3" t="s">
+      <c r="B261" s="4">
+        <f>B260</f>
+        <v>352</v>
+      </c>
+      <c r="C261" s="4">
+        <v>39</v>
+      </c>
+      <c r="D261" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D261" s="3" t="s">
+      <c r="E261" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E261" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F261" s="3">
-        <v>1</v>
-      </c>
-      <c r="G261" s="3" t="str">
+      <c r="F261" s="4">
+        <v>1</v>
+      </c>
+      <c r="G261" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1450, 353, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1450, 352, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -51219,11 +51219,11 @@
         <v>1451</v>
       </c>
       <c r="B262" s="4">
-        <f>B258+1</f>
-        <v>354</v>
-      </c>
-      <c r="C262" s="4" t="s">
-        <v>18</v>
+        <f>B260</f>
+        <v>352</v>
+      </c>
+      <c r="C262" s="4">
+        <v>20</v>
       </c>
       <c r="D262" s="4" t="s">
         <v>18</v>
@@ -51236,7 +51236,7 @@
       </c>
       <c r="G262" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1451, 354, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1451, 352, 20, null, null, 2);</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
@@ -51245,11 +51245,11 @@
         <v>1452</v>
       </c>
       <c r="B263" s="4">
-        <f>B262</f>
-        <v>354</v>
-      </c>
-      <c r="C263" s="4" t="s">
-        <v>18</v>
+        <f t="shared" ref="B263" si="47">B260</f>
+        <v>352</v>
+      </c>
+      <c r="C263" s="4">
+        <v>20</v>
       </c>
       <c r="D263" s="4" t="s">
         <v>18</v>
@@ -51262,59 +51262,59 @@
       </c>
       <c r="G263" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1452, 354, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1452, 352, 20, null, null, 1);</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A264" s="4">
+      <c r="A264" s="3">
         <f t="shared" si="36"/>
         <v>1453</v>
       </c>
-      <c r="B264" s="4">
-        <f>B262</f>
-        <v>354</v>
-      </c>
-      <c r="C264" s="4" t="s">
+      <c r="B264" s="3">
+        <f>B260+1</f>
+        <v>353</v>
+      </c>
+      <c r="C264" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D264" s="4" t="s">
+      <c r="D264" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E264" s="4" t="s">
+      <c r="E264" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F264" s="4">
-        <v>2</v>
-      </c>
-      <c r="G264" s="4" t="str">
+      <c r="F264" s="3">
+        <v>2</v>
+      </c>
+      <c r="G264" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1453, 354, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1453, 353, null, null, null, 2);</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A265" s="4">
+      <c r="A265" s="3">
         <f t="shared" si="36"/>
         <v>1454</v>
       </c>
-      <c r="B265" s="4">
-        <f t="shared" ref="B265" si="49">B262</f>
-        <v>354</v>
-      </c>
-      <c r="C265" s="4" t="s">
+      <c r="B265" s="3">
+        <f>B264</f>
+        <v>353</v>
+      </c>
+      <c r="C265" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D265" s="4" t="s">
+      <c r="D265" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E265" s="4" t="s">
+      <c r="E265" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F265" s="4">
-        <v>1</v>
-      </c>
-      <c r="G265" s="4" t="str">
+      <c r="F265" s="3">
+        <v>1</v>
+      </c>
+      <c r="G265" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1454, 354, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1454, 353, null, null, null, 1);</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -51323,8 +51323,8 @@
         <v>1455</v>
       </c>
       <c r="B266" s="3">
-        <f>B262+1</f>
-        <v>355</v>
+        <f>B264</f>
+        <v>353</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>18</v>
@@ -51340,7 +51340,7 @@
       </c>
       <c r="G266" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1455, 355, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1455, 353, null, null, null, 2);</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -51349,8 +51349,8 @@
         <v>1456</v>
       </c>
       <c r="B267" s="3">
-        <f>B266</f>
-        <v>355</v>
+        <f t="shared" ref="B267" si="48">B264</f>
+        <v>353</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>18</v>
@@ -51366,59 +51366,59 @@
       </c>
       <c r="G267" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1456, 355, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1456, 353, null, null, null, 1);</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A268" s="3">
+      <c r="A268" s="4">
         <f t="shared" si="36"/>
         <v>1457</v>
       </c>
-      <c r="B268" s="3">
-        <f>B266</f>
-        <v>355</v>
-      </c>
-      <c r="C268" s="3" t="s">
+      <c r="B268" s="4">
+        <f>B264+1</f>
+        <v>354</v>
+      </c>
+      <c r="C268" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D268" s="3" t="s">
+      <c r="D268" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E268" s="3" t="s">
+      <c r="E268" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F268" s="3">
-        <v>2</v>
-      </c>
-      <c r="G268" s="3" t="str">
+      <c r="F268" s="4">
+        <v>2</v>
+      </c>
+      <c r="G268" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1457, 355, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1457, 354, null, null, null, 2);</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="3">
+      <c r="A269" s="4">
         <f t="shared" si="36"/>
         <v>1458</v>
       </c>
-      <c r="B269" s="3">
-        <f t="shared" ref="B269" si="50">B266</f>
-        <v>355</v>
-      </c>
-      <c r="C269" s="3" t="s">
+      <c r="B269" s="4">
+        <f>B268</f>
+        <v>354</v>
+      </c>
+      <c r="C269" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D269" s="3" t="s">
+      <c r="D269" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E269" s="3" t="s">
+      <c r="E269" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F269" s="3">
-        <v>1</v>
-      </c>
-      <c r="G269" s="3" t="str">
+      <c r="F269" s="4">
+        <v>1</v>
+      </c>
+      <c r="G269" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1458, 355, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1458, 354, null, null, null, 1);</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
@@ -51427,8 +51427,8 @@
         <v>1459</v>
       </c>
       <c r="B270" s="4">
-        <f>B266+1</f>
-        <v>356</v>
+        <f>B268</f>
+        <v>354</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>18</v>
@@ -51444,7 +51444,7 @@
       </c>
       <c r="G270" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1459, 356, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1459, 354, null, null, null, 2);</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
@@ -51453,8 +51453,8 @@
         <v>1460</v>
       </c>
       <c r="B271" s="4">
-        <f>B270</f>
-        <v>356</v>
+        <f t="shared" ref="B271" si="49">B268</f>
+        <v>354</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>18</v>
@@ -51470,59 +51470,59 @@
       </c>
       <c r="G271" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1460, 356, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1460, 354, null, null, null, 1);</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A272" s="4">
+      <c r="A272" s="3">
         <f t="shared" si="36"/>
         <v>1461</v>
       </c>
-      <c r="B272" s="4">
-        <f>B270</f>
-        <v>356</v>
-      </c>
-      <c r="C272" s="4" t="s">
+      <c r="B272" s="3">
+        <f>B268+1</f>
+        <v>355</v>
+      </c>
+      <c r="C272" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D272" s="4" t="s">
+      <c r="D272" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E272" s="4" t="s">
+      <c r="E272" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F272" s="4">
-        <v>2</v>
-      </c>
-      <c r="G272" s="4" t="str">
+      <c r="F272" s="3">
+        <v>2</v>
+      </c>
+      <c r="G272" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1461, 356, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1461, 355, null, null, null, 2);</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A273" s="4">
+      <c r="A273" s="3">
         <f t="shared" si="36"/>
         <v>1462</v>
       </c>
-      <c r="B273" s="4">
-        <f t="shared" ref="B273" si="51">B270</f>
-        <v>356</v>
-      </c>
-      <c r="C273" s="4" t="s">
+      <c r="B273" s="3">
+        <f>B272</f>
+        <v>355</v>
+      </c>
+      <c r="C273" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D273" s="4" t="s">
+      <c r="D273" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E273" s="4" t="s">
+      <c r="E273" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F273" s="4">
-        <v>1</v>
-      </c>
-      <c r="G273" s="4" t="str">
+      <c r="F273" s="3">
+        <v>1</v>
+      </c>
+      <c r="G273" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1462, 356, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1462, 355, null, null, null, 1);</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
@@ -51531,8 +51531,8 @@
         <v>1463</v>
       </c>
       <c r="B274" s="3">
-        <f>B270+1</f>
-        <v>357</v>
+        <f>B272</f>
+        <v>355</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>18</v>
@@ -51547,8 +51547,8 @@
         <v>2</v>
       </c>
       <c r="G274" s="3" t="str">
-        <f t="shared" ref="G274:G289" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A274 &amp; ", " &amp; B274 &amp; ", " &amp; C274 &amp; ", " &amp; D274 &amp; ", " &amp; E274 &amp; ", " &amp; F274 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1463, 357, null, null, null, 2);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1463, 355, null, null, null, 2);</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
@@ -51557,8 +51557,8 @@
         <v>1464</v>
       </c>
       <c r="B275" s="3">
-        <f>B274</f>
-        <v>357</v>
+        <f t="shared" ref="B275" si="50">B272</f>
+        <v>355</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>18</v>
@@ -51573,70 +51573,70 @@
         <v>1</v>
       </c>
       <c r="G275" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1464, 357, null, null, null, 1);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1464, 355, null, null, null, 1);</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A276" s="3">
+      <c r="A276" s="4">
         <f t="shared" si="36"/>
         <v>1465</v>
       </c>
-      <c r="B276" s="3">
-        <f>B274</f>
-        <v>357</v>
-      </c>
-      <c r="C276" s="3" t="s">
+      <c r="B276" s="4">
+        <f>B272+1</f>
+        <v>356</v>
+      </c>
+      <c r="C276" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D276" s="3" t="s">
+      <c r="D276" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E276" s="3" t="s">
+      <c r="E276" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F276" s="3">
-        <v>2</v>
-      </c>
-      <c r="G276" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1465, 357, null, null, null, 2);</v>
+      <c r="F276" s="4">
+        <v>2</v>
+      </c>
+      <c r="G276" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1465, 356, null, null, null, 2);</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277" s="3">
+      <c r="A277" s="4">
         <f t="shared" si="36"/>
         <v>1466</v>
       </c>
-      <c r="B277" s="3">
-        <f t="shared" ref="B277" si="53">B274</f>
-        <v>357</v>
-      </c>
-      <c r="C277" s="3" t="s">
+      <c r="B277" s="4">
+        <f>B276</f>
+        <v>356</v>
+      </c>
+      <c r="C277" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D277" s="3" t="s">
+      <c r="D277" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E277" s="3" t="s">
+      <c r="E277" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F277" s="3">
-        <v>1</v>
-      </c>
-      <c r="G277" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1466, 357, null, null, null, 1);</v>
+      <c r="F277" s="4">
+        <v>1</v>
+      </c>
+      <c r="G277" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1466, 356, null, null, null, 1);</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
-        <f t="shared" ref="A278:A289" si="54">A277+1</f>
+        <f t="shared" si="36"/>
         <v>1467</v>
       </c>
       <c r="B278" s="4">
-        <f>B274+1</f>
-        <v>358</v>
+        <f>B276</f>
+        <v>356</v>
       </c>
       <c r="C278" s="4" t="s">
         <v>18</v>
@@ -51651,18 +51651,18 @@
         <v>2</v>
       </c>
       <c r="G278" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1467, 358, null, null, null, 2);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1467, 356, null, null, null, 2);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1468</v>
       </c>
       <c r="B279" s="4">
-        <f>B278</f>
-        <v>358</v>
+        <f t="shared" ref="B279" si="51">B276</f>
+        <v>356</v>
       </c>
       <c r="C279" s="4" t="s">
         <v>18</v>
@@ -51677,70 +51677,70 @@
         <v>1</v>
       </c>
       <c r="G279" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1468, 356, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="3">
+        <f t="shared" si="36"/>
+        <v>1469</v>
+      </c>
+      <c r="B280" s="3">
+        <f>B276+1</f>
+        <v>357</v>
+      </c>
+      <c r="C280" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D280" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E280" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F280" s="3">
+        <v>2</v>
+      </c>
+      <c r="G280" s="3" t="str">
+        <f t="shared" ref="G280:G295" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A280 &amp; ", " &amp; B280 &amp; ", " &amp; C280 &amp; ", " &amp; D280 &amp; ", " &amp; E280 &amp; ", " &amp; F280 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1469, 357, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="3">
+        <f t="shared" si="36"/>
+        <v>1470</v>
+      </c>
+      <c r="B281" s="3">
+        <f>B280</f>
+        <v>357</v>
+      </c>
+      <c r="C281" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D281" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E281" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F281" s="3">
+        <v>1</v>
+      </c>
+      <c r="G281" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1468, 358, null, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A280" s="4">
-        <f t="shared" si="54"/>
-        <v>1469</v>
-      </c>
-      <c r="B280" s="4">
-        <f>B278</f>
-        <v>358</v>
-      </c>
-      <c r="C280" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D280" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E280" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F280" s="4">
-        <v>2</v>
-      </c>
-      <c r="G280" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1469, 358, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A281" s="4">
-        <f t="shared" si="54"/>
-        <v>1470</v>
-      </c>
-      <c r="B281" s="4">
-        <f t="shared" ref="B281" si="55">B278</f>
-        <v>358</v>
-      </c>
-      <c r="C281" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D281" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E281" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F281" s="4">
-        <v>1</v>
-      </c>
-      <c r="G281" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1470, 358, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1470, 357, null, null, null, 1);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1471</v>
       </c>
       <c r="B282" s="3">
-        <f>B278+1</f>
-        <v>359</v>
+        <f>B280</f>
+        <v>357</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>18</v>
@@ -51756,17 +51756,17 @@
       </c>
       <c r="G282" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1471, 359, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1471, 357, null, null, null, 2);</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1472</v>
       </c>
       <c r="B283" s="3">
-        <f>B282</f>
-        <v>359</v>
+        <f t="shared" ref="B283" si="53">B280</f>
+        <v>357</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>18</v>
@@ -51782,59 +51782,59 @@
       </c>
       <c r="G283" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1472, 359, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1472, 357, null, null, null, 1);</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A284" s="3">
-        <f t="shared" si="54"/>
+      <c r="A284" s="4">
+        <f t="shared" ref="A284:A295" si="54">A283+1</f>
         <v>1473</v>
       </c>
-      <c r="B284" s="3">
-        <f>B282</f>
-        <v>359</v>
-      </c>
-      <c r="C284" s="3" t="s">
+      <c r="B284" s="4">
+        <f>B280+1</f>
+        <v>358</v>
+      </c>
+      <c r="C284" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D284" s="3" t="s">
+      <c r="D284" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E284" s="3" t="s">
+      <c r="E284" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F284" s="3">
-        <v>2</v>
-      </c>
-      <c r="G284" s="3" t="str">
+      <c r="F284" s="4">
+        <v>2</v>
+      </c>
+      <c r="G284" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1473, 359, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1473, 358, null, null, null, 2);</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" s="3">
+      <c r="A285" s="4">
         <f t="shared" si="54"/>
         <v>1474</v>
       </c>
-      <c r="B285" s="3">
-        <f t="shared" ref="B285" si="56">B282</f>
-        <v>359</v>
-      </c>
-      <c r="C285" s="3" t="s">
+      <c r="B285" s="4">
+        <f>B284</f>
+        <v>358</v>
+      </c>
+      <c r="C285" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D285" s="3" t="s">
+      <c r="D285" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E285" s="3" t="s">
+      <c r="E285" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F285" s="3">
-        <v>1</v>
-      </c>
-      <c r="G285" s="3" t="str">
+      <c r="F285" s="4">
+        <v>1</v>
+      </c>
+      <c r="G285" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1474, 359, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1474, 358, null, null, null, 1);</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
@@ -51843,8 +51843,8 @@
         <v>1475</v>
       </c>
       <c r="B286" s="4">
-        <f>B282+1</f>
-        <v>360</v>
+        <f>B284</f>
+        <v>358</v>
       </c>
       <c r="C286" s="4" t="s">
         <v>18</v>
@@ -51860,7 +51860,7 @@
       </c>
       <c r="G286" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1475, 360, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1475, 358, null, null, null, 2);</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
@@ -51869,8 +51869,8 @@
         <v>1476</v>
       </c>
       <c r="B287" s="4">
-        <f>B286</f>
-        <v>360</v>
+        <f t="shared" ref="B287" si="55">B284</f>
+        <v>358</v>
       </c>
       <c r="C287" s="4" t="s">
         <v>18</v>
@@ -51886,59 +51886,215 @@
       </c>
       <c r="G287" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1476, 360, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1476, 358, null, null, null, 1);</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A288" s="4">
+      <c r="A288" s="3">
         <f t="shared" si="54"/>
         <v>1477</v>
       </c>
-      <c r="B288" s="4">
-        <f>B286</f>
-        <v>360</v>
-      </c>
-      <c r="C288" s="4" t="s">
+      <c r="B288" s="3">
+        <f>B284+1</f>
+        <v>359</v>
+      </c>
+      <c r="C288" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D288" s="4" t="s">
+      <c r="D288" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E288" s="4" t="s">
+      <c r="E288" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F288" s="4">
-        <v>2</v>
-      </c>
-      <c r="G288" s="4" t="str">
+      <c r="F288" s="3">
+        <v>2</v>
+      </c>
+      <c r="G288" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1477, 360, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1477, 359, null, null, null, 2);</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A289" s="4">
+      <c r="A289" s="3">
         <f t="shared" si="54"/>
         <v>1478</v>
       </c>
-      <c r="B289" s="4">
-        <f t="shared" ref="B289" si="57">B286</f>
+      <c r="B289" s="3">
+        <f>B288</f>
+        <v>359</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F289" s="3">
+        <v>1</v>
+      </c>
+      <c r="G289" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1478, 359, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="3">
+        <f t="shared" si="54"/>
+        <v>1479</v>
+      </c>
+      <c r="B290" s="3">
+        <f>B288</f>
+        <v>359</v>
+      </c>
+      <c r="C290" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E290" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F290" s="3">
+        <v>2</v>
+      </c>
+      <c r="G290" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1479, 359, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="3">
+        <f t="shared" si="54"/>
+        <v>1480</v>
+      </c>
+      <c r="B291" s="3">
+        <f t="shared" ref="B291" si="56">B288</f>
+        <v>359</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D291" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E291" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F291" s="3">
+        <v>1</v>
+      </c>
+      <c r="G291" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1480, 359, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="4">
+        <f t="shared" si="54"/>
+        <v>1481</v>
+      </c>
+      <c r="B292" s="4">
+        <f>B288+1</f>
         <v>360</v>
       </c>
-      <c r="C289" s="4" t="s">
+      <c r="C292" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D289" s="4" t="s">
+      <c r="D292" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E289" s="4" t="s">
+      <c r="E292" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F289" s="4">
-        <v>1</v>
-      </c>
-      <c r="G289" s="4" t="str">
+      <c r="F292" s="4">
+        <v>2</v>
+      </c>
+      <c r="G292" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1478, 360, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1481, 360, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="4">
+        <f t="shared" si="54"/>
+        <v>1482</v>
+      </c>
+      <c r="B293" s="4">
+        <f>B292</f>
+        <v>360</v>
+      </c>
+      <c r="C293" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D293" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E293" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F293" s="4">
+        <v>1</v>
+      </c>
+      <c r="G293" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1482, 360, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="4">
+        <f t="shared" si="54"/>
+        <v>1483</v>
+      </c>
+      <c r="B294" s="4">
+        <f>B292</f>
+        <v>360</v>
+      </c>
+      <c r="C294" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D294" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E294" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F294" s="4">
+        <v>2</v>
+      </c>
+      <c r="G294" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1483, 360, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="4">
+        <f t="shared" si="54"/>
+        <v>1484</v>
+      </c>
+      <c r="B295" s="4">
+        <f t="shared" ref="B295" si="57">B292</f>
+        <v>360</v>
+      </c>
+      <c r="C295" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D295" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E295" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F295" s="4">
+        <v>1</v>
+      </c>
+      <c r="G295" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1484, 360, null, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Futsal WorldCup Round of 16 Date 2 and 3
Futsal WorldCup Round of 16 Date 2 and 3
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -44729,7 +44729,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G295"/>
+  <dimension ref="A1:G309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -49883,7 +49883,7 @@
         <v>2</v>
       </c>
       <c r="G210" s="3" t="str">
-        <f t="shared" ref="G210:G279" si="34">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A210 &amp; ", " &amp; B210 &amp; ", " &amp; C210 &amp; ", " &amp; D210 &amp; ", " &amp; E210 &amp; ", " &amp; F210 &amp; ");"</f>
+        <f t="shared" ref="G210:G293" si="34">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A210 &amp; ", " &amp; B210 &amp; ", " &amp; C210 &amp; ", " &amp; D210 &amp; ", " &amp; E210 &amp; ", " &amp; F210 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1399, 341, 994, 2, 0, 2);</v>
       </c>
     </row>
@@ -49967,7 +49967,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
-        <f t="shared" ref="A214:A283" si="36">A213+1</f>
+        <f t="shared" ref="A214:A297" si="36">A213+1</f>
         <v>1403</v>
       </c>
       <c r="B214" s="4">
@@ -50653,18 +50653,18 @@
       <c r="C240" s="3">
         <v>55</v>
       </c>
-      <c r="D240" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E240" s="3" t="s">
-        <v>18</v>
+      <c r="D240" s="3">
+        <v>3</v>
+      </c>
+      <c r="E240" s="3">
+        <v>0</v>
       </c>
       <c r="F240" s="3">
         <v>2</v>
       </c>
       <c r="G240" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1429, 347, 55, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1429, 347, 55, 3, 0, 2);</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -50679,18 +50679,18 @@
       <c r="C241" s="3">
         <v>55</v>
       </c>
-      <c r="D241" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E241" s="3" t="s">
-        <v>18</v>
+      <c r="D241" s="3">
+        <v>2</v>
+      </c>
+      <c r="E241" s="3">
+        <v>0</v>
       </c>
       <c r="F241" s="3">
         <v>1</v>
       </c>
       <c r="G241" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1430, 347, 55, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1430, 347, 55, 2, 0, 1);</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -50705,18 +50705,18 @@
       <c r="C242" s="3">
         <v>98</v>
       </c>
-      <c r="D242" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>18</v>
+      <c r="D242" s="3">
+        <v>3</v>
+      </c>
+      <c r="E242" s="3">
+        <v>0</v>
       </c>
       <c r="F242" s="3">
         <v>2</v>
       </c>
       <c r="G242" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1431, 347, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1431, 347, 98, 3, 0, 2);</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -50725,128 +50725,128 @@
         <v>1432</v>
       </c>
       <c r="B243" s="3">
-        <f t="shared" ref="B243" si="42">B240</f>
+        <f t="shared" ref="B243:B249" si="42">B240</f>
         <v>347</v>
       </c>
       <c r="C243" s="3">
         <v>98</v>
       </c>
-      <c r="D243" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E243" s="3" t="s">
-        <v>18</v>
+      <c r="D243" s="3">
+        <v>1</v>
+      </c>
+      <c r="E243" s="3">
+        <v>0</v>
       </c>
       <c r="F243" s="3">
         <v>1</v>
       </c>
       <c r="G243" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1432, 347, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1432, 347, 98, 1, 0, 1);</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="4">
+      <c r="A244" s="3">
         <f t="shared" si="36"/>
         <v>1433</v>
       </c>
-      <c r="B244" s="4">
-        <f>B240+1</f>
-        <v>348</v>
-      </c>
-      <c r="C244" s="4">
-        <v>34</v>
-      </c>
-      <c r="D244" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E244" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F244" s="4">
-        <v>2</v>
-      </c>
-      <c r="G244" s="4" t="str">
+      <c r="B244" s="3">
+        <f t="shared" si="42"/>
+        <v>347</v>
+      </c>
+      <c r="C244" s="3">
+        <v>55</v>
+      </c>
+      <c r="D244" s="3">
+        <v>4</v>
+      </c>
+      <c r="E244" s="3">
+        <v>1</v>
+      </c>
+      <c r="F244" s="3">
+        <v>4</v>
+      </c>
+      <c r="G244" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1433, 348, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1433, 347, 55, 4, 1, 4);</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A245" s="4">
+      <c r="A245" s="3">
         <f t="shared" si="36"/>
         <v>1434</v>
       </c>
-      <c r="B245" s="4">
-        <f>B244</f>
-        <v>348</v>
-      </c>
-      <c r="C245" s="4">
-        <v>34</v>
-      </c>
-      <c r="D245" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E245" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F245" s="4">
-        <v>1</v>
-      </c>
-      <c r="G245" s="4" t="str">
+      <c r="B245" s="3">
+        <f t="shared" si="42"/>
+        <v>347</v>
+      </c>
+      <c r="C245" s="3">
+        <v>55</v>
+      </c>
+      <c r="D245" s="3">
+        <v>3</v>
+      </c>
+      <c r="E245" s="3">
+        <v>0</v>
+      </c>
+      <c r="F245" s="3">
+        <v>3</v>
+      </c>
+      <c r="G245" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1434, 348, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1434, 347, 55, 3, 0, 3);</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A246" s="4">
+      <c r="A246" s="3">
         <f t="shared" si="36"/>
         <v>1435</v>
       </c>
-      <c r="B246" s="4">
-        <f>B244</f>
-        <v>348</v>
-      </c>
-      <c r="C246" s="4">
-        <v>76</v>
-      </c>
-      <c r="D246" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E246" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F246" s="4">
-        <v>2</v>
-      </c>
-      <c r="G246" s="4" t="str">
+      <c r="B246" s="3">
+        <f t="shared" si="42"/>
+        <v>347</v>
+      </c>
+      <c r="C246" s="3">
+        <v>98</v>
+      </c>
+      <c r="D246" s="3">
+        <v>4</v>
+      </c>
+      <c r="E246" s="3">
+        <v>1</v>
+      </c>
+      <c r="F246" s="3">
+        <v>4</v>
+      </c>
+      <c r="G246" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1435, 348, 76, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1435, 347, 98, 4, 1, 4);</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A247" s="4">
+      <c r="A247" s="3">
         <f t="shared" si="36"/>
         <v>1436</v>
       </c>
-      <c r="B247" s="4">
-        <f t="shared" ref="B247" si="43">B244</f>
-        <v>348</v>
-      </c>
-      <c r="C247" s="4">
-        <v>76</v>
-      </c>
-      <c r="D247" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E247" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F247" s="4">
-        <v>1</v>
-      </c>
-      <c r="G247" s="4" t="str">
+      <c r="B247" s="3">
+        <f t="shared" si="42"/>
+        <v>347</v>
+      </c>
+      <c r="C247" s="3">
+        <v>98</v>
+      </c>
+      <c r="D247" s="3">
+        <v>3</v>
+      </c>
+      <c r="E247" s="3">
+        <v>0</v>
+      </c>
+      <c r="F247" s="3">
+        <v>3</v>
+      </c>
+      <c r="G247" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1436, 348, 76, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1436, 347, 98, 3, 0, 3);</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -50855,24 +50855,24 @@
         <v>1437</v>
       </c>
       <c r="B248" s="3">
-        <f>B244+1</f>
-        <v>349</v>
+        <f t="shared" si="42"/>
+        <v>347</v>
       </c>
       <c r="C248" s="3">
-        <v>351</v>
-      </c>
-      <c r="D248" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E248" s="3" t="s">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="D248" s="3">
+        <v>2</v>
+      </c>
+      <c r="E248" s="3">
+        <v>0</v>
       </c>
       <c r="F248" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G248" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1437, 349, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1437, 347, 55, 2, 0, 7);</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -50881,76 +50881,76 @@
         <v>1438</v>
       </c>
       <c r="B249" s="3">
-        <f>B248</f>
-        <v>349</v>
+        <f t="shared" si="42"/>
+        <v>347</v>
       </c>
       <c r="C249" s="3">
-        <v>351</v>
-      </c>
-      <c r="D249" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E249" s="3" t="s">
-        <v>18</v>
+        <v>98</v>
+      </c>
+      <c r="D249" s="3">
+        <v>3</v>
+      </c>
+      <c r="E249" s="3">
+        <v>0</v>
       </c>
       <c r="F249" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G249" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1438, 349, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1438, 347, 98, 3, 0, 7);</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A250" s="3">
+      <c r="A250" s="4">
         <f t="shared" si="36"/>
         <v>1439</v>
       </c>
-      <c r="B250" s="3">
-        <f>B248</f>
-        <v>349</v>
-      </c>
-      <c r="C250" s="3">
-        <v>506</v>
-      </c>
-      <c r="D250" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E250" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F250" s="3">
-        <v>2</v>
-      </c>
-      <c r="G250" s="3" t="str">
+      <c r="B250" s="4">
+        <f>B240+1</f>
+        <v>348</v>
+      </c>
+      <c r="C250" s="4">
+        <v>34</v>
+      </c>
+      <c r="D250" s="4">
+        <v>5</v>
+      </c>
+      <c r="E250" s="4">
+        <v>3</v>
+      </c>
+      <c r="F250" s="4">
+        <v>2</v>
+      </c>
+      <c r="G250" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1439, 349, 506, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1439, 348, 34, 5, 3, 2);</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A251" s="3">
+      <c r="A251" s="4">
         <f t="shared" si="36"/>
         <v>1440</v>
       </c>
-      <c r="B251" s="3">
-        <f t="shared" ref="B251" si="44">B248</f>
-        <v>349</v>
-      </c>
-      <c r="C251" s="3">
-        <v>506</v>
-      </c>
-      <c r="D251" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E251" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F251" s="3">
-        <v>1</v>
-      </c>
-      <c r="G251" s="3" t="str">
+      <c r="B251" s="4">
+        <f>B250</f>
+        <v>348</v>
+      </c>
+      <c r="C251" s="4">
+        <v>34</v>
+      </c>
+      <c r="D251" s="4">
+        <v>1</v>
+      </c>
+      <c r="E251" s="4">
+        <v>0</v>
+      </c>
+      <c r="F251" s="4">
+        <v>1</v>
+      </c>
+      <c r="G251" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1440, 349, 506, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1440, 348, 34, 1, 0, 1);</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -50959,24 +50959,24 @@
         <v>1441</v>
       </c>
       <c r="B252" s="4">
-        <f>B248+1</f>
-        <v>350</v>
+        <f>B250</f>
+        <v>348</v>
       </c>
       <c r="C252" s="4">
-        <v>54</v>
-      </c>
-      <c r="D252" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E252" s="4" t="s">
-        <v>18</v>
+        <v>76</v>
+      </c>
+      <c r="D252" s="4">
+        <v>2</v>
+      </c>
+      <c r="E252" s="4">
+        <v>0</v>
       </c>
       <c r="F252" s="4">
         <v>2</v>
       </c>
       <c r="G252" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1441, 350, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1441, 348, 76, 2, 0, 2);</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -50985,76 +50985,76 @@
         <v>1442</v>
       </c>
       <c r="B253" s="4">
-        <f>B252</f>
-        <v>350</v>
+        <f t="shared" ref="B253" si="43">B250</f>
+        <v>348</v>
       </c>
       <c r="C253" s="4">
-        <v>54</v>
-      </c>
-      <c r="D253" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E253" s="4" t="s">
-        <v>18</v>
+        <v>76</v>
+      </c>
+      <c r="D253" s="4">
+        <v>1</v>
+      </c>
+      <c r="E253" s="4">
+        <v>0</v>
       </c>
       <c r="F253" s="4">
         <v>1</v>
       </c>
       <c r="G253" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1442, 350, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1442, 348, 76, 1, 0, 1);</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="4">
+      <c r="A254" s="3">
         <f t="shared" si="36"/>
         <v>1443</v>
       </c>
-      <c r="B254" s="4">
-        <f>B252</f>
-        <v>350</v>
-      </c>
-      <c r="C254" s="4">
-        <v>380</v>
-      </c>
-      <c r="D254" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E254" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F254" s="4">
-        <v>2</v>
-      </c>
-      <c r="G254" s="4" t="str">
+      <c r="B254" s="3">
+        <f>B250+1</f>
+        <v>349</v>
+      </c>
+      <c r="C254" s="3">
+        <v>351</v>
+      </c>
+      <c r="D254" s="3">
+        <v>4</v>
+      </c>
+      <c r="E254" s="3">
+        <v>3</v>
+      </c>
+      <c r="F254" s="3">
+        <v>2</v>
+      </c>
+      <c r="G254" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1443, 350, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1443, 349, 351, 4, 3, 2);</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A255" s="4">
+      <c r="A255" s="3">
         <f t="shared" si="36"/>
         <v>1444</v>
       </c>
-      <c r="B255" s="4">
-        <f t="shared" ref="B255" si="45">B252</f>
-        <v>350</v>
-      </c>
-      <c r="C255" s="4">
-        <v>380</v>
-      </c>
-      <c r="D255" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E255" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F255" s="4">
-        <v>1</v>
-      </c>
-      <c r="G255" s="4" t="str">
+      <c r="B255" s="3">
+        <f>B254</f>
+        <v>349</v>
+      </c>
+      <c r="C255" s="3">
+        <v>351</v>
+      </c>
+      <c r="D255" s="3">
+        <v>1</v>
+      </c>
+      <c r="E255" s="3">
+        <v>0</v>
+      </c>
+      <c r="F255" s="3">
+        <v>1</v>
+      </c>
+      <c r="G255" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1444, 350, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1444, 349, 351, 1, 0, 1);</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -51063,24 +51063,24 @@
         <v>1445</v>
       </c>
       <c r="B256" s="3">
-        <f>B252+1</f>
-        <v>351</v>
+        <f>B254</f>
+        <v>349</v>
       </c>
       <c r="C256" s="3">
-        <v>66</v>
-      </c>
-      <c r="D256" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E256" s="3" t="s">
-        <v>18</v>
+        <v>506</v>
+      </c>
+      <c r="D256" s="3">
+        <v>0</v>
+      </c>
+      <c r="E256" s="3">
+        <v>0</v>
       </c>
       <c r="F256" s="3">
         <v>2</v>
       </c>
       <c r="G256" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1445, 351, 66, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1445, 349, 506, 0, 0, 2);</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -51089,76 +51089,76 @@
         <v>1446</v>
       </c>
       <c r="B257" s="3">
-        <f>B256</f>
-        <v>351</v>
+        <f t="shared" ref="B257" si="44">B254</f>
+        <v>349</v>
       </c>
       <c r="C257" s="3">
-        <v>66</v>
-      </c>
-      <c r="D257" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E257" s="3" t="s">
-        <v>18</v>
+        <v>506</v>
+      </c>
+      <c r="D257" s="3">
+        <v>0</v>
+      </c>
+      <c r="E257" s="3">
+        <v>0</v>
       </c>
       <c r="F257" s="3">
         <v>1</v>
       </c>
       <c r="G257" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1446, 351, 66, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1446, 349, 506, 0, 0, 1);</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A258" s="3">
+      <c r="A258" s="4">
         <f t="shared" si="36"/>
         <v>1447</v>
       </c>
-      <c r="B258" s="3">
-        <f>B256</f>
-        <v>351</v>
-      </c>
-      <c r="C258" s="3">
-        <v>994</v>
-      </c>
-      <c r="D258" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E258" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F258" s="3">
-        <v>2</v>
-      </c>
-      <c r="G258" s="3" t="str">
+      <c r="B258" s="4">
+        <f>B254+1</f>
+        <v>350</v>
+      </c>
+      <c r="C258" s="4">
+        <v>54</v>
+      </c>
+      <c r="D258" s="4">
+        <v>1</v>
+      </c>
+      <c r="E258" s="4">
+        <v>3</v>
+      </c>
+      <c r="F258" s="4">
+        <v>2</v>
+      </c>
+      <c r="G258" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1447, 351, 994, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1447, 350, 54, 1, 3, 2);</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A259" s="3">
+      <c r="A259" s="4">
         <f t="shared" si="36"/>
         <v>1448</v>
       </c>
-      <c r="B259" s="3">
-        <f t="shared" ref="B259" si="46">B256</f>
-        <v>351</v>
-      </c>
-      <c r="C259" s="3">
-        <v>994</v>
-      </c>
-      <c r="D259" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E259" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F259" s="3">
-        <v>1</v>
-      </c>
-      <c r="G259" s="3" t="str">
+      <c r="B259" s="4">
+        <f>B258</f>
+        <v>350</v>
+      </c>
+      <c r="C259" s="4">
+        <v>54</v>
+      </c>
+      <c r="D259" s="4">
+        <v>0</v>
+      </c>
+      <c r="E259" s="4">
+        <v>0</v>
+      </c>
+      <c r="F259" s="4">
+        <v>1</v>
+      </c>
+      <c r="G259" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1448, 351, 994, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1448, 350, 54, 0, 0, 1);</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -51167,24 +51167,24 @@
         <v>1449</v>
       </c>
       <c r="B260" s="4">
-        <f>B256+1</f>
-        <v>352</v>
+        <f>B258</f>
+        <v>350</v>
       </c>
       <c r="C260" s="4">
-        <v>39</v>
-      </c>
-      <c r="D260" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E260" s="4" t="s">
-        <v>18</v>
+        <v>380</v>
+      </c>
+      <c r="D260" s="4">
+        <v>0</v>
+      </c>
+      <c r="E260" s="4">
+        <v>0</v>
       </c>
       <c r="F260" s="4">
         <v>2</v>
       </c>
       <c r="G260" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1449, 352, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1449, 350, 380, 0, 0, 2);</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -51193,76 +51193,76 @@
         <v>1450</v>
       </c>
       <c r="B261" s="4">
-        <f>B260</f>
-        <v>352</v>
+        <f t="shared" ref="B261" si="45">B258</f>
+        <v>350</v>
       </c>
       <c r="C261" s="4">
-        <v>39</v>
-      </c>
-      <c r="D261" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E261" s="4" t="s">
-        <v>18</v>
+        <v>380</v>
+      </c>
+      <c r="D261" s="4">
+        <v>0</v>
+      </c>
+      <c r="E261" s="4">
+        <v>0</v>
       </c>
       <c r="F261" s="4">
         <v>1</v>
       </c>
       <c r="G261" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1450, 352, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1450, 350, 380, 0, 0, 1);</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A262" s="4">
+      <c r="A262" s="3">
         <f t="shared" si="36"/>
         <v>1451</v>
       </c>
-      <c r="B262" s="4">
-        <f>B260</f>
-        <v>352</v>
-      </c>
-      <c r="C262" s="4">
-        <v>20</v>
-      </c>
-      <c r="D262" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E262" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F262" s="4">
-        <v>2</v>
-      </c>
-      <c r="G262" s="4" t="str">
+      <c r="B262" s="3">
+        <f>B258+1</f>
+        <v>351</v>
+      </c>
+      <c r="C262" s="3">
+        <v>66</v>
+      </c>
+      <c r="D262" s="3">
+        <v>7</v>
+      </c>
+      <c r="E262" s="3">
+        <v>0</v>
+      </c>
+      <c r="F262" s="3">
+        <v>2</v>
+      </c>
+      <c r="G262" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1451, 352, 20, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1451, 351, 66, 7, 0, 2);</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A263" s="4">
+      <c r="A263" s="3">
         <f t="shared" si="36"/>
         <v>1452</v>
       </c>
-      <c r="B263" s="4">
-        <f t="shared" ref="B263" si="47">B260</f>
-        <v>352</v>
-      </c>
-      <c r="C263" s="4">
-        <v>20</v>
-      </c>
-      <c r="D263" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E263" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F263" s="4">
-        <v>1</v>
-      </c>
-      <c r="G263" s="4" t="str">
+      <c r="B263" s="3">
+        <f>B262</f>
+        <v>351</v>
+      </c>
+      <c r="C263" s="3">
+        <v>66</v>
+      </c>
+      <c r="D263" s="3">
+        <v>4</v>
+      </c>
+      <c r="E263" s="3">
+        <v>0</v>
+      </c>
+      <c r="F263" s="3">
+        <v>1</v>
+      </c>
+      <c r="G263" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1452, 352, 20, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1452, 351, 66, 4, 0, 1);</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
@@ -51271,24 +51271,24 @@
         <v>1453</v>
       </c>
       <c r="B264" s="3">
-        <f>B260+1</f>
-        <v>353</v>
-      </c>
-      <c r="C264" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D264" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E264" s="3" t="s">
-        <v>18</v>
+        <f>B262</f>
+        <v>351</v>
+      </c>
+      <c r="C264" s="3">
+        <v>994</v>
+      </c>
+      <c r="D264" s="3">
+        <v>7</v>
+      </c>
+      <c r="E264" s="3">
+        <v>0</v>
       </c>
       <c r="F264" s="3">
         <v>2</v>
       </c>
       <c r="G264" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1453, 353, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1453, 351, 994, 7, 0, 2);</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
@@ -51297,24 +51297,24 @@
         <v>1454</v>
       </c>
       <c r="B265" s="3">
-        <f>B264</f>
-        <v>353</v>
-      </c>
-      <c r="C265" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D265" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E265" s="3" t="s">
-        <v>18</v>
+        <f t="shared" ref="B265:B269" si="46">B262</f>
+        <v>351</v>
+      </c>
+      <c r="C265" s="3">
+        <v>994</v>
+      </c>
+      <c r="D265" s="3">
+        <v>4</v>
+      </c>
+      <c r="E265" s="3">
+        <v>0</v>
       </c>
       <c r="F265" s="3">
         <v>1</v>
       </c>
       <c r="G265" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1454, 353, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1454, 351, 994, 4, 0, 1);</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -51323,24 +51323,24 @@
         <v>1455</v>
       </c>
       <c r="B266" s="3">
-        <f>B264</f>
-        <v>353</v>
-      </c>
-      <c r="C266" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D266" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E266" s="3" t="s">
-        <v>18</v>
+        <f t="shared" si="46"/>
+        <v>351</v>
+      </c>
+      <c r="C266" s="3">
+        <v>66</v>
+      </c>
+      <c r="D266" s="3">
+        <v>8</v>
+      </c>
+      <c r="E266" s="3">
+        <v>0</v>
       </c>
       <c r="F266" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G266" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1455, 353, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1455, 351, 66, 8, 0, 4);</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -51349,76 +51349,76 @@
         <v>1456</v>
       </c>
       <c r="B267" s="3">
-        <f t="shared" ref="B267" si="48">B264</f>
-        <v>353</v>
-      </c>
-      <c r="C267" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D267" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E267" s="3" t="s">
-        <v>18</v>
+        <f t="shared" si="46"/>
+        <v>351</v>
+      </c>
+      <c r="C267" s="3">
+        <v>66</v>
+      </c>
+      <c r="D267" s="3">
+        <v>7</v>
+      </c>
+      <c r="E267" s="3">
+        <v>0</v>
       </c>
       <c r="F267" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G267" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1456, 353, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1456, 351, 66, 7, 0, 3);</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A268" s="4">
+      <c r="A268" s="3">
         <f t="shared" si="36"/>
         <v>1457</v>
       </c>
-      <c r="B268" s="4">
-        <f>B264+1</f>
-        <v>354</v>
-      </c>
-      <c r="C268" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D268" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E268" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F268" s="4">
-        <v>2</v>
-      </c>
-      <c r="G268" s="4" t="str">
+      <c r="B268" s="3">
+        <f t="shared" si="46"/>
+        <v>351</v>
+      </c>
+      <c r="C268" s="3">
+        <v>994</v>
+      </c>
+      <c r="D268" s="3">
+        <v>13</v>
+      </c>
+      <c r="E268" s="3">
+        <v>3</v>
+      </c>
+      <c r="F268" s="3">
+        <v>4</v>
+      </c>
+      <c r="G268" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1457, 354, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1457, 351, 994, 13, 3, 4);</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="4">
+      <c r="A269" s="3">
         <f t="shared" si="36"/>
         <v>1458</v>
       </c>
-      <c r="B269" s="4">
-        <f>B268</f>
-        <v>354</v>
-      </c>
-      <c r="C269" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D269" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E269" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F269" s="4">
-        <v>1</v>
-      </c>
-      <c r="G269" s="4" t="str">
+      <c r="B269" s="3">
+        <f t="shared" si="46"/>
+        <v>351</v>
+      </c>
+      <c r="C269" s="3">
+        <v>994</v>
+      </c>
+      <c r="D269" s="3">
+        <v>10</v>
+      </c>
+      <c r="E269" s="3">
+        <v>0</v>
+      </c>
+      <c r="F269" s="3">
+        <v>3</v>
+      </c>
+      <c r="G269" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1458, 354, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1458, 351, 994, 10, 0, 3);</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
@@ -51427,24 +51427,24 @@
         <v>1459</v>
       </c>
       <c r="B270" s="4">
-        <f>B268</f>
-        <v>354</v>
-      </c>
-      <c r="C270" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D270" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E270" s="4" t="s">
-        <v>18</v>
+        <f>B262+1</f>
+        <v>352</v>
+      </c>
+      <c r="C270" s="4">
+        <v>39</v>
+      </c>
+      <c r="D270" s="4">
+        <v>3</v>
+      </c>
+      <c r="E270" s="4">
+        <v>0</v>
       </c>
       <c r="F270" s="4">
         <v>2</v>
       </c>
       <c r="G270" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1459, 354, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1459, 352, 39, 3, 0, 2);</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
@@ -51453,128 +51453,128 @@
         <v>1460</v>
       </c>
       <c r="B271" s="4">
-        <f t="shared" ref="B271" si="49">B268</f>
-        <v>354</v>
-      </c>
-      <c r="C271" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D271" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E271" s="4" t="s">
-        <v>18</v>
+        <f>B270</f>
+        <v>352</v>
+      </c>
+      <c r="C271" s="4">
+        <v>39</v>
+      </c>
+      <c r="D271" s="4">
+        <v>2</v>
+      </c>
+      <c r="E271" s="4">
+        <v>0</v>
       </c>
       <c r="F271" s="4">
         <v>1</v>
       </c>
       <c r="G271" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1460, 354, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1460, 352, 39, 2, 0, 1);</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A272" s="3">
+      <c r="A272" s="4">
         <f t="shared" si="36"/>
         <v>1461</v>
       </c>
-      <c r="B272" s="3">
-        <f>B268+1</f>
-        <v>355</v>
-      </c>
-      <c r="C272" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D272" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E272" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F272" s="3">
-        <v>2</v>
-      </c>
-      <c r="G272" s="3" t="str">
+      <c r="B272" s="4">
+        <f>B270</f>
+        <v>352</v>
+      </c>
+      <c r="C272" s="4">
+        <v>20</v>
+      </c>
+      <c r="D272" s="4">
+        <v>3</v>
+      </c>
+      <c r="E272" s="4">
+        <v>0</v>
+      </c>
+      <c r="F272" s="4">
+        <v>2</v>
+      </c>
+      <c r="G272" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1461, 355, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1461, 352, 20, 3, 0, 2);</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A273" s="3">
+      <c r="A273" s="4">
         <f t="shared" si="36"/>
         <v>1462</v>
       </c>
-      <c r="B273" s="3">
-        <f>B272</f>
-        <v>355</v>
-      </c>
-      <c r="C273" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D273" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E273" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F273" s="3">
-        <v>1</v>
-      </c>
-      <c r="G273" s="3" t="str">
+      <c r="B273" s="4">
+        <f t="shared" ref="B273:B277" si="47">B270</f>
+        <v>352</v>
+      </c>
+      <c r="C273" s="4">
+        <v>20</v>
+      </c>
+      <c r="D273" s="4">
+        <v>2</v>
+      </c>
+      <c r="E273" s="4">
+        <v>0</v>
+      </c>
+      <c r="F273" s="4">
+        <v>1</v>
+      </c>
+      <c r="G273" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1462, 355, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1462, 352, 20, 2, 0, 1);</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A274" s="3">
+      <c r="A274" s="4">
         <f t="shared" si="36"/>
         <v>1463</v>
       </c>
-      <c r="B274" s="3">
-        <f>B272</f>
-        <v>355</v>
-      </c>
-      <c r="C274" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D274" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E274" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F274" s="3">
-        <v>2</v>
-      </c>
-      <c r="G274" s="3" t="str">
+      <c r="B274" s="4">
+        <f t="shared" si="47"/>
+        <v>352</v>
+      </c>
+      <c r="C274" s="4">
+        <v>39</v>
+      </c>
+      <c r="D274" s="4">
+        <v>3</v>
+      </c>
+      <c r="E274" s="4">
+        <v>1</v>
+      </c>
+      <c r="F274" s="4">
+        <v>4</v>
+      </c>
+      <c r="G274" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1463, 355, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1463, 352, 39, 3, 1, 4);</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A275" s="3">
+      <c r="A275" s="4">
         <f t="shared" si="36"/>
         <v>1464</v>
       </c>
-      <c r="B275" s="3">
-        <f t="shared" ref="B275" si="50">B272</f>
-        <v>355</v>
-      </c>
-      <c r="C275" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D275" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E275" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F275" s="3">
-        <v>1</v>
-      </c>
-      <c r="G275" s="3" t="str">
+      <c r="B275" s="4">
+        <f t="shared" si="47"/>
+        <v>352</v>
+      </c>
+      <c r="C275" s="4">
+        <v>39</v>
+      </c>
+      <c r="D275" s="4">
+        <v>3</v>
+      </c>
+      <c r="E275" s="4">
+        <v>0</v>
+      </c>
+      <c r="F275" s="4">
+        <v>3</v>
+      </c>
+      <c r="G275" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1464, 355, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1464, 352, 39, 3, 0, 3);</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
@@ -51583,24 +51583,24 @@
         <v>1465</v>
       </c>
       <c r="B276" s="4">
-        <f>B272+1</f>
-        <v>356</v>
-      </c>
-      <c r="C276" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D276" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E276" s="4" t="s">
-        <v>18</v>
+        <f t="shared" si="47"/>
+        <v>352</v>
+      </c>
+      <c r="C276" s="4">
+        <v>20</v>
+      </c>
+      <c r="D276" s="4">
+        <v>4</v>
+      </c>
+      <c r="E276" s="4">
+        <v>1</v>
       </c>
       <c r="F276" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G276" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1465, 356, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1465, 352, 20, 4, 1, 4);</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
@@ -51609,76 +51609,76 @@
         <v>1466</v>
       </c>
       <c r="B277" s="4">
-        <f>B276</f>
-        <v>356</v>
-      </c>
-      <c r="C277" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D277" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E277" s="4" t="s">
-        <v>18</v>
+        <f t="shared" si="47"/>
+        <v>352</v>
+      </c>
+      <c r="C277" s="4">
+        <v>20</v>
+      </c>
+      <c r="D277" s="4">
+        <v>3</v>
+      </c>
+      <c r="E277" s="4">
+        <v>0</v>
       </c>
       <c r="F277" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G277" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1466, 356, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1466, 352, 20, 3, 0, 3);</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="4">
+      <c r="A278" s="3">
         <f t="shared" si="36"/>
         <v>1467</v>
       </c>
-      <c r="B278" s="4">
-        <f>B276</f>
-        <v>356</v>
-      </c>
-      <c r="C278" s="4" t="s">
+      <c r="B278" s="3">
+        <f>B270+1</f>
+        <v>353</v>
+      </c>
+      <c r="C278" s="3">
+        <v>595</v>
+      </c>
+      <c r="D278" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D278" s="4" t="s">
+      <c r="E278" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E278" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F278" s="4">
-        <v>2</v>
-      </c>
-      <c r="G278" s="4" t="str">
+      <c r="F278" s="3">
+        <v>2</v>
+      </c>
+      <c r="G278" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1467, 356, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1467, 353, 595, null, null, 2);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A279" s="4">
+      <c r="A279" s="3">
         <f t="shared" si="36"/>
         <v>1468</v>
       </c>
-      <c r="B279" s="4">
-        <f t="shared" ref="B279" si="51">B276</f>
-        <v>356</v>
-      </c>
-      <c r="C279" s="4" t="s">
+      <c r="B279" s="3">
+        <f>B278</f>
+        <v>353</v>
+      </c>
+      <c r="C279" s="3">
+        <v>595</v>
+      </c>
+      <c r="D279" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D279" s="4" t="s">
+      <c r="E279" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E279" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F279" s="4">
-        <v>1</v>
-      </c>
-      <c r="G279" s="4" t="str">
+      <c r="F279" s="3">
+        <v>1</v>
+      </c>
+      <c r="G279" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1468, 356, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1468, 353, 595, null, null, 1);</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -51687,11 +51687,11 @@
         <v>1469</v>
       </c>
       <c r="B280" s="3">
-        <f>B276+1</f>
-        <v>357</v>
-      </c>
-      <c r="C280" s="3" t="s">
-        <v>18</v>
+        <f>B278</f>
+        <v>353</v>
+      </c>
+      <c r="C280" s="3">
+        <v>98</v>
       </c>
       <c r="D280" s="3" t="s">
         <v>18</v>
@@ -51703,8 +51703,8 @@
         <v>2</v>
       </c>
       <c r="G280" s="3" t="str">
-        <f t="shared" ref="G280:G295" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A280 &amp; ", " &amp; B280 &amp; ", " &amp; C280 &amp; ", " &amp; D280 &amp; ", " &amp; E280 &amp; ", " &amp; F280 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1469, 357, null, null, null, 2);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1469, 353, 98, null, null, 2);</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -51713,11 +51713,11 @@
         <v>1470</v>
       </c>
       <c r="B281" s="3">
-        <f>B280</f>
-        <v>357</v>
-      </c>
-      <c r="C281" s="3" t="s">
-        <v>18</v>
+        <f t="shared" ref="B281" si="48">B278</f>
+        <v>353</v>
+      </c>
+      <c r="C281" s="3">
+        <v>98</v>
       </c>
       <c r="D281" s="3" t="s">
         <v>18</v>
@@ -51729,73 +51729,73 @@
         <v>1</v>
       </c>
       <c r="G281" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1470, 357, null, null, null, 1);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1470, 353, 98, null, null, 1);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282" s="3">
+      <c r="A282" s="4">
         <f t="shared" si="36"/>
         <v>1471</v>
       </c>
-      <c r="B282" s="3">
-        <f>B280</f>
-        <v>357</v>
-      </c>
-      <c r="C282" s="3" t="s">
+      <c r="B282" s="4">
+        <f>B278+1</f>
+        <v>354</v>
+      </c>
+      <c r="C282" s="4">
+        <v>7</v>
+      </c>
+      <c r="D282" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D282" s="3" t="s">
+      <c r="E282" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E282" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F282" s="3">
-        <v>2</v>
-      </c>
-      <c r="G282" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1471, 357, null, null, null, 2);</v>
+      <c r="F282" s="4">
+        <v>2</v>
+      </c>
+      <c r="G282" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1471, 354, 7, null, null, 2);</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A283" s="3">
+      <c r="A283" s="4">
         <f t="shared" si="36"/>
         <v>1472</v>
       </c>
-      <c r="B283" s="3">
-        <f t="shared" ref="B283" si="53">B280</f>
-        <v>357</v>
-      </c>
-      <c r="C283" s="3" t="s">
+      <c r="B283" s="4">
+        <f>B282</f>
+        <v>354</v>
+      </c>
+      <c r="C283" s="4">
+        <v>7</v>
+      </c>
+      <c r="D283" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D283" s="3" t="s">
+      <c r="E283" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E283" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F283" s="3">
-        <v>1</v>
-      </c>
-      <c r="G283" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1472, 357, null, null, null, 1);</v>
+      <c r="F283" s="4">
+        <v>1</v>
+      </c>
+      <c r="G283" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1472, 354, 7, null, null, 1);</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="4">
-        <f t="shared" ref="A284:A295" si="54">A283+1</f>
+        <f t="shared" si="36"/>
         <v>1473</v>
       </c>
       <c r="B284" s="4">
-        <f>B280+1</f>
-        <v>358</v>
-      </c>
-      <c r="C284" s="4" t="s">
-        <v>18</v>
+        <f>B282</f>
+        <v>354</v>
+      </c>
+      <c r="C284" s="4">
+        <v>34</v>
       </c>
       <c r="D284" s="4" t="s">
         <v>18</v>
@@ -51807,21 +51807,21 @@
         <v>2</v>
       </c>
       <c r="G284" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1473, 358, null, null, null, 2);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1473, 354, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1474</v>
       </c>
       <c r="B285" s="4">
-        <f>B284</f>
-        <v>358</v>
-      </c>
-      <c r="C285" s="4" t="s">
-        <v>18</v>
+        <f t="shared" ref="B285" si="49">B282</f>
+        <v>354</v>
+      </c>
+      <c r="C285" s="4">
+        <v>34</v>
       </c>
       <c r="D285" s="4" t="s">
         <v>18</v>
@@ -51833,73 +51833,73 @@
         <v>1</v>
       </c>
       <c r="G285" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1474, 358, null, null, null, 1);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1474, 354, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="4">
-        <f t="shared" si="54"/>
+      <c r="A286" s="3">
+        <f t="shared" si="36"/>
         <v>1475</v>
       </c>
-      <c r="B286" s="4">
-        <f>B284</f>
-        <v>358</v>
-      </c>
-      <c r="C286" s="4" t="s">
+      <c r="B286" s="3">
+        <f>B282+1</f>
+        <v>355</v>
+      </c>
+      <c r="C286" s="3">
+        <v>54</v>
+      </c>
+      <c r="D286" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D286" s="4" t="s">
+      <c r="E286" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E286" s="4" t="s">
+      <c r="F286" s="3">
+        <v>2</v>
+      </c>
+      <c r="G286" s="3" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1475, 355, 54, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="3">
+        <f t="shared" si="36"/>
+        <v>1476</v>
+      </c>
+      <c r="B287" s="3">
+        <f>B286</f>
+        <v>355</v>
+      </c>
+      <c r="C287" s="3">
+        <v>54</v>
+      </c>
+      <c r="D287" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F286" s="4">
-        <v>2</v>
-      </c>
-      <c r="G286" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1475, 358, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" s="4">
-        <f t="shared" si="54"/>
-        <v>1476</v>
-      </c>
-      <c r="B287" s="4">
-        <f t="shared" ref="B287" si="55">B284</f>
-        <v>358</v>
-      </c>
-      <c r="C287" s="4" t="s">
+      <c r="E287" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D287" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E287" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F287" s="4">
-        <v>1</v>
-      </c>
-      <c r="G287" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1476, 358, null, null, null, 1);</v>
+      <c r="F287" s="3">
+        <v>1</v>
+      </c>
+      <c r="G287" s="3" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1476, 355, 54, null, null, 1);</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1477</v>
       </c>
       <c r="B288" s="3">
-        <f>B284+1</f>
-        <v>359</v>
-      </c>
-      <c r="C288" s="3" t="s">
-        <v>18</v>
+        <f>B286</f>
+        <v>355</v>
+      </c>
+      <c r="C288" s="3">
+        <v>20</v>
       </c>
       <c r="D288" s="3" t="s">
         <v>18</v>
@@ -51911,21 +51911,21 @@
         <v>2</v>
       </c>
       <c r="G288" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1477, 359, null, null, null, 2);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1477, 355, 20, null, null, 2);</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1478</v>
       </c>
       <c r="B289" s="3">
-        <f>B288</f>
-        <v>359</v>
-      </c>
-      <c r="C289" s="3" t="s">
-        <v>18</v>
+        <f t="shared" ref="B289" si="50">B286</f>
+        <v>355</v>
+      </c>
+      <c r="C289" s="3">
+        <v>20</v>
       </c>
       <c r="D289" s="3" t="s">
         <v>18</v>
@@ -51937,73 +51937,73 @@
         <v>1</v>
       </c>
       <c r="G289" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1478, 359, null, null, null, 1);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1478, 355, 20, null, null, 1);</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A290" s="3">
-        <f t="shared" si="54"/>
+      <c r="A290" s="4">
+        <f t="shared" si="36"/>
         <v>1479</v>
       </c>
-      <c r="B290" s="3">
-        <f>B288</f>
-        <v>359</v>
-      </c>
-      <c r="C290" s="3" t="s">
+      <c r="B290" s="4">
+        <f>B286+1</f>
+        <v>356</v>
+      </c>
+      <c r="C290" s="4">
+        <v>994</v>
+      </c>
+      <c r="D290" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D290" s="3" t="s">
+      <c r="E290" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E290" s="3" t="s">
+      <c r="F290" s="4">
+        <v>2</v>
+      </c>
+      <c r="G290" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1479, 356, 994, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="4">
+        <f t="shared" si="36"/>
+        <v>1480</v>
+      </c>
+      <c r="B291" s="4">
+        <f>B290</f>
+        <v>356</v>
+      </c>
+      <c r="C291" s="4">
+        <v>994</v>
+      </c>
+      <c r="D291" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F290" s="3">
-        <v>2</v>
-      </c>
-      <c r="G290" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1479, 359, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A291" s="3">
-        <f t="shared" si="54"/>
-        <v>1480</v>
-      </c>
-      <c r="B291" s="3">
-        <f t="shared" ref="B291" si="56">B288</f>
-        <v>359</v>
-      </c>
-      <c r="C291" s="3" t="s">
+      <c r="E291" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D291" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E291" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F291" s="3">
-        <v>1</v>
-      </c>
-      <c r="G291" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1480, 359, null, null, null, 1);</v>
+      <c r="F291" s="4">
+        <v>1</v>
+      </c>
+      <c r="G291" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1480, 356, 994, null, null, 1);</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1481</v>
       </c>
       <c r="B292" s="4">
-        <f>B288+1</f>
-        <v>360</v>
-      </c>
-      <c r="C292" s="4" t="s">
-        <v>18</v>
+        <f>B290</f>
+        <v>356</v>
+      </c>
+      <c r="C292" s="4">
+        <v>351</v>
       </c>
       <c r="D292" s="4" t="s">
         <v>18</v>
@@ -52015,21 +52015,21 @@
         <v>2</v>
       </c>
       <c r="G292" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1481, 360, null, null, null, 2);</v>
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1481, 356, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="36"/>
         <v>1482</v>
       </c>
       <c r="B293" s="4">
-        <f>B292</f>
-        <v>360</v>
-      </c>
-      <c r="C293" s="4" t="s">
-        <v>18</v>
+        <f t="shared" ref="B293" si="51">B290</f>
+        <v>356</v>
+      </c>
+      <c r="C293" s="4">
+        <v>351</v>
       </c>
       <c r="D293" s="4" t="s">
         <v>18</v>
@@ -52041,60 +52041,424 @@
         <v>1</v>
       </c>
       <c r="G293" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1482, 356, 351, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="3">
+        <f t="shared" si="36"/>
+        <v>1483</v>
+      </c>
+      <c r="B294" s="3">
+        <f>B290+1</f>
+        <v>357</v>
+      </c>
+      <c r="C294" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D294" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E294" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F294" s="3">
+        <v>2</v>
+      </c>
+      <c r="G294" s="3" t="str">
+        <f t="shared" ref="G294:G309" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A294 &amp; ", " &amp; B294 &amp; ", " &amp; C294 &amp; ", " &amp; D294 &amp; ", " &amp; E294 &amp; ", " &amp; F294 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1483, 357, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="3">
+        <f t="shared" si="36"/>
+        <v>1484</v>
+      </c>
+      <c r="B295" s="3">
+        <f>B294</f>
+        <v>357</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D295" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E295" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F295" s="3">
+        <v>1</v>
+      </c>
+      <c r="G295" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1482, 360, null, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A294" s="4">
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1484, 357, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="3">
+        <f t="shared" si="36"/>
+        <v>1485</v>
+      </c>
+      <c r="B296" s="3">
+        <f>B294</f>
+        <v>357</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E296" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F296" s="3">
+        <v>2</v>
+      </c>
+      <c r="G296" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1485, 357, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="3">
+        <f t="shared" si="36"/>
+        <v>1486</v>
+      </c>
+      <c r="B297" s="3">
+        <f t="shared" ref="B297" si="53">B294</f>
+        <v>357</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D297" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E297" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F297" s="3">
+        <v>1</v>
+      </c>
+      <c r="G297" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1486, 357, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="4">
+        <f t="shared" ref="A298:A309" si="54">A297+1</f>
+        <v>1487</v>
+      </c>
+      <c r="B298" s="4">
+        <f>B294+1</f>
+        <v>358</v>
+      </c>
+      <c r="C298" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D298" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E298" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F298" s="4">
+        <v>2</v>
+      </c>
+      <c r="G298" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1487, 358, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="4">
         <f t="shared" si="54"/>
-        <v>1483</v>
-      </c>
-      <c r="B294" s="4">
-        <f>B292</f>
+        <v>1488</v>
+      </c>
+      <c r="B299" s="4">
+        <f>B298</f>
+        <v>358</v>
+      </c>
+      <c r="C299" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D299" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E299" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F299" s="4">
+        <v>1</v>
+      </c>
+      <c r="G299" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1488, 358, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="4">
+        <f t="shared" si="54"/>
+        <v>1489</v>
+      </c>
+      <c r="B300" s="4">
+        <f>B298</f>
+        <v>358</v>
+      </c>
+      <c r="C300" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D300" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E300" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F300" s="4">
+        <v>2</v>
+      </c>
+      <c r="G300" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1489, 358, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="4">
+        <f t="shared" si="54"/>
+        <v>1490</v>
+      </c>
+      <c r="B301" s="4">
+        <f t="shared" ref="B301" si="55">B298</f>
+        <v>358</v>
+      </c>
+      <c r="C301" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D301" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E301" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F301" s="4">
+        <v>1</v>
+      </c>
+      <c r="G301" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1490, 358, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="3">
+        <f t="shared" si="54"/>
+        <v>1491</v>
+      </c>
+      <c r="B302" s="3">
+        <f>B298+1</f>
+        <v>359</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D302" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F302" s="3">
+        <v>2</v>
+      </c>
+      <c r="G302" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1491, 359, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="3">
+        <f t="shared" si="54"/>
+        <v>1492</v>
+      </c>
+      <c r="B303" s="3">
+        <f>B302</f>
+        <v>359</v>
+      </c>
+      <c r="C303" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D303" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E303" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F303" s="3">
+        <v>1</v>
+      </c>
+      <c r="G303" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1492, 359, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="3">
+        <f t="shared" si="54"/>
+        <v>1493</v>
+      </c>
+      <c r="B304" s="3">
+        <f>B302</f>
+        <v>359</v>
+      </c>
+      <c r="C304" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D304" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E304" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F304" s="3">
+        <v>2</v>
+      </c>
+      <c r="G304" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1493, 359, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="3">
+        <f t="shared" si="54"/>
+        <v>1494</v>
+      </c>
+      <c r="B305" s="3">
+        <f t="shared" ref="B305" si="56">B302</f>
+        <v>359</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D305" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E305" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F305" s="3">
+        <v>1</v>
+      </c>
+      <c r="G305" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1494, 359, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="4">
+        <f t="shared" si="54"/>
+        <v>1495</v>
+      </c>
+      <c r="B306" s="4">
+        <f>B302+1</f>
         <v>360</v>
       </c>
-      <c r="C294" s="4" t="s">
+      <c r="C306" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D294" s="4" t="s">
+      <c r="D306" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E294" s="4" t="s">
+      <c r="E306" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F294" s="4">
-        <v>2</v>
-      </c>
-      <c r="G294" s="4" t="str">
+      <c r="F306" s="4">
+        <v>2</v>
+      </c>
+      <c r="G306" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1483, 360, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A295" s="4">
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1495, 360, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="4">
         <f t="shared" si="54"/>
-        <v>1484</v>
-      </c>
-      <c r="B295" s="4">
-        <f t="shared" ref="B295" si="57">B292</f>
+        <v>1496</v>
+      </c>
+      <c r="B307" s="4">
+        <f>B306</f>
         <v>360</v>
       </c>
-      <c r="C295" s="4" t="s">
+      <c r="C307" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D295" s="4" t="s">
+      <c r="D307" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E295" s="4" t="s">
+      <c r="E307" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F295" s="4">
-        <v>1</v>
-      </c>
-      <c r="G295" s="4" t="str">
+      <c r="F307" s="4">
+        <v>1</v>
+      </c>
+      <c r="G307" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1484, 360, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1496, 360, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="4">
+        <f t="shared" si="54"/>
+        <v>1497</v>
+      </c>
+      <c r="B308" s="4">
+        <f>B306</f>
+        <v>360</v>
+      </c>
+      <c r="C308" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D308" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E308" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F308" s="4">
+        <v>2</v>
+      </c>
+      <c r="G308" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1497, 360, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="4">
+        <f t="shared" si="54"/>
+        <v>1498</v>
+      </c>
+      <c r="B309" s="4">
+        <f t="shared" ref="B309" si="57">B306</f>
+        <v>360</v>
+      </c>
+      <c r="C309" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D309" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E309" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F309" s="4">
+        <v>1</v>
+      </c>
+      <c r="G309" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1498, 360, null, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Futsal World Cup Quarter-Finals 1st Date
Futsal World Cup Quarter-Finals 1st Date
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -44729,7 +44729,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G309"/>
+  <dimension ref="A1:G313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -49883,7 +49883,7 @@
         <v>2</v>
       </c>
       <c r="G210" s="3" t="str">
-        <f t="shared" ref="G210:G293" si="34">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A210 &amp; ", " &amp; B210 &amp; ", " &amp; C210 &amp; ", " &amp; D210 &amp; ", " &amp; E210 &amp; ", " &amp; F210 &amp; ");"</f>
+        <f t="shared" ref="G210:G297" si="34">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A210 &amp; ", " &amp; B210 &amp; ", " &amp; C210 &amp; ", " &amp; D210 &amp; ", " &amp; E210 &amp; ", " &amp; F210 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1399, 341, 994, 2, 0, 2);</v>
       </c>
     </row>
@@ -49967,7 +49967,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
-        <f t="shared" ref="A214:A297" si="36">A213+1</f>
+        <f t="shared" ref="A214:A301" si="36">A213+1</f>
         <v>1403</v>
       </c>
       <c r="B214" s="4">
@@ -51641,18 +51641,18 @@
       <c r="C278" s="3">
         <v>595</v>
       </c>
-      <c r="D278" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E278" s="3" t="s">
-        <v>18</v>
+      <c r="D278" s="3">
+        <v>3</v>
+      </c>
+      <c r="E278" s="3">
+        <v>0</v>
       </c>
       <c r="F278" s="3">
         <v>2</v>
       </c>
       <c r="G278" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1467, 353, 595, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1467, 353, 595, 3, 0, 2);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
@@ -51667,18 +51667,18 @@
       <c r="C279" s="3">
         <v>595</v>
       </c>
-      <c r="D279" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E279" s="3" t="s">
-        <v>18</v>
+      <c r="D279" s="3">
+        <v>2</v>
+      </c>
+      <c r="E279" s="3">
+        <v>0</v>
       </c>
       <c r="F279" s="3">
         <v>1</v>
       </c>
       <c r="G279" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1468, 353, 595, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1468, 353, 595, 2, 0, 1);</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -51693,18 +51693,18 @@
       <c r="C280" s="3">
         <v>98</v>
       </c>
-      <c r="D280" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E280" s="3" t="s">
-        <v>18</v>
+      <c r="D280" s="3">
+        <v>3</v>
+      </c>
+      <c r="E280" s="3">
+        <v>0</v>
       </c>
       <c r="F280" s="3">
         <v>2</v>
       </c>
       <c r="G280" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1469, 353, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1469, 353, 98, 3, 0, 2);</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -51713,752 +51713,856 @@
         <v>1470</v>
       </c>
       <c r="B281" s="3">
-        <f t="shared" ref="B281" si="48">B278</f>
+        <f t="shared" ref="B281:B285" si="48">B278</f>
         <v>353</v>
       </c>
       <c r="C281" s="3">
         <v>98</v>
       </c>
-      <c r="D281" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E281" s="3" t="s">
-        <v>18</v>
+      <c r="D281" s="3">
+        <v>1</v>
+      </c>
+      <c r="E281" s="3">
+        <v>0</v>
       </c>
       <c r="F281" s="3">
         <v>1</v>
       </c>
       <c r="G281" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1470, 353, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1470, 353, 98, 1, 0, 1);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282" s="4">
+      <c r="A282" s="3">
         <f t="shared" si="36"/>
         <v>1471</v>
       </c>
-      <c r="B282" s="4">
+      <c r="B282" s="3">
+        <f t="shared" si="48"/>
+        <v>353</v>
+      </c>
+      <c r="C282" s="3">
+        <v>595</v>
+      </c>
+      <c r="D282" s="3">
+        <v>3</v>
+      </c>
+      <c r="E282" s="3">
+        <v>0</v>
+      </c>
+      <c r="F282" s="3">
+        <v>4</v>
+      </c>
+      <c r="G282" s="3" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1471, 353, 595, 3, 0, 4);</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="3">
+        <f t="shared" si="36"/>
+        <v>1472</v>
+      </c>
+      <c r="B283" s="3">
+        <f t="shared" si="48"/>
+        <v>353</v>
+      </c>
+      <c r="C283" s="3">
+        <v>595</v>
+      </c>
+      <c r="D283" s="3">
+        <v>3</v>
+      </c>
+      <c r="E283" s="3">
+        <v>0</v>
+      </c>
+      <c r="F283" s="3">
+        <v>3</v>
+      </c>
+      <c r="G283" s="3" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1472, 353, 595, 3, 0, 3);</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="3">
+        <f t="shared" si="36"/>
+        <v>1473</v>
+      </c>
+      <c r="B284" s="3">
+        <f t="shared" si="48"/>
+        <v>353</v>
+      </c>
+      <c r="C284" s="3">
+        <v>98</v>
+      </c>
+      <c r="D284" s="3">
+        <v>4</v>
+      </c>
+      <c r="E284" s="3">
+        <v>3</v>
+      </c>
+      <c r="F284" s="3">
+        <v>4</v>
+      </c>
+      <c r="G284" s="3" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1473, 353, 98, 4, 3, 4);</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="3">
+        <f t="shared" si="36"/>
+        <v>1474</v>
+      </c>
+      <c r="B285" s="3">
+        <f t="shared" si="48"/>
+        <v>353</v>
+      </c>
+      <c r="C285" s="3">
+        <v>98</v>
+      </c>
+      <c r="D285" s="3">
+        <v>3</v>
+      </c>
+      <c r="E285" s="3">
+        <v>0</v>
+      </c>
+      <c r="F285" s="3">
+        <v>3</v>
+      </c>
+      <c r="G285" s="3" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1474, 353, 98, 3, 0, 3);</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="4">
+        <f t="shared" si="36"/>
+        <v>1475</v>
+      </c>
+      <c r="B286" s="4">
         <f>B278+1</f>
         <v>354</v>
       </c>
-      <c r="C282" s="4">
+      <c r="C286" s="4">
         <v>7</v>
       </c>
-      <c r="D282" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E282" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F282" s="4">
-        <v>2</v>
-      </c>
-      <c r="G282" s="4" t="str">
+      <c r="D286" s="4">
+        <v>6</v>
+      </c>
+      <c r="E286" s="4">
+        <v>3</v>
+      </c>
+      <c r="F286" s="4">
+        <v>2</v>
+      </c>
+      <c r="G286" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1471, 354, 7, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A283" s="4">
-        <f t="shared" si="36"/>
-        <v>1472</v>
-      </c>
-      <c r="B283" s="4">
-        <f>B282</f>
-        <v>354</v>
-      </c>
-      <c r="C283" s="4">
-        <v>7</v>
-      </c>
-      <c r="D283" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E283" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F283" s="4">
-        <v>1</v>
-      </c>
-      <c r="G283" s="4" t="str">
-        <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1472, 354, 7, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A284" s="4">
-        <f t="shared" si="36"/>
-        <v>1473</v>
-      </c>
-      <c r="B284" s="4">
-        <f>B282</f>
-        <v>354</v>
-      </c>
-      <c r="C284" s="4">
-        <v>34</v>
-      </c>
-      <c r="D284" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E284" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F284" s="4">
-        <v>2</v>
-      </c>
-      <c r="G284" s="4" t="str">
-        <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1473, 354, 34, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" s="4">
-        <f t="shared" si="36"/>
-        <v>1474</v>
-      </c>
-      <c r="B285" s="4">
-        <f t="shared" ref="B285" si="49">B282</f>
-        <v>354</v>
-      </c>
-      <c r="C285" s="4">
-        <v>34</v>
-      </c>
-      <c r="D285" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E285" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F285" s="4">
-        <v>1</v>
-      </c>
-      <c r="G285" s="4" t="str">
-        <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1474, 354, 34, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="3">
-        <f t="shared" si="36"/>
-        <v>1475</v>
-      </c>
-      <c r="B286" s="3">
-        <f>B282+1</f>
-        <v>355</v>
-      </c>
-      <c r="C286" s="3">
-        <v>54</v>
-      </c>
-      <c r="D286" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E286" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F286" s="3">
-        <v>2</v>
-      </c>
-      <c r="G286" s="3" t="str">
-        <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1475, 355, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1475, 354, 7, 6, 3, 2);</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" s="3">
+      <c r="A287" s="4">
         <f t="shared" si="36"/>
         <v>1476</v>
       </c>
-      <c r="B287" s="3">
+      <c r="B287" s="4">
         <f>B286</f>
-        <v>355</v>
-      </c>
-      <c r="C287" s="3">
-        <v>54</v>
-      </c>
-      <c r="D287" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E287" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F287" s="3">
-        <v>1</v>
-      </c>
-      <c r="G287" s="3" t="str">
+        <v>354</v>
+      </c>
+      <c r="C287" s="4">
+        <v>7</v>
+      </c>
+      <c r="D287" s="4">
+        <v>3</v>
+      </c>
+      <c r="E287" s="4">
+        <v>0</v>
+      </c>
+      <c r="F287" s="4">
+        <v>1</v>
+      </c>
+      <c r="G287" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1476, 355, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1476, 354, 7, 3, 0, 1);</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A288" s="3">
+      <c r="A288" s="4">
         <f t="shared" si="36"/>
         <v>1477</v>
       </c>
-      <c r="B288" s="3">
+      <c r="B288" s="4">
         <f>B286</f>
-        <v>355</v>
-      </c>
-      <c r="C288" s="3">
-        <v>20</v>
-      </c>
-      <c r="D288" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E288" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F288" s="3">
-        <v>2</v>
-      </c>
-      <c r="G288" s="3" t="str">
+        <v>354</v>
+      </c>
+      <c r="C288" s="4">
+        <v>34</v>
+      </c>
+      <c r="D288" s="4">
+        <v>2</v>
+      </c>
+      <c r="E288" s="4">
+        <v>0</v>
+      </c>
+      <c r="F288" s="4">
+        <v>2</v>
+      </c>
+      <c r="G288" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1477, 355, 20, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1477, 354, 34, 2, 0, 2);</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A289" s="3">
+      <c r="A289" s="4">
         <f t="shared" si="36"/>
         <v>1478</v>
       </c>
-      <c r="B289" s="3">
-        <f t="shared" ref="B289" si="50">B286</f>
-        <v>355</v>
-      </c>
-      <c r="C289" s="3">
-        <v>20</v>
-      </c>
-      <c r="D289" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E289" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F289" s="3">
-        <v>1</v>
-      </c>
-      <c r="G289" s="3" t="str">
+      <c r="B289" s="4">
+        <f t="shared" ref="B289" si="49">B286</f>
+        <v>354</v>
+      </c>
+      <c r="C289" s="4">
+        <v>34</v>
+      </c>
+      <c r="D289" s="4">
+        <v>2</v>
+      </c>
+      <c r="E289" s="4">
+        <v>0</v>
+      </c>
+      <c r="F289" s="4">
+        <v>1</v>
+      </c>
+      <c r="G289" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1478, 355, 20, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1478, 354, 34, 2, 0, 1);</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A290" s="4">
+      <c r="A290" s="3">
         <f t="shared" si="36"/>
         <v>1479</v>
       </c>
-      <c r="B290" s="4">
+      <c r="B290" s="3">
         <f>B286+1</f>
-        <v>356</v>
-      </c>
-      <c r="C290" s="4">
-        <v>994</v>
-      </c>
-      <c r="D290" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C290" s="3">
+        <v>54</v>
+      </c>
+      <c r="D290" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E290" s="4" t="s">
+      <c r="E290" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F290" s="4">
-        <v>2</v>
-      </c>
-      <c r="G290" s="4" t="str">
+      <c r="F290" s="3">
+        <v>2</v>
+      </c>
+      <c r="G290" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1479, 356, 994, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1479, 355, 54, null, null, 2);</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A291" s="4">
+      <c r="A291" s="3">
         <f t="shared" si="36"/>
         <v>1480</v>
       </c>
-      <c r="B291" s="4">
+      <c r="B291" s="3">
         <f>B290</f>
-        <v>356</v>
-      </c>
-      <c r="C291" s="4">
-        <v>994</v>
-      </c>
-      <c r="D291" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C291" s="3">
+        <v>54</v>
+      </c>
+      <c r="D291" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E291" s="4" t="s">
+      <c r="E291" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F291" s="4">
-        <v>1</v>
-      </c>
-      <c r="G291" s="4" t="str">
+      <c r="F291" s="3">
+        <v>1</v>
+      </c>
+      <c r="G291" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1480, 356, 994, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1480, 355, 54, null, null, 1);</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A292" s="4">
+      <c r="A292" s="3">
         <f t="shared" si="36"/>
         <v>1481</v>
       </c>
-      <c r="B292" s="4">
+      <c r="B292" s="3">
         <f>B290</f>
-        <v>356</v>
-      </c>
-      <c r="C292" s="4">
-        <v>351</v>
-      </c>
-      <c r="D292" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C292" s="3">
+        <v>20</v>
+      </c>
+      <c r="D292" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E292" s="4" t="s">
+      <c r="E292" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F292" s="4">
-        <v>2</v>
-      </c>
-      <c r="G292" s="4" t="str">
+      <c r="F292" s="3">
+        <v>2</v>
+      </c>
+      <c r="G292" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1481, 356, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1481, 355, 20, null, null, 2);</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A293" s="4">
+      <c r="A293" s="3">
         <f t="shared" si="36"/>
         <v>1482</v>
       </c>
-      <c r="B293" s="4">
-        <f t="shared" ref="B293" si="51">B290</f>
-        <v>356</v>
-      </c>
-      <c r="C293" s="4">
-        <v>351</v>
-      </c>
-      <c r="D293" s="4" t="s">
+      <c r="B293" s="3">
+        <f t="shared" ref="B293" si="50">B290</f>
+        <v>355</v>
+      </c>
+      <c r="C293" s="3">
+        <v>20</v>
+      </c>
+      <c r="D293" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E293" s="4" t="s">
+      <c r="E293" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F293" s="4">
-        <v>1</v>
-      </c>
-      <c r="G293" s="4" t="str">
+      <c r="F293" s="3">
+        <v>1</v>
+      </c>
+      <c r="G293" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1482, 356, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1482, 355, 20, null, null, 1);</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A294" s="3">
+      <c r="A294" s="4">
         <f t="shared" si="36"/>
         <v>1483</v>
       </c>
-      <c r="B294" s="3">
+      <c r="B294" s="4">
         <f>B290+1</f>
-        <v>357</v>
-      </c>
-      <c r="C294" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C294" s="4">
+        <v>994</v>
+      </c>
+      <c r="D294" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D294" s="3" t="s">
+      <c r="E294" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E294" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F294" s="3">
-        <v>2</v>
-      </c>
-      <c r="G294" s="3" t="str">
-        <f t="shared" ref="G294:G309" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A294 &amp; ", " &amp; B294 &amp; ", " &amp; C294 &amp; ", " &amp; D294 &amp; ", " &amp; E294 &amp; ", " &amp; F294 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1483, 357, null, null, null, 2);</v>
+      <c r="F294" s="4">
+        <v>2</v>
+      </c>
+      <c r="G294" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1483, 356, 994, null, null, 2);</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A295" s="3">
+      <c r="A295" s="4">
         <f t="shared" si="36"/>
         <v>1484</v>
       </c>
-      <c r="B295" s="3">
+      <c r="B295" s="4">
         <f>B294</f>
-        <v>357</v>
-      </c>
-      <c r="C295" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C295" s="4">
+        <v>994</v>
+      </c>
+      <c r="D295" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D295" s="3" t="s">
+      <c r="E295" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E295" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F295" s="3">
-        <v>1</v>
-      </c>
-      <c r="G295" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1484, 357, null, null, null, 1);</v>
+      <c r="F295" s="4">
+        <v>1</v>
+      </c>
+      <c r="G295" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1484, 356, 994, null, null, 1);</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A296" s="3">
+      <c r="A296" s="4">
         <f t="shared" si="36"/>
         <v>1485</v>
       </c>
-      <c r="B296" s="3">
+      <c r="B296" s="4">
         <f>B294</f>
-        <v>357</v>
-      </c>
-      <c r="C296" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C296" s="4">
+        <v>351</v>
+      </c>
+      <c r="D296" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D296" s="3" t="s">
+      <c r="E296" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E296" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F296" s="3">
-        <v>2</v>
-      </c>
-      <c r="G296" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1485, 357, null, null, null, 2);</v>
+      <c r="F296" s="4">
+        <v>2</v>
+      </c>
+      <c r="G296" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1485, 356, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A297" s="3">
+      <c r="A297" s="4">
         <f t="shared" si="36"/>
         <v>1486</v>
       </c>
-      <c r="B297" s="3">
-        <f t="shared" ref="B297" si="53">B294</f>
+      <c r="B297" s="4">
+        <f t="shared" ref="B297" si="51">B294</f>
+        <v>356</v>
+      </c>
+      <c r="C297" s="4">
+        <v>351</v>
+      </c>
+      <c r="D297" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E297" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F297" s="4">
+        <v>1</v>
+      </c>
+      <c r="G297" s="4" t="str">
+        <f t="shared" si="34"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1486, 356, 351, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="3">
+        <f t="shared" si="36"/>
+        <v>1487</v>
+      </c>
+      <c r="B298" s="3">
+        <f>B294+1</f>
         <v>357</v>
       </c>
-      <c r="C297" s="3" t="s">
+      <c r="C298" s="3">
+        <v>98</v>
+      </c>
+      <c r="D298" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D297" s="3" t="s">
+      <c r="E298" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E297" s="3" t="s">
+      <c r="F298" s="3">
+        <v>2</v>
+      </c>
+      <c r="G298" s="3" t="str">
+        <f t="shared" ref="G298:G313" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A298 &amp; ", " &amp; B298 &amp; ", " &amp; C298 &amp; ", " &amp; D298 &amp; ", " &amp; E298 &amp; ", " &amp; F298 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1487, 357, 98, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="3">
+        <f t="shared" si="36"/>
+        <v>1488</v>
+      </c>
+      <c r="B299" s="3">
+        <f>B298</f>
+        <v>357</v>
+      </c>
+      <c r="C299" s="3">
+        <v>98</v>
+      </c>
+      <c r="D299" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F297" s="3">
-        <v>1</v>
-      </c>
-      <c r="G297" s="3" t="str">
+      <c r="E299" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F299" s="3">
+        <v>1</v>
+      </c>
+      <c r="G299" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1486, 357, null, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A298" s="4">
-        <f t="shared" ref="A298:A309" si="54">A297+1</f>
-        <v>1487</v>
-      </c>
-      <c r="B298" s="4">
-        <f>B294+1</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1488, 357, 98, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="3">
+        <f t="shared" si="36"/>
+        <v>1489</v>
+      </c>
+      <c r="B300" s="3">
+        <f>B298</f>
+        <v>357</v>
+      </c>
+      <c r="C300" s="3">
+        <v>7</v>
+      </c>
+      <c r="D300" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E300" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F300" s="3">
+        <v>2</v>
+      </c>
+      <c r="G300" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1489, 357, 7, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="3">
+        <f t="shared" si="36"/>
+        <v>1490</v>
+      </c>
+      <c r="B301" s="3">
+        <f t="shared" ref="B301" si="53">B298</f>
+        <v>357</v>
+      </c>
+      <c r="C301" s="3">
+        <v>7</v>
+      </c>
+      <c r="D301" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E301" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F301" s="3">
+        <v>1</v>
+      </c>
+      <c r="G301" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1490, 357, 7, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="4">
+        <f t="shared" ref="A302:A313" si="54">A301+1</f>
+        <v>1491</v>
+      </c>
+      <c r="B302" s="4">
+        <f>B298+1</f>
         <v>358</v>
       </c>
-      <c r="C298" s="4" t="s">
+      <c r="C302" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D298" s="4" t="s">
+      <c r="D302" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E298" s="4" t="s">
+      <c r="E302" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F298" s="4">
-        <v>2</v>
-      </c>
-      <c r="G298" s="4" t="str">
+      <c r="F302" s="4">
+        <v>2</v>
+      </c>
+      <c r="G302" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1487, 358, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A299" s="4">
-        <f t="shared" si="54"/>
-        <v>1488</v>
-      </c>
-      <c r="B299" s="4">
-        <f>B298</f>
-        <v>358</v>
-      </c>
-      <c r="C299" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D299" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E299" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F299" s="4">
-        <v>1</v>
-      </c>
-      <c r="G299" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1488, 358, null, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A300" s="4">
-        <f t="shared" si="54"/>
-        <v>1489</v>
-      </c>
-      <c r="B300" s="4">
-        <f>B298</f>
-        <v>358</v>
-      </c>
-      <c r="C300" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D300" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E300" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F300" s="4">
-        <v>2</v>
-      </c>
-      <c r="G300" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1489, 358, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A301" s="4">
-        <f t="shared" si="54"/>
-        <v>1490</v>
-      </c>
-      <c r="B301" s="4">
-        <f t="shared" ref="B301" si="55">B298</f>
-        <v>358</v>
-      </c>
-      <c r="C301" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D301" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E301" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F301" s="4">
-        <v>1</v>
-      </c>
-      <c r="G301" s="4" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1490, 358, null, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A302" s="3">
-        <f t="shared" si="54"/>
-        <v>1491</v>
-      </c>
-      <c r="B302" s="3">
-        <f>B298+1</f>
-        <v>359</v>
-      </c>
-      <c r="C302" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D302" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E302" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F302" s="3">
-        <v>2</v>
-      </c>
-      <c r="G302" s="3" t="str">
-        <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1491, 359, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1491, 358, null, null, null, 2);</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A303" s="3">
+      <c r="A303" s="4">
         <f t="shared" si="54"/>
         <v>1492</v>
       </c>
-      <c r="B303" s="3">
+      <c r="B303" s="4">
         <f>B302</f>
-        <v>359</v>
-      </c>
-      <c r="C303" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C303" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D303" s="3" t="s">
+      <c r="D303" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E303" s="3" t="s">
+      <c r="E303" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F303" s="3">
-        <v>1</v>
-      </c>
-      <c r="G303" s="3" t="str">
+      <c r="F303" s="4">
+        <v>1</v>
+      </c>
+      <c r="G303" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1492, 359, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1492, 358, null, null, null, 1);</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A304" s="3">
+      <c r="A304" s="4">
         <f t="shared" si="54"/>
         <v>1493</v>
       </c>
-      <c r="B304" s="3">
+      <c r="B304" s="4">
         <f>B302</f>
-        <v>359</v>
-      </c>
-      <c r="C304" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C304" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D304" s="3" t="s">
+      <c r="D304" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E304" s="3" t="s">
+      <c r="E304" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F304" s="3">
-        <v>2</v>
-      </c>
-      <c r="G304" s="3" t="str">
+      <c r="F304" s="4">
+        <v>2</v>
+      </c>
+      <c r="G304" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1493, 359, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1493, 358, null, null, null, 2);</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A305" s="3">
+      <c r="A305" s="4">
         <f t="shared" si="54"/>
         <v>1494</v>
       </c>
-      <c r="B305" s="3">
-        <f t="shared" ref="B305" si="56">B302</f>
-        <v>359</v>
-      </c>
-      <c r="C305" s="3" t="s">
+      <c r="B305" s="4">
+        <f t="shared" ref="B305" si="55">B302</f>
+        <v>358</v>
+      </c>
+      <c r="C305" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D305" s="3" t="s">
+      <c r="D305" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E305" s="3" t="s">
+      <c r="E305" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F305" s="3">
-        <v>1</v>
-      </c>
-      <c r="G305" s="3" t="str">
+      <c r="F305" s="4">
+        <v>1</v>
+      </c>
+      <c r="G305" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1494, 359, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1494, 358, null, null, null, 1);</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A306" s="4">
+      <c r="A306" s="3">
         <f t="shared" si="54"/>
         <v>1495</v>
       </c>
-      <c r="B306" s="4">
+      <c r="B306" s="3">
         <f>B302+1</f>
-        <v>360</v>
-      </c>
-      <c r="C306" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C306" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D306" s="4" t="s">
+      <c r="D306" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E306" s="4" t="s">
+      <c r="E306" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F306" s="4">
-        <v>2</v>
-      </c>
-      <c r="G306" s="4" t="str">
+      <c r="F306" s="3">
+        <v>2</v>
+      </c>
+      <c r="G306" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1495, 360, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1495, 359, null, null, null, 2);</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A307" s="4">
+      <c r="A307" s="3">
         <f t="shared" si="54"/>
         <v>1496</v>
       </c>
-      <c r="B307" s="4">
+      <c r="B307" s="3">
         <f>B306</f>
-        <v>360</v>
-      </c>
-      <c r="C307" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C307" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D307" s="4" t="s">
+      <c r="D307" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E307" s="4" t="s">
+      <c r="E307" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F307" s="4">
-        <v>1</v>
-      </c>
-      <c r="G307" s="4" t="str">
+      <c r="F307" s="3">
+        <v>1</v>
+      </c>
+      <c r="G307" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1496, 360, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1496, 359, null, null, null, 1);</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A308" s="4">
+      <c r="A308" s="3">
         <f t="shared" si="54"/>
         <v>1497</v>
       </c>
-      <c r="B308" s="4">
+      <c r="B308" s="3">
         <f>B306</f>
-        <v>360</v>
-      </c>
-      <c r="C308" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C308" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D308" s="4" t="s">
+      <c r="D308" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E308" s="4" t="s">
+      <c r="E308" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F308" s="4">
-        <v>2</v>
-      </c>
-      <c r="G308" s="4" t="str">
+      <c r="F308" s="3">
+        <v>2</v>
+      </c>
+      <c r="G308" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1497, 360, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1497, 359, null, null, null, 2);</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A309" s="4">
+      <c r="A309" s="3">
         <f t="shared" si="54"/>
         <v>1498</v>
       </c>
-      <c r="B309" s="4">
-        <f t="shared" ref="B309" si="57">B306</f>
+      <c r="B309" s="3">
+        <f t="shared" ref="B309" si="56">B306</f>
+        <v>359</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D309" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E309" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F309" s="3">
+        <v>1</v>
+      </c>
+      <c r="G309" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1498, 359, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="4">
+        <f t="shared" si="54"/>
+        <v>1499</v>
+      </c>
+      <c r="B310" s="4">
+        <f>B306+1</f>
         <v>360</v>
       </c>
-      <c r="C309" s="4" t="s">
+      <c r="C310" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D309" s="4" t="s">
+      <c r="D310" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E309" s="4" t="s">
+      <c r="E310" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F309" s="4">
-        <v>1</v>
-      </c>
-      <c r="G309" s="4" t="str">
+      <c r="F310" s="4">
+        <v>2</v>
+      </c>
+      <c r="G310" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1498, 360, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1499, 360, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="4">
+        <f t="shared" si="54"/>
+        <v>1500</v>
+      </c>
+      <c r="B311" s="4">
+        <f>B310</f>
+        <v>360</v>
+      </c>
+      <c r="C311" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D311" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E311" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F311" s="4">
+        <v>1</v>
+      </c>
+      <c r="G311" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1500, 360, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="4">
+        <f t="shared" si="54"/>
+        <v>1501</v>
+      </c>
+      <c r="B312" s="4">
+        <f>B310</f>
+        <v>360</v>
+      </c>
+      <c r="C312" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D312" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E312" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F312" s="4">
+        <v>2</v>
+      </c>
+      <c r="G312" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1501, 360, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="4">
+        <f t="shared" si="54"/>
+        <v>1502</v>
+      </c>
+      <c r="B313" s="4">
+        <f t="shared" ref="B313" si="57">B310</f>
+        <v>360</v>
+      </c>
+      <c r="C313" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D313" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E313" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F313" s="4">
+        <v>1</v>
+      </c>
+      <c r="G313" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1502, 360, null, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Futsal World Cup 2016 Quarter-Finals "nd Date
Futsal World Cup 2016 Quarter-Finals "nd Date
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -44731,7 +44731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -51953,18 +51955,18 @@
       <c r="C290" s="3">
         <v>54</v>
       </c>
-      <c r="D290" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E290" s="3" t="s">
-        <v>18</v>
+      <c r="D290" s="3">
+        <v>5</v>
+      </c>
+      <c r="E290" s="3">
+        <v>3</v>
       </c>
       <c r="F290" s="3">
         <v>2</v>
       </c>
       <c r="G290" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1479, 355, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1479, 355, 54, 5, 3, 2);</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
@@ -51979,18 +51981,18 @@
       <c r="C291" s="3">
         <v>54</v>
       </c>
-      <c r="D291" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E291" s="3" t="s">
-        <v>18</v>
+      <c r="D291" s="3">
+        <v>2</v>
+      </c>
+      <c r="E291" s="3">
+        <v>0</v>
       </c>
       <c r="F291" s="3">
         <v>1</v>
       </c>
       <c r="G291" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1480, 355, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1480, 355, 54, 2, 0, 1);</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
@@ -52005,18 +52007,18 @@
       <c r="C292" s="3">
         <v>20</v>
       </c>
-      <c r="D292" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E292" s="3" t="s">
-        <v>18</v>
+      <c r="D292" s="3">
+        <v>0</v>
+      </c>
+      <c r="E292" s="3">
+        <v>0</v>
       </c>
       <c r="F292" s="3">
         <v>2</v>
       </c>
       <c r="G292" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1481, 355, 20, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1481, 355, 20, 0, 0, 2);</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
@@ -52031,18 +52033,18 @@
       <c r="C293" s="3">
         <v>20</v>
       </c>
-      <c r="D293" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E293" s="3" t="s">
-        <v>18</v>
+      <c r="D293" s="3">
+        <v>0</v>
+      </c>
+      <c r="E293" s="3">
+        <v>0</v>
       </c>
       <c r="F293" s="3">
         <v>1</v>
       </c>
       <c r="G293" s="3" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1482, 355, 20, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1482, 355, 20, 0, 0, 1);</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
@@ -52057,18 +52059,18 @@
       <c r="C294" s="4">
         <v>994</v>
       </c>
-      <c r="D294" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E294" s="4" t="s">
-        <v>18</v>
+      <c r="D294" s="4">
+        <v>2</v>
+      </c>
+      <c r="E294" s="4">
+        <v>0</v>
       </c>
       <c r="F294" s="4">
         <v>2</v>
       </c>
       <c r="G294" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1483, 356, 994, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1483, 356, 994, 2, 0, 2);</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
@@ -52083,18 +52085,18 @@
       <c r="C295" s="4">
         <v>994</v>
       </c>
-      <c r="D295" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E295" s="4" t="s">
-        <v>18</v>
+      <c r="D295" s="4">
+        <v>1</v>
+      </c>
+      <c r="E295" s="4">
+        <v>0</v>
       </c>
       <c r="F295" s="4">
         <v>1</v>
       </c>
       <c r="G295" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1484, 356, 994, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1484, 356, 994, 1, 0, 1);</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
@@ -52109,18 +52111,18 @@
       <c r="C296" s="4">
         <v>351</v>
       </c>
-      <c r="D296" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E296" s="4" t="s">
-        <v>18</v>
+      <c r="D296" s="4">
+        <v>3</v>
+      </c>
+      <c r="E296" s="4">
+        <v>3</v>
       </c>
       <c r="F296" s="4">
         <v>2</v>
       </c>
       <c r="G296" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1485, 356, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1485, 356, 351, 3, 3, 2);</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
@@ -52135,18 +52137,18 @@
       <c r="C297" s="4">
         <v>351</v>
       </c>
-      <c r="D297" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E297" s="4" t="s">
-        <v>18</v>
+      <c r="D297" s="4">
+        <v>2</v>
+      </c>
+      <c r="E297" s="4">
+        <v>0</v>
       </c>
       <c r="F297" s="4">
         <v>1</v>
       </c>
       <c r="G297" s="4" t="str">
         <f t="shared" si="34"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1486, 356, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1486, 356, 351, 2, 0, 1);</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
@@ -52262,8 +52264,8 @@
         <f>B298+1</f>
         <v>358</v>
       </c>
-      <c r="C302" s="4" t="s">
-        <v>18</v>
+      <c r="C302" s="4">
+        <v>54</v>
       </c>
       <c r="D302" s="4" t="s">
         <v>18</v>
@@ -52276,7 +52278,7 @@
       </c>
       <c r="G302" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1491, 358, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1491, 358, 54, null, null, 2);</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
@@ -52288,8 +52290,8 @@
         <f>B302</f>
         <v>358</v>
       </c>
-      <c r="C303" s="4" t="s">
-        <v>18</v>
+      <c r="C303" s="4">
+        <v>54</v>
       </c>
       <c r="D303" s="4" t="s">
         <v>18</v>
@@ -52302,7 +52304,7 @@
       </c>
       <c r="G303" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1492, 358, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1492, 358, 54, null, null, 1);</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
@@ -52314,8 +52316,8 @@
         <f>B302</f>
         <v>358</v>
       </c>
-      <c r="C304" s="4" t="s">
-        <v>18</v>
+      <c r="C304" s="4">
+        <v>351</v>
       </c>
       <c r="D304" s="4" t="s">
         <v>18</v>
@@ -52328,7 +52330,7 @@
       </c>
       <c r="G304" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1493, 358, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1493, 358, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
@@ -52340,8 +52342,8 @@
         <f t="shared" ref="B305" si="55">B302</f>
         <v>358</v>
       </c>
-      <c r="C305" s="4" t="s">
-        <v>18</v>
+      <c r="C305" s="4">
+        <v>351</v>
       </c>
       <c r="D305" s="4" t="s">
         <v>18</v>
@@ -52354,7 +52356,7 @@
       </c>
       <c r="G305" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1494, 358, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1494, 358, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FIFA Futsal World Cup Semifinals
FIFA Futsal World Cup Semifinals
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -44731,9 +44731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -52163,18 +52161,18 @@
       <c r="C298" s="3">
         <v>98</v>
       </c>
-      <c r="D298" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E298" s="3" t="s">
-        <v>18</v>
+      <c r="D298" s="3">
+        <v>3</v>
+      </c>
+      <c r="E298" s="3">
+        <v>0</v>
       </c>
       <c r="F298" s="3">
         <v>2</v>
       </c>
       <c r="G298" s="3" t="str">
         <f t="shared" ref="G298:G313" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A298 &amp; ", " &amp; B298 &amp; ", " &amp; C298 &amp; ", " &amp; D298 &amp; ", " &amp; E298 &amp; ", " &amp; F298 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1487, 357, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1487, 357, 98, 3, 0, 2);</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">
@@ -52189,18 +52187,18 @@
       <c r="C299" s="3">
         <v>98</v>
       </c>
-      <c r="D299" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E299" s="3" t="s">
-        <v>18</v>
+      <c r="D299" s="3">
+        <v>1</v>
+      </c>
+      <c r="E299" s="3">
+        <v>0</v>
       </c>
       <c r="F299" s="3">
         <v>1</v>
       </c>
       <c r="G299" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1488, 357, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1488, 357, 98, 1, 0, 1);</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.25">
@@ -52215,18 +52213,18 @@
       <c r="C300" s="3">
         <v>7</v>
       </c>
-      <c r="D300" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E300" s="3" t="s">
-        <v>18</v>
+      <c r="D300" s="3">
+        <v>4</v>
+      </c>
+      <c r="E300" s="3">
+        <v>3</v>
       </c>
       <c r="F300" s="3">
         <v>2</v>
       </c>
       <c r="G300" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1489, 357, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1489, 357, 7, 4, 3, 2);</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.25">
@@ -52241,18 +52239,18 @@
       <c r="C301" s="3">
         <v>7</v>
       </c>
-      <c r="D301" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E301" s="3" t="s">
-        <v>18</v>
+      <c r="D301" s="3">
+        <v>1</v>
+      </c>
+      <c r="E301" s="3">
+        <v>0</v>
       </c>
       <c r="F301" s="3">
         <v>1</v>
       </c>
       <c r="G301" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1490, 357, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1490, 357, 7, 1, 0, 1);</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
@@ -52267,18 +52265,18 @@
       <c r="C302" s="4">
         <v>54</v>
       </c>
-      <c r="D302" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E302" s="4" t="s">
-        <v>18</v>
+      <c r="D302" s="4">
+        <v>6</v>
+      </c>
+      <c r="E302" s="4">
+        <v>3</v>
       </c>
       <c r="F302" s="4">
         <v>2</v>
       </c>
       <c r="G302" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1491, 358, 54, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1491, 358, 54, 6, 3, 2);</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
@@ -52293,18 +52291,18 @@
       <c r="C303" s="4">
         <v>54</v>
       </c>
-      <c r="D303" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E303" s="4" t="s">
-        <v>18</v>
+      <c r="D303" s="4">
+        <v>4</v>
+      </c>
+      <c r="E303" s="4">
+        <v>0</v>
       </c>
       <c r="F303" s="4">
         <v>1</v>
       </c>
       <c r="G303" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1492, 358, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1492, 358, 54, 4, 0, 1);</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
@@ -52319,18 +52317,18 @@
       <c r="C304" s="4">
         <v>351</v>
       </c>
-      <c r="D304" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E304" s="4" t="s">
-        <v>18</v>
+      <c r="D304" s="4">
+        <v>2</v>
+      </c>
+      <c r="E304" s="4">
+        <v>0</v>
       </c>
       <c r="F304" s="4">
         <v>2</v>
       </c>
       <c r="G304" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1493, 358, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1493, 358, 351, 2, 0, 2);</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
@@ -52345,18 +52343,18 @@
       <c r="C305" s="4">
         <v>351</v>
       </c>
-      <c r="D305" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E305" s="4" t="s">
-        <v>18</v>
+      <c r="D305" s="4">
+        <v>1</v>
+      </c>
+      <c r="E305" s="4">
+        <v>0</v>
       </c>
       <c r="F305" s="4">
         <v>1</v>
       </c>
       <c r="G305" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1494, 358, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1494, 358, 351, 1, 0, 1);</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
@@ -52368,8 +52366,8 @@
         <f>B302+1</f>
         <v>359</v>
       </c>
-      <c r="C306" s="3" t="s">
-        <v>18</v>
+      <c r="C306" s="3">
+        <v>98</v>
       </c>
       <c r="D306" s="3" t="s">
         <v>18</v>
@@ -52382,7 +52380,7 @@
       </c>
       <c r="G306" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1495, 359, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1495, 359, 98, null, null, 2);</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
@@ -52394,8 +52392,8 @@
         <f>B306</f>
         <v>359</v>
       </c>
-      <c r="C307" s="3" t="s">
-        <v>18</v>
+      <c r="C307" s="3">
+        <v>98</v>
       </c>
       <c r="D307" s="3" t="s">
         <v>18</v>
@@ -52408,7 +52406,7 @@
       </c>
       <c r="G307" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1496, 359, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1496, 359, 98, null, null, 1);</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
@@ -52420,8 +52418,8 @@
         <f>B306</f>
         <v>359</v>
       </c>
-      <c r="C308" s="3" t="s">
-        <v>18</v>
+      <c r="C308" s="3">
+        <v>351</v>
       </c>
       <c r="D308" s="3" t="s">
         <v>18</v>
@@ -52434,7 +52432,7 @@
       </c>
       <c r="G308" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1497, 359, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1497, 359, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
@@ -52446,8 +52444,8 @@
         <f t="shared" ref="B309" si="56">B306</f>
         <v>359</v>
       </c>
-      <c r="C309" s="3" t="s">
-        <v>18</v>
+      <c r="C309" s="3">
+        <v>351</v>
       </c>
       <c r="D309" s="3" t="s">
         <v>18</v>
@@ -52460,7 +52458,7 @@
       </c>
       <c r="G309" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1498, 359, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1498, 359, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
@@ -52472,8 +52470,8 @@
         <f>B306+1</f>
         <v>360</v>
       </c>
-      <c r="C310" s="4" t="s">
-        <v>18</v>
+      <c r="C310" s="4">
+        <v>7</v>
       </c>
       <c r="D310" s="4" t="s">
         <v>18</v>
@@ -52486,7 +52484,7 @@
       </c>
       <c r="G310" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1499, 360, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1499, 360, 7, null, null, 2);</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.25">
@@ -52498,8 +52496,8 @@
         <f>B310</f>
         <v>360</v>
       </c>
-      <c r="C311" s="4" t="s">
-        <v>18</v>
+      <c r="C311" s="4">
+        <v>7</v>
       </c>
       <c r="D311" s="4" t="s">
         <v>18</v>
@@ -52512,7 +52510,7 @@
       </c>
       <c r="G311" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1500, 360, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1500, 360, 7, null, null, 1);</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
@@ -52524,8 +52522,8 @@
         <f>B310</f>
         <v>360</v>
       </c>
-      <c r="C312" s="4" t="s">
-        <v>18</v>
+      <c r="C312" s="4">
+        <v>54</v>
       </c>
       <c r="D312" s="4" t="s">
         <v>18</v>
@@ -52538,7 +52536,7 @@
       </c>
       <c r="G312" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1501, 360, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1501, 360, 54, null, null, 2);</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
@@ -52550,8 +52548,8 @@
         <f t="shared" ref="B313" si="57">B310</f>
         <v>360</v>
       </c>
-      <c r="C313" s="4" t="s">
-        <v>18</v>
+      <c r="C313" s="4">
+        <v>54</v>
       </c>
       <c r="D313" s="4" t="s">
         <v>18</v>
@@ -52564,7 +52562,7 @@
       </c>
       <c r="G313" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1502, 360, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1502, 360, 54, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIFA Futsal World Cup finals
FIFA Futsal World Cup finals
</commit_message>
<xml_diff>
--- a/Scripts/futsalworldcup/futsalworkdcup.xlsx
+++ b/Scripts/futsalworldcup/futsalworkdcup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
 </sst>
 </file>
@@ -44729,7 +44726,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G313"/>
+  <dimension ref="A1:G319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -52171,7 +52168,7 @@
         <v>2</v>
       </c>
       <c r="G298" s="3" t="str">
-        <f t="shared" ref="G298:G313" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A298 &amp; ", " &amp; B298 &amp; ", " &amp; C298 &amp; ", " &amp; D298 &amp; ", " &amp; E298 &amp; ", " &amp; F298 &amp; ");"</f>
+        <f t="shared" ref="G298:G319" si="52">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A298 &amp; ", " &amp; B298 &amp; ", " &amp; C298 &amp; ", " &amp; D298 &amp; ", " &amp; E298 &amp; ", " &amp; F298 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1487, 357, 98, 3, 0, 2);</v>
       </c>
     </row>
@@ -52255,7 +52252,7 @@
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="4">
-        <f t="shared" ref="A302:A313" si="54">A301+1</f>
+        <f t="shared" ref="A302:A319" si="54">A301+1</f>
         <v>1491</v>
       </c>
       <c r="B302" s="4">
@@ -52369,18 +52366,18 @@
       <c r="C306" s="3">
         <v>98</v>
       </c>
-      <c r="D306" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E306" s="3" t="s">
-        <v>18</v>
+      <c r="D306" s="3">
+        <v>2</v>
+      </c>
+      <c r="E306" s="3">
+        <v>0</v>
       </c>
       <c r="F306" s="3">
         <v>2</v>
       </c>
       <c r="G306" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1495, 359, 98, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1495, 359, 98, 2, 0, 2);</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
@@ -52395,18 +52392,18 @@
       <c r="C307" s="3">
         <v>98</v>
       </c>
-      <c r="D307" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E307" s="3" t="s">
-        <v>18</v>
+      <c r="D307" s="3">
+        <v>0</v>
+      </c>
+      <c r="E307" s="3">
+        <v>0</v>
       </c>
       <c r="F307" s="3">
         <v>1</v>
       </c>
       <c r="G307" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1496, 359, 98, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1496, 359, 98, 0, 0, 1);</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
@@ -52421,18 +52418,18 @@
       <c r="C308" s="3">
         <v>351</v>
       </c>
-      <c r="D308" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E308" s="3" t="s">
-        <v>18</v>
+      <c r="D308" s="3">
+        <v>2</v>
+      </c>
+      <c r="E308" s="3">
+        <v>0</v>
       </c>
       <c r="F308" s="3">
         <v>2</v>
       </c>
       <c r="G308" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1497, 359, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1497, 359, 351, 2, 0, 2);</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
@@ -52441,128 +52438,284 @@
         <v>1498</v>
       </c>
       <c r="B309" s="3">
-        <f t="shared" ref="B309" si="56">B306</f>
+        <f t="shared" ref="B309:B315" si="56">B306</f>
         <v>359</v>
       </c>
       <c r="C309" s="3">
         <v>351</v>
       </c>
-      <c r="D309" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E309" s="3" t="s">
-        <v>18</v>
+      <c r="D309" s="3">
+        <v>0</v>
+      </c>
+      <c r="E309" s="3">
+        <v>0</v>
       </c>
       <c r="F309" s="3">
         <v>1</v>
       </c>
       <c r="G309" s="3" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1498, 359, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1498, 359, 351, 0, 0, 1);</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A310" s="4">
+      <c r="A310" s="3">
         <f t="shared" si="54"/>
         <v>1499</v>
       </c>
-      <c r="B310" s="4">
+      <c r="B310" s="3">
+        <f t="shared" si="56"/>
+        <v>359</v>
+      </c>
+      <c r="C310" s="3">
+        <v>98</v>
+      </c>
+      <c r="D310" s="3">
+        <v>2</v>
+      </c>
+      <c r="E310" s="3">
+        <v>1</v>
+      </c>
+      <c r="F310" s="3">
+        <v>4</v>
+      </c>
+      <c r="G310" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1499, 359, 98, 2, 1, 4);</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="3">
+        <f t="shared" si="54"/>
+        <v>1500</v>
+      </c>
+      <c r="B311" s="3">
+        <f t="shared" si="56"/>
+        <v>359</v>
+      </c>
+      <c r="C311" s="3">
+        <v>98</v>
+      </c>
+      <c r="D311" s="3">
+        <v>2</v>
+      </c>
+      <c r="E311" s="3">
+        <v>0</v>
+      </c>
+      <c r="F311" s="3">
+        <v>3</v>
+      </c>
+      <c r="G311" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1500, 359, 98, 2, 0, 3);</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="3">
+        <f t="shared" si="54"/>
+        <v>1501</v>
+      </c>
+      <c r="B312" s="3">
+        <f t="shared" si="56"/>
+        <v>359</v>
+      </c>
+      <c r="C312" s="3">
+        <v>351</v>
+      </c>
+      <c r="D312" s="3">
+        <v>2</v>
+      </c>
+      <c r="E312" s="3">
+        <v>1</v>
+      </c>
+      <c r="F312" s="3">
+        <v>4</v>
+      </c>
+      <c r="G312" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1501, 359, 351, 2, 1, 4);</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="3">
+        <f t="shared" si="54"/>
+        <v>1502</v>
+      </c>
+      <c r="B313" s="3">
+        <f t="shared" si="56"/>
+        <v>359</v>
+      </c>
+      <c r="C313" s="3">
+        <v>351</v>
+      </c>
+      <c r="D313" s="3">
+        <v>2</v>
+      </c>
+      <c r="E313" s="3">
+        <v>0</v>
+      </c>
+      <c r="F313" s="3">
+        <v>3</v>
+      </c>
+      <c r="G313" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1502, 359, 351, 2, 0, 3);</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="3">
+        <f t="shared" si="54"/>
+        <v>1503</v>
+      </c>
+      <c r="B314" s="3">
+        <f t="shared" si="56"/>
+        <v>359</v>
+      </c>
+      <c r="C314" s="3">
+        <v>98</v>
+      </c>
+      <c r="D314" s="3">
+        <v>4</v>
+      </c>
+      <c r="E314" s="3">
+        <v>0</v>
+      </c>
+      <c r="F314" s="3">
+        <v>7</v>
+      </c>
+      <c r="G314" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1503, 359, 98, 4, 0, 7);</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="3">
+        <f t="shared" si="54"/>
+        <v>1504</v>
+      </c>
+      <c r="B315" s="3">
+        <f t="shared" si="56"/>
+        <v>359</v>
+      </c>
+      <c r="C315" s="3">
+        <v>351</v>
+      </c>
+      <c r="D315" s="3">
+        <v>3</v>
+      </c>
+      <c r="E315" s="3">
+        <v>0</v>
+      </c>
+      <c r="F315" s="3">
+        <v>7</v>
+      </c>
+      <c r="G315" s="3" t="str">
+        <f t="shared" si="52"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1504, 359, 351, 3, 0, 7);</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="4">
+        <f t="shared" si="54"/>
+        <v>1505</v>
+      </c>
+      <c r="B316" s="4">
         <f>B306+1</f>
         <v>360</v>
       </c>
-      <c r="C310" s="4">
+      <c r="C316" s="4">
         <v>7</v>
       </c>
-      <c r="D310" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E310" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F310" s="4">
-        <v>2</v>
-      </c>
-      <c r="G310" s="4" t="str">
+      <c r="D316" s="4">
+        <v>4</v>
+      </c>
+      <c r="E316" s="4">
+        <v>0</v>
+      </c>
+      <c r="F316" s="4">
+        <v>2</v>
+      </c>
+      <c r="G316" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1499, 360, 7, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A311" s="4">
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1505, 360, 7, 4, 0, 2);</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="4">
         <f t="shared" si="54"/>
-        <v>1500</v>
-      </c>
-      <c r="B311" s="4">
-        <f>B310</f>
+        <v>1506</v>
+      </c>
+      <c r="B317" s="4">
+        <f>B316</f>
         <v>360</v>
       </c>
-      <c r="C311" s="4">
+      <c r="C317" s="4">
         <v>7</v>
       </c>
-      <c r="D311" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E311" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F311" s="4">
-        <v>1</v>
-      </c>
-      <c r="G311" s="4" t="str">
+      <c r="D317" s="4">
+        <v>1</v>
+      </c>
+      <c r="E317" s="4">
+        <v>0</v>
+      </c>
+      <c r="F317" s="4">
+        <v>1</v>
+      </c>
+      <c r="G317" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1500, 360, 7, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A312" s="4">
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1506, 360, 7, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="4">
         <f t="shared" si="54"/>
-        <v>1501</v>
-      </c>
-      <c r="B312" s="4">
-        <f>B310</f>
+        <v>1507</v>
+      </c>
+      <c r="B318" s="4">
+        <f>B316</f>
         <v>360</v>
       </c>
-      <c r="C312" s="4">
+      <c r="C318" s="4">
         <v>54</v>
       </c>
-      <c r="D312" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E312" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F312" s="4">
-        <v>2</v>
-      </c>
-      <c r="G312" s="4" t="str">
+      <c r="D318" s="4">
+        <v>5</v>
+      </c>
+      <c r="E318" s="4">
+        <v>3</v>
+      </c>
+      <c r="F318" s="4">
+        <v>2</v>
+      </c>
+      <c r="G318" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1501, 360, 54, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A313" s="4">
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1507, 360, 54, 5, 3, 2);</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="4">
         <f t="shared" si="54"/>
-        <v>1502</v>
-      </c>
-      <c r="B313" s="4">
-        <f t="shared" ref="B313" si="57">B310</f>
+        <v>1508</v>
+      </c>
+      <c r="B319" s="4">
+        <f t="shared" ref="B319" si="57">B316</f>
         <v>360</v>
       </c>
-      <c r="C313" s="4">
+      <c r="C319" s="4">
         <v>54</v>
       </c>
-      <c r="D313" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E313" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F313" s="4">
-        <v>1</v>
-      </c>
-      <c r="G313" s="4" t="str">
+      <c r="D319" s="4">
+        <v>2</v>
+      </c>
+      <c r="E319" s="4">
+        <v>0</v>
+      </c>
+      <c r="F319" s="4">
+        <v>1</v>
+      </c>
+      <c r="G319" s="4" t="str">
         <f t="shared" si="52"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1502, 360, 54, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1508, 360, 54, 2, 0, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>